<commit_message>
Refactored. Made constants for the tile dimensions that are defined in the defineConstants script. Whenever you're working in a room make sure there is an instance of o_GameEngine in the room and it is being created first so that the global variables and constants can be defined. Also working on the movement mechanics. Successfully creating a map with adjacency lists for tiles, and developed an untested calcTargets function for getting a global list of the current targets. Changed humans to have a movement button that is shown when the human can move, and changes to a cancel button when the player is supposed to be selecting a place to move to. Still need to implement selecting a target. Need to implement a way for tiles to know what objects are occupying them and vis versa
</commit_message>
<xml_diff>
--- a/Production Documents/To-Do.xlsx
+++ b/Production Documents/To-Do.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Shiva\Production Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmgam\Desktop\Shiva\Production Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C3542D1-45D1-4062-8D0F-7E1855505B19}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A95B87C1-1D13-41BB-98A6-4CE6A3FC52D0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{669DCC34-C837-4342-A908-0F87EB315612}"/>
+    <workbookView xWindow="32010" yWindow="1455" windowWidth="16530" windowHeight="10125" xr2:uid="{669DCC34-C837-4342-A908-0F87EB315612}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -360,21 +360,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -699,35 +700,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4D254F2-4E19-40CF-BD85-766CDBA8C5EF}">
   <dimension ref="A2:F64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H61" sqref="H61"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="18" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:6" ht="18" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-    </row>
-    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -747,7 +748,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>75</v>
       </c>
@@ -767,8 +768,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -787,7 +788,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
@@ -807,7 +808,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
@@ -823,7 +824,7 @@
       </c>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
@@ -839,7 +840,7 @@
       </c>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
@@ -853,7 +854,7 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>13</v>
       </c>
@@ -865,7 +866,7 @@
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
@@ -873,22 +874,22 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C13" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A15" s="6" t="s">
+    <row r="15" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-    </row>
-    <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+    </row>
+    <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1" t="s">
         <v>3</v>
@@ -906,7 +907,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
         <v>15</v>
       </c>
@@ -923,7 +924,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>16</v>
       </c>
@@ -938,7 +939,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>17</v>
       </c>
@@ -953,7 +954,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
         <v>18</v>
       </c>
@@ -963,7 +964,7 @@
       <c r="D20" s="4"/>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
         <v>19</v>
       </c>
@@ -974,7 +975,7 @@
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
         <v>20</v>
       </c>
@@ -985,326 +986,346 @@
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C23" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C24" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C25" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="7" t="s">
+    <row r="27" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-    </row>
-    <row r="28" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+    </row>
+    <row r="28" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="9" t="s">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B29" s="9"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="9" t="s">
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="9" t="s">
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="9" t="s">
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B32" s="9"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="9"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="9" t="s">
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B33" s="9"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="9" t="s">
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B34" s="9"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9"/>
-    </row>
-    <row r="36" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+    </row>
+    <row r="36" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="9" t="s">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="B37" s="9"/>
-      <c r="C37" s="9"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="9"/>
-      <c r="F37" s="9"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="9" t="s">
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="B38" s="9"/>
-      <c r="C38" s="9"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="9"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="9" t="s">
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="B39" s="9"/>
-      <c r="C39" s="9"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="9"/>
-    </row>
-    <row r="40" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B39" s="7"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
+    </row>
+    <row r="40" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
     </row>
-    <row r="41" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" s="9" t="s">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B42" s="9"/>
-      <c r="C42" s="9"/>
-      <c r="D42" s="9"/>
-      <c r="E42" s="9"/>
-      <c r="F42" s="9"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="9" t="s">
+      <c r="B42" s="7"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B43" s="9"/>
-      <c r="C43" s="9"/>
-      <c r="D43" s="9"/>
-      <c r="E43" s="9"/>
-      <c r="F43" s="9"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" s="9" t="s">
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B44" s="9"/>
-      <c r="C44" s="9"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="9"/>
-      <c r="F44" s="9"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45" s="9" t="s">
+      <c r="B44" s="7"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B45" s="9"/>
-      <c r="C45" s="9"/>
-      <c r="D45" s="9"/>
-      <c r="E45" s="9"/>
-      <c r="F45" s="9"/>
-    </row>
-    <row r="47" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B45" s="7"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7"/>
+    </row>
+    <row r="47" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A48" s="9" t="s">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B48" s="9"/>
-      <c r="C48" s="9"/>
-      <c r="D48" s="9"/>
-      <c r="E48" s="9"/>
-      <c r="F48" s="9"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49" s="9" t="s">
+      <c r="B48" s="7"/>
+      <c r="C48" s="7"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="7"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B49" s="9"/>
-      <c r="C49" s="9"/>
-      <c r="D49" s="9"/>
-      <c r="E49" s="9"/>
-      <c r="F49" s="9"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" s="9" t="s">
+      <c r="B49" s="7"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="7"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B50" s="9"/>
-      <c r="C50" s="9"/>
-      <c r="D50" s="9"/>
-      <c r="E50" s="9"/>
-      <c r="F50" s="9"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" s="9" t="s">
+      <c r="B50" s="7"/>
+      <c r="C50" s="7"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="7"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="B51" s="9"/>
-      <c r="C51" s="9"/>
-      <c r="D51" s="9"/>
-      <c r="E51" s="9"/>
-      <c r="F51" s="9"/>
-    </row>
-    <row r="53" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B51" s="7"/>
+      <c r="C51" s="7"/>
+      <c r="D51" s="7"/>
+      <c r="E51" s="7"/>
+      <c r="F51" s="7"/>
+    </row>
+    <row r="53" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A54" s="9" t="s">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="B54" s="9"/>
-      <c r="C54" s="9"/>
-      <c r="D54" s="9"/>
-      <c r="E54" s="9"/>
-      <c r="F54" s="9"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A55" s="9" t="s">
+      <c r="B54" s="7"/>
+      <c r="C54" s="7"/>
+      <c r="D54" s="7"/>
+      <c r="E54" s="7"/>
+      <c r="F54" s="7"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B55" s="9"/>
-      <c r="C55" s="9"/>
-      <c r="D55" s="9"/>
-      <c r="E55" s="9"/>
-      <c r="F55" s="9"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A56" s="9" t="s">
+      <c r="B55" s="7"/>
+      <c r="C55" s="7"/>
+      <c r="D55" s="7"/>
+      <c r="E55" s="7"/>
+      <c r="F55" s="7"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="B56" s="9"/>
-      <c r="C56" s="9"/>
-      <c r="D56" s="9"/>
-      <c r="E56" s="9"/>
-      <c r="F56" s="9"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A57" s="9" t="s">
+      <c r="B56" s="7"/>
+      <c r="C56" s="7"/>
+      <c r="D56" s="7"/>
+      <c r="E56" s="7"/>
+      <c r="F56" s="7"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="B57" s="9"/>
-      <c r="C57" s="9"/>
-      <c r="D57" s="9"/>
-      <c r="E57" s="9"/>
-      <c r="F57" s="9"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A58" s="9" t="s">
+      <c r="B57" s="7"/>
+      <c r="C57" s="7"/>
+      <c r="D57" s="7"/>
+      <c r="E57" s="7"/>
+      <c r="F57" s="7"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B58" s="9"/>
-      <c r="C58" s="9"/>
-      <c r="D58" s="9"/>
-      <c r="E58" s="9"/>
-      <c r="F58" s="9"/>
-    </row>
-    <row r="60" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B58" s="7"/>
+      <c r="C58" s="7"/>
+      <c r="D58" s="7"/>
+      <c r="E58" s="7"/>
+      <c r="F58" s="7"/>
+    </row>
+    <row r="60" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A61" s="9" t="s">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="B61" s="9"/>
-      <c r="C61" s="9"/>
-      <c r="D61" s="9"/>
-      <c r="E61" s="9"/>
-      <c r="F61" s="9"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A62" s="9" t="s">
+      <c r="B61" s="7"/>
+      <c r="C61" s="7"/>
+      <c r="D61" s="7"/>
+      <c r="E61" s="7"/>
+      <c r="F61" s="7"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B62" s="9"/>
-      <c r="C62" s="9"/>
-      <c r="D62" s="9"/>
-      <c r="E62" s="9"/>
-      <c r="F62" s="9"/>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A63" s="9" t="s">
+      <c r="B62" s="7"/>
+      <c r="C62" s="7"/>
+      <c r="D62" s="7"/>
+      <c r="E62" s="7"/>
+      <c r="F62" s="7"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="B63" s="9"/>
-      <c r="C63" s="9"/>
-      <c r="D63" s="9"/>
-      <c r="E63" s="9"/>
-      <c r="F63" s="9"/>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A64" s="9" t="s">
+      <c r="B63" s="7"/>
+      <c r="C63" s="7"/>
+      <c r="D63" s="7"/>
+      <c r="E63" s="7"/>
+      <c r="F63" s="7"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B64" s="9"/>
-      <c r="C64" s="9"/>
-      <c r="D64" s="9"/>
-      <c r="E64" s="9"/>
-      <c r="F64" s="9"/>
+      <c r="B64" s="7"/>
+      <c r="C64" s="7"/>
+      <c r="D64" s="7"/>
+      <c r="E64" s="7"/>
+      <c r="F64" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A15:F15"/>
+    <mergeCell ref="A27:F27"/>
+    <mergeCell ref="A29:F29"/>
+    <mergeCell ref="A30:F30"/>
+    <mergeCell ref="A31:F31"/>
+    <mergeCell ref="A32:F32"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A34:F34"/>
+    <mergeCell ref="A37:F37"/>
+    <mergeCell ref="A38:F38"/>
+    <mergeCell ref="A39:F39"/>
+    <mergeCell ref="A42:F42"/>
+    <mergeCell ref="A43:F43"/>
+    <mergeCell ref="A44:F44"/>
+    <mergeCell ref="A45:F45"/>
+    <mergeCell ref="A48:F48"/>
+    <mergeCell ref="A49:F49"/>
+    <mergeCell ref="A50:F50"/>
+    <mergeCell ref="A51:F51"/>
     <mergeCell ref="A61:F61"/>
     <mergeCell ref="A62:F62"/>
     <mergeCell ref="A63:F63"/>
@@ -1314,26 +1335,6 @@
     <mergeCell ref="A56:F56"/>
     <mergeCell ref="A57:F57"/>
     <mergeCell ref="A58:F58"/>
-    <mergeCell ref="A45:F45"/>
-    <mergeCell ref="A48:F48"/>
-    <mergeCell ref="A49:F49"/>
-    <mergeCell ref="A50:F50"/>
-    <mergeCell ref="A51:F51"/>
-    <mergeCell ref="A38:F38"/>
-    <mergeCell ref="A39:F39"/>
-    <mergeCell ref="A42:F42"/>
-    <mergeCell ref="A43:F43"/>
-    <mergeCell ref="A44:F44"/>
-    <mergeCell ref="A31:F31"/>
-    <mergeCell ref="A32:F32"/>
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="A34:F34"/>
-    <mergeCell ref="A37:F37"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A15:F15"/>
-    <mergeCell ref="A27:F27"/>
-    <mergeCell ref="A29:F29"/>
-    <mergeCell ref="A30:F30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Implemented being able to tell a moveable unit where to move to
</commit_message>
<xml_diff>
--- a/Production Documents/To-Do.xlsx
+++ b/Production Documents/To-Do.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmgam\Desktop\Shiva\Production Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A95B87C1-1D13-41BB-98A6-4CE6A3FC52D0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F135FB8-2C42-4112-B146-5AC004200565}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32010" yWindow="1455" windowWidth="16530" windowHeight="10125" xr2:uid="{669DCC34-C837-4342-A908-0F87EB315612}"/>
   </bookViews>
@@ -368,7 +368,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -376,6 +375,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -700,8 +700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4D254F2-4E19-40CF-BD85-766CDBA8C5EF}">
   <dimension ref="A2:F64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -719,14 +719,14 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="18" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -880,14 +880,14 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
     </row>
     <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
@@ -1002,14 +1002,14 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="9" t="s">
+      <c r="A27" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B27" s="9"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
     </row>
     <row r="28" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
@@ -1017,64 +1017,64 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="10" t="s">
+      <c r="A29" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
+      <c r="A30" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="7" t="s">
+      <c r="A31" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="7" t="s">
+      <c r="A32" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="7" t="s">
+      <c r="A33" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="7" t="s">
+      <c r="A34" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
     </row>
     <row r="36" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
@@ -1082,34 +1082,34 @@
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="7" t="s">
+      <c r="A37" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="B37" s="7"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="7" t="s">
+      <c r="A38" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
+      <c r="B38" s="10"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="7" t="s">
+      <c r="A39" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="B39" s="7"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
     </row>
     <row r="40" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
@@ -1120,44 +1120,44 @@
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="7" t="s">
+      <c r="A42" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="B42" s="7"/>
-      <c r="C42" s="7"/>
-      <c r="D42" s="7"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7"/>
+      <c r="B42" s="10"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="10"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="7" t="s">
+      <c r="A43" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="B43" s="7"/>
-      <c r="C43" s="7"/>
-      <c r="D43" s="7"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="7"/>
+      <c r="B43" s="10"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="7" t="s">
+      <c r="A44" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="B44" s="7"/>
-      <c r="C44" s="7"/>
-      <c r="D44" s="7"/>
-      <c r="E44" s="7"/>
-      <c r="F44" s="7"/>
+      <c r="B44" s="10"/>
+      <c r="C44" s="10"/>
+      <c r="D44" s="10"/>
+      <c r="E44" s="10"/>
+      <c r="F44" s="10"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="7" t="s">
+      <c r="A45" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="B45" s="7"/>
-      <c r="C45" s="7"/>
-      <c r="D45" s="7"/>
-      <c r="E45" s="7"/>
-      <c r="F45" s="7"/>
+      <c r="B45" s="10"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="10"/>
     </row>
     <row r="47" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
@@ -1165,44 +1165,44 @@
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="7" t="s">
+      <c r="A48" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B48" s="7"/>
-      <c r="C48" s="7"/>
-      <c r="D48" s="7"/>
-      <c r="E48" s="7"/>
-      <c r="F48" s="7"/>
+      <c r="B48" s="10"/>
+      <c r="C48" s="10"/>
+      <c r="D48" s="10"/>
+      <c r="E48" s="10"/>
+      <c r="F48" s="10"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="7" t="s">
+      <c r="A49" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="B49" s="7"/>
-      <c r="C49" s="7"/>
-      <c r="D49" s="7"/>
-      <c r="E49" s="7"/>
-      <c r="F49" s="7"/>
+      <c r="B49" s="10"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="10"/>
+      <c r="E49" s="10"/>
+      <c r="F49" s="10"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="7" t="s">
+      <c r="A50" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="B50" s="7"/>
-      <c r="C50" s="7"/>
-      <c r="D50" s="7"/>
-      <c r="E50" s="7"/>
-      <c r="F50" s="7"/>
+      <c r="B50" s="10"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="10"/>
+      <c r="E50" s="10"/>
+      <c r="F50" s="10"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="7" t="s">
+      <c r="A51" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="B51" s="7"/>
-      <c r="C51" s="7"/>
-      <c r="D51" s="7"/>
-      <c r="E51" s="7"/>
-      <c r="F51" s="7"/>
+      <c r="B51" s="10"/>
+      <c r="C51" s="10"/>
+      <c r="D51" s="10"/>
+      <c r="E51" s="10"/>
+      <c r="F51" s="10"/>
     </row>
     <row r="53" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
@@ -1210,54 +1210,54 @@
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="7" t="s">
+      <c r="A54" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="B54" s="7"/>
-      <c r="C54" s="7"/>
-      <c r="D54" s="7"/>
-      <c r="E54" s="7"/>
-      <c r="F54" s="7"/>
+      <c r="B54" s="10"/>
+      <c r="C54" s="10"/>
+      <c r="D54" s="10"/>
+      <c r="E54" s="10"/>
+      <c r="F54" s="10"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="7" t="s">
+      <c r="A55" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="B55" s="7"/>
-      <c r="C55" s="7"/>
-      <c r="D55" s="7"/>
-      <c r="E55" s="7"/>
-      <c r="F55" s="7"/>
+      <c r="B55" s="10"/>
+      <c r="C55" s="10"/>
+      <c r="D55" s="10"/>
+      <c r="E55" s="10"/>
+      <c r="F55" s="10"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="7" t="s">
+      <c r="A56" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="B56" s="7"/>
-      <c r="C56" s="7"/>
-      <c r="D56" s="7"/>
-      <c r="E56" s="7"/>
-      <c r="F56" s="7"/>
+      <c r="B56" s="10"/>
+      <c r="C56" s="10"/>
+      <c r="D56" s="10"/>
+      <c r="E56" s="10"/>
+      <c r="F56" s="10"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="7" t="s">
+      <c r="A57" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="B57" s="7"/>
-      <c r="C57" s="7"/>
-      <c r="D57" s="7"/>
-      <c r="E57" s="7"/>
-      <c r="F57" s="7"/>
+      <c r="B57" s="10"/>
+      <c r="C57" s="10"/>
+      <c r="D57" s="10"/>
+      <c r="E57" s="10"/>
+      <c r="F57" s="10"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="7" t="s">
+      <c r="A58" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="B58" s="7"/>
-      <c r="C58" s="7"/>
-      <c r="D58" s="7"/>
-      <c r="E58" s="7"/>
-      <c r="F58" s="7"/>
+      <c r="B58" s="10"/>
+      <c r="C58" s="10"/>
+      <c r="D58" s="10"/>
+      <c r="E58" s="10"/>
+      <c r="F58" s="10"/>
     </row>
     <row r="60" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
@@ -1265,67 +1265,47 @@
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="7" t="s">
+      <c r="A61" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="B61" s="7"/>
-      <c r="C61" s="7"/>
-      <c r="D61" s="7"/>
-      <c r="E61" s="7"/>
-      <c r="F61" s="7"/>
+      <c r="B61" s="10"/>
+      <c r="C61" s="10"/>
+      <c r="D61" s="10"/>
+      <c r="E61" s="10"/>
+      <c r="F61" s="10"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="7" t="s">
+      <c r="A62" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="B62" s="7"/>
-      <c r="C62" s="7"/>
-      <c r="D62" s="7"/>
-      <c r="E62" s="7"/>
-      <c r="F62" s="7"/>
+      <c r="B62" s="10"/>
+      <c r="C62" s="10"/>
+      <c r="D62" s="10"/>
+      <c r="E62" s="10"/>
+      <c r="F62" s="10"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="7" t="s">
+      <c r="A63" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="B63" s="7"/>
-      <c r="C63" s="7"/>
-      <c r="D63" s="7"/>
-      <c r="E63" s="7"/>
-      <c r="F63" s="7"/>
+      <c r="B63" s="10"/>
+      <c r="C63" s="10"/>
+      <c r="D63" s="10"/>
+      <c r="E63" s="10"/>
+      <c r="F63" s="10"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="7" t="s">
+      <c r="A64" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="B64" s="7"/>
-      <c r="C64" s="7"/>
-      <c r="D64" s="7"/>
-      <c r="E64" s="7"/>
-      <c r="F64" s="7"/>
+      <c r="B64" s="10"/>
+      <c r="C64" s="10"/>
+      <c r="D64" s="10"/>
+      <c r="E64" s="10"/>
+      <c r="F64" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A15:F15"/>
-    <mergeCell ref="A27:F27"/>
-    <mergeCell ref="A29:F29"/>
-    <mergeCell ref="A30:F30"/>
-    <mergeCell ref="A31:F31"/>
-    <mergeCell ref="A32:F32"/>
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="A34:F34"/>
-    <mergeCell ref="A37:F37"/>
-    <mergeCell ref="A38:F38"/>
-    <mergeCell ref="A39:F39"/>
-    <mergeCell ref="A42:F42"/>
-    <mergeCell ref="A43:F43"/>
-    <mergeCell ref="A44:F44"/>
-    <mergeCell ref="A45:F45"/>
-    <mergeCell ref="A48:F48"/>
-    <mergeCell ref="A49:F49"/>
-    <mergeCell ref="A50:F50"/>
-    <mergeCell ref="A51:F51"/>
     <mergeCell ref="A61:F61"/>
     <mergeCell ref="A62:F62"/>
     <mergeCell ref="A63:F63"/>
@@ -1335,6 +1315,26 @@
     <mergeCell ref="A56:F56"/>
     <mergeCell ref="A57:F57"/>
     <mergeCell ref="A58:F58"/>
+    <mergeCell ref="A45:F45"/>
+    <mergeCell ref="A48:F48"/>
+    <mergeCell ref="A49:F49"/>
+    <mergeCell ref="A50:F50"/>
+    <mergeCell ref="A51:F51"/>
+    <mergeCell ref="A38:F38"/>
+    <mergeCell ref="A39:F39"/>
+    <mergeCell ref="A42:F42"/>
+    <mergeCell ref="A43:F43"/>
+    <mergeCell ref="A44:F44"/>
+    <mergeCell ref="A31:F31"/>
+    <mergeCell ref="A32:F32"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A34:F34"/>
+    <mergeCell ref="A37:F37"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A15:F15"/>
+    <mergeCell ref="A27:F27"/>
+    <mergeCell ref="A29:F29"/>
+    <mergeCell ref="A30:F30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Finished implementing targeting system. Implemented walls
</commit_message>
<xml_diff>
--- a/Production Documents/To-Do.xlsx
+++ b/Production Documents/To-Do.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmgam\Desktop\Shiva\Production Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F135FB8-2C42-4112-B146-5AC004200565}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0434F781-E18E-4A2F-85EB-93AE87E94ACE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32010" yWindow="1455" windowWidth="16530" windowHeight="10125" xr2:uid="{669DCC34-C837-4342-A908-0F87EB315612}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{669DCC34-C837-4342-A908-0F87EB315612}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="77">
   <si>
     <t>Sprites</t>
   </si>
@@ -259,6 +259,9 @@
   </si>
   <si>
     <t>Home Base</t>
+  </si>
+  <si>
+    <t>Rudra - Attack</t>
   </si>
 </sst>
 </file>
@@ -360,7 +363,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
@@ -368,14 +371,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -698,10 +702,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4D254F2-4E19-40CF-BD85-766CDBA8C5EF}">
-  <dimension ref="A2:F64"/>
+  <dimension ref="A2:F66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -719,14 +723,14 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="18" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -775,8 +779,8 @@
       <c r="B6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>38</v>
+      <c r="C6" s="7" t="s">
+        <v>76</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>22</v>
@@ -796,7 +800,7 @@
         <v>17</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>23</v>
@@ -816,7 +820,7 @@
         <v>18</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="5" t="s">
@@ -832,7 +836,7 @@
         <v>19</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="5" t="s">
@@ -848,7 +852,7 @@
         <v>20</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
@@ -860,7 +864,7 @@
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
@@ -871,184 +875,174 @@
         <v>14</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C13" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C14" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
+    <row r="16" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A16" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-    </row>
-    <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="3" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C18" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D18" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E18" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F18" s="3" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E18" s="4"/>
-      <c r="F18" s="3" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>36</v>
+        <v>16</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>76</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20" s="4"/>
+      <c r="F20" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D20" s="4"/>
-      <c r="F20" s="4"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
       <c r="F21" s="4"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="C23" s="3" t="s">
-        <v>37</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C24" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C25" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C26" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C27" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="8" t="s">
+    <row r="29" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-    </row>
-    <row r="28" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+    </row>
+    <row r="30" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B29" s="9"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B32" s="9"/>
       <c r="C32" s="9"/>
@@ -1058,7 +1052,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
-        <v>47</v>
+        <v>74</v>
       </c>
       <c r="B33" s="9"/>
       <c r="C33" s="9"/>
@@ -1068,7 +1062,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B34" s="9"/>
       <c r="C34" s="9"/>
@@ -1076,265 +1070,285 @@
       <c r="E34" s="9"/>
       <c r="F34" s="9"/>
     </row>
-    <row r="36" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B36" s="9"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+    </row>
+    <row r="38" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="10" t="s">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="B37" s="10"/>
-      <c r="C37" s="10"/>
-      <c r="D37" s="10"/>
-      <c r="E37" s="10"/>
-      <c r="F37" s="10"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="10" t="s">
+      <c r="B39" s="8"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="B38" s="10"/>
-      <c r="C38" s="10"/>
-      <c r="D38" s="10"/>
-      <c r="E38" s="10"/>
-      <c r="F38" s="10"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="10" t="s">
+      <c r="B40" s="8"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="B39" s="10"/>
-      <c r="C39" s="10"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="10"/>
-      <c r="F39" s="10"/>
-    </row>
-    <row r="40" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="1"/>
-    </row>
-    <row r="41" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="1" t="s">
+      <c r="B41" s="8"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
+    </row>
+    <row r="42" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="1"/>
+    </row>
+    <row r="43" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="10" t="s">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="B42" s="10"/>
-      <c r="C42" s="10"/>
-      <c r="D42" s="10"/>
-      <c r="E42" s="10"/>
-      <c r="F42" s="10"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="10" t="s">
+      <c r="B44" s="9"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="9"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B43" s="10"/>
-      <c r="C43" s="10"/>
-      <c r="D43" s="10"/>
-      <c r="E43" s="10"/>
-      <c r="F43" s="10"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="10" t="s">
+      <c r="B45" s="9"/>
+      <c r="C45" s="9"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="9"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="B44" s="10"/>
-      <c r="C44" s="10"/>
-      <c r="D44" s="10"/>
-      <c r="E44" s="10"/>
-      <c r="F44" s="10"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="10" t="s">
+      <c r="B46" s="9"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="9"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B45" s="10"/>
-      <c r="C45" s="10"/>
-      <c r="D45" s="10"/>
-      <c r="E45" s="10"/>
-      <c r="F45" s="10"/>
-    </row>
-    <row r="47" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="1" t="s">
+      <c r="B47" s="9"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="9"/>
+    </row>
+    <row r="49" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="10" t="s">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B48" s="10"/>
-      <c r="C48" s="10"/>
-      <c r="D48" s="10"/>
-      <c r="E48" s="10"/>
-      <c r="F48" s="10"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="10" t="s">
+      <c r="B50" s="8"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="8"/>
+      <c r="E50" s="8"/>
+      <c r="F50" s="8"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="B49" s="10"/>
-      <c r="C49" s="10"/>
-      <c r="D49" s="10"/>
-      <c r="E49" s="10"/>
-      <c r="F49" s="10"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="10" t="s">
+      <c r="B51" s="8"/>
+      <c r="C51" s="8"/>
+      <c r="D51" s="8"/>
+      <c r="E51" s="8"/>
+      <c r="F51" s="8"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="B50" s="10"/>
-      <c r="C50" s="10"/>
-      <c r="D50" s="10"/>
-      <c r="E50" s="10"/>
-      <c r="F50" s="10"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="10" t="s">
+      <c r="B52" s="8"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="8"/>
+      <c r="E52" s="8"/>
+      <c r="F52" s="8"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B51" s="10"/>
-      <c r="C51" s="10"/>
-      <c r="D51" s="10"/>
-      <c r="E51" s="10"/>
-      <c r="F51" s="10"/>
-    </row>
-    <row r="53" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="1" t="s">
+      <c r="B53" s="8"/>
+      <c r="C53" s="8"/>
+      <c r="D53" s="8"/>
+      <c r="E53" s="8"/>
+      <c r="F53" s="8"/>
+    </row>
+    <row r="55" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="10" t="s">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="B54" s="10"/>
-      <c r="C54" s="10"/>
-      <c r="D54" s="10"/>
-      <c r="E54" s="10"/>
-      <c r="F54" s="10"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="10" t="s">
+      <c r="B56" s="8"/>
+      <c r="C56" s="8"/>
+      <c r="D56" s="8"/>
+      <c r="E56" s="8"/>
+      <c r="F56" s="8"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="B55" s="10"/>
-      <c r="C55" s="10"/>
-      <c r="D55" s="10"/>
-      <c r="E55" s="10"/>
-      <c r="F55" s="10"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="10" t="s">
+      <c r="B57" s="8"/>
+      <c r="C57" s="8"/>
+      <c r="D57" s="8"/>
+      <c r="E57" s="8"/>
+      <c r="F57" s="8"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="B56" s="10"/>
-      <c r="C56" s="10"/>
-      <c r="D56" s="10"/>
-      <c r="E56" s="10"/>
-      <c r="F56" s="10"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="10" t="s">
+      <c r="B58" s="8"/>
+      <c r="C58" s="8"/>
+      <c r="D58" s="8"/>
+      <c r="E58" s="8"/>
+      <c r="F58" s="8"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="B57" s="10"/>
-      <c r="C57" s="10"/>
-      <c r="D57" s="10"/>
-      <c r="E57" s="10"/>
-      <c r="F57" s="10"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="10" t="s">
+      <c r="B59" s="8"/>
+      <c r="C59" s="8"/>
+      <c r="D59" s="8"/>
+      <c r="E59" s="8"/>
+      <c r="F59" s="8"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="B58" s="10"/>
-      <c r="C58" s="10"/>
-      <c r="D58" s="10"/>
-      <c r="E58" s="10"/>
-      <c r="F58" s="10"/>
-    </row>
-    <row r="60" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="1" t="s">
+      <c r="B60" s="8"/>
+      <c r="C60" s="8"/>
+      <c r="D60" s="8"/>
+      <c r="E60" s="8"/>
+      <c r="F60" s="8"/>
+    </row>
+    <row r="62" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="10" t="s">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="B61" s="10"/>
-      <c r="C61" s="10"/>
-      <c r="D61" s="10"/>
-      <c r="E61" s="10"/>
-      <c r="F61" s="10"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="10" t="s">
+      <c r="B63" s="8"/>
+      <c r="C63" s="8"/>
+      <c r="D63" s="8"/>
+      <c r="E63" s="8"/>
+      <c r="F63" s="8"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="B62" s="10"/>
-      <c r="C62" s="10"/>
-      <c r="D62" s="10"/>
-      <c r="E62" s="10"/>
-      <c r="F62" s="10"/>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="10" t="s">
+      <c r="B64" s="8"/>
+      <c r="C64" s="8"/>
+      <c r="D64" s="8"/>
+      <c r="E64" s="8"/>
+      <c r="F64" s="8"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B63" s="10"/>
-      <c r="C63" s="10"/>
-      <c r="D63" s="10"/>
-      <c r="E63" s="10"/>
-      <c r="F63" s="10"/>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="10" t="s">
+      <c r="B65" s="8"/>
+      <c r="C65" s="8"/>
+      <c r="D65" s="8"/>
+      <c r="E65" s="8"/>
+      <c r="F65" s="8"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="B64" s="10"/>
-      <c r="C64" s="10"/>
-      <c r="D64" s="10"/>
-      <c r="E64" s="10"/>
-      <c r="F64" s="10"/>
+      <c r="B66" s="8"/>
+      <c r="C66" s="8"/>
+      <c r="D66" s="8"/>
+      <c r="E66" s="8"/>
+      <c r="F66" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="A61:F61"/>
-    <mergeCell ref="A62:F62"/>
-    <mergeCell ref="A63:F63"/>
-    <mergeCell ref="A64:F64"/>
-    <mergeCell ref="A54:F54"/>
-    <mergeCell ref="A55:F55"/>
-    <mergeCell ref="A56:F56"/>
-    <mergeCell ref="A57:F57"/>
-    <mergeCell ref="A58:F58"/>
-    <mergeCell ref="A45:F45"/>
-    <mergeCell ref="A48:F48"/>
-    <mergeCell ref="A49:F49"/>
-    <mergeCell ref="A50:F50"/>
-    <mergeCell ref="A51:F51"/>
-    <mergeCell ref="A38:F38"/>
-    <mergeCell ref="A39:F39"/>
-    <mergeCell ref="A42:F42"/>
-    <mergeCell ref="A43:F43"/>
-    <mergeCell ref="A44:F44"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A29:F29"/>
     <mergeCell ref="A31:F31"/>
     <mergeCell ref="A32:F32"/>
     <mergeCell ref="A33:F33"/>
     <mergeCell ref="A34:F34"/>
-    <mergeCell ref="A37:F37"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A15:F15"/>
-    <mergeCell ref="A27:F27"/>
-    <mergeCell ref="A29:F29"/>
-    <mergeCell ref="A30:F30"/>
+    <mergeCell ref="A35:F35"/>
+    <mergeCell ref="A36:F36"/>
+    <mergeCell ref="A39:F39"/>
+    <mergeCell ref="A40:F40"/>
+    <mergeCell ref="A41:F41"/>
+    <mergeCell ref="A44:F44"/>
+    <mergeCell ref="A45:F45"/>
+    <mergeCell ref="A46:F46"/>
+    <mergeCell ref="A47:F47"/>
+    <mergeCell ref="A50:F50"/>
+    <mergeCell ref="A51:F51"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="A53:F53"/>
+    <mergeCell ref="A63:F63"/>
+    <mergeCell ref="A64:F64"/>
+    <mergeCell ref="A65:F65"/>
+    <mergeCell ref="A66:F66"/>
+    <mergeCell ref="A56:F56"/>
+    <mergeCell ref="A57:F57"/>
+    <mergeCell ref="A58:F58"/>
+    <mergeCell ref="A59:F59"/>
+    <mergeCell ref="A60:F60"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Made sprites for civilians in ShivaSprites folder. Made new sprites for home base and spawn pods and added to the main game
</commit_message>
<xml_diff>
--- a/Production Documents/To-Do.xlsx
+++ b/Production Documents/To-Do.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmgam\Desktop\Shiva\Production Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Shiva\Production Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0434F781-E18E-4A2F-85EB-93AE87E94ACE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E8F4BF3-9A72-41FA-AE19-6785223643EF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{669DCC34-C837-4342-A908-0F87EB315612}"/>
+    <workbookView xWindow="5760" yWindow="3996" windowWidth="17280" windowHeight="8964" xr2:uid="{669DCC34-C837-4342-A908-0F87EB315612}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -363,7 +363,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
@@ -372,7 +372,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -380,6 +379,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -705,34 +706,34 @@
   <dimension ref="A2:F66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="18" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
+    <row r="3" spans="1:6" ht="18" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+    </row>
+    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -752,11 +753,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="5" t="s">
@@ -772,7 +773,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -792,7 +793,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
@@ -812,7 +813,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
@@ -828,7 +829,7 @@
       </c>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
@@ -844,7 +845,7 @@
       </c>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
@@ -858,8 +859,8 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="4"/>
@@ -870,7 +871,7 @@
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
@@ -878,27 +879,27 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C13" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C14" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A16" s="10" t="s">
+    <row r="16" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A16" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-    </row>
-    <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+    </row>
+    <row r="17" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
         <v>3</v>
@@ -916,8 +917,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="3" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B18" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -933,7 +934,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
@@ -948,7 +949,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
@@ -963,7 +964,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B21" s="3" t="s">
         <v>18</v>
       </c>
@@ -973,7 +974,7 @@
       <c r="D21" s="4"/>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B22" s="3" t="s">
         <v>19</v>
       </c>
@@ -984,7 +985,7 @@
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B23" s="3" t="s">
         <v>20</v>
       </c>
@@ -995,351 +996,331 @@
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C24" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C25" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C26" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C27" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="11" t="s">
+    <row r="29" spans="1:6" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A29" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="11"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-    </row>
-    <row r="30" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+    </row>
+    <row r="30" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="9" t="s">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="9" t="s">
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="B32" s="9"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="9"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="9" t="s">
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="B33" s="9"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="9" t="s">
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="B34" s="9"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="9" t="s">
+      <c r="B34" s="11"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="B35" s="9"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="9" t="s">
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="B36" s="9"/>
-      <c r="C36" s="9"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="9"/>
-    </row>
-    <row r="38" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="11"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+    </row>
+    <row r="38" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="8" t="s">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="B39" s="8"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
-      <c r="F39" s="8"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="8" t="s">
+      <c r="B39" s="12"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="12"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="B40" s="8"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
-      <c r="F40" s="8"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="8" t="s">
+      <c r="B40" s="12"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="12"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="B41" s="8"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="8"/>
-      <c r="F41" s="8"/>
-    </row>
-    <row r="42" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="12"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="12"/>
+      <c r="F41" s="12"/>
+    </row>
+    <row r="42" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="1"/>
     </row>
-    <row r="43" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="9" t="s">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B44" s="9"/>
-      <c r="C44" s="9"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="9"/>
-      <c r="F44" s="9"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="9" t="s">
+      <c r="B44" s="11"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="11"/>
+      <c r="E44" s="11"/>
+      <c r="F44" s="11"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="B45" s="9"/>
-      <c r="C45" s="9"/>
-      <c r="D45" s="9"/>
-      <c r="E45" s="9"/>
-      <c r="F45" s="9"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="9" t="s">
+      <c r="B45" s="11"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="11"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="B46" s="9"/>
-      <c r="C46" s="9"/>
-      <c r="D46" s="9"/>
-      <c r="E46" s="9"/>
-      <c r="F46" s="9"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="9" t="s">
+      <c r="B46" s="11"/>
+      <c r="C46" s="11"/>
+      <c r="D46" s="11"/>
+      <c r="E46" s="11"/>
+      <c r="F46" s="11"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="B47" s="9"/>
-      <c r="C47" s="9"/>
-      <c r="D47" s="9"/>
-      <c r="E47" s="9"/>
-      <c r="F47" s="9"/>
-    </row>
-    <row r="49" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="11"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="11"/>
+      <c r="E47" s="11"/>
+      <c r="F47" s="11"/>
+    </row>
+    <row r="49" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="8" t="s">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="B50" s="8"/>
-      <c r="C50" s="8"/>
-      <c r="D50" s="8"/>
-      <c r="E50" s="8"/>
-      <c r="F50" s="8"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="8" t="s">
+      <c r="B50" s="12"/>
+      <c r="C50" s="12"/>
+      <c r="D50" s="12"/>
+      <c r="E50" s="12"/>
+      <c r="F50" s="12"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="B51" s="8"/>
-      <c r="C51" s="8"/>
-      <c r="D51" s="8"/>
-      <c r="E51" s="8"/>
-      <c r="F51" s="8"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="8" t="s">
+      <c r="B51" s="12"/>
+      <c r="C51" s="12"/>
+      <c r="D51" s="12"/>
+      <c r="E51" s="12"/>
+      <c r="F51" s="12"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B52" s="8"/>
-      <c r="C52" s="8"/>
-      <c r="D52" s="8"/>
-      <c r="E52" s="8"/>
-      <c r="F52" s="8"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="8" t="s">
+      <c r="B52" s="12"/>
+      <c r="C52" s="12"/>
+      <c r="D52" s="12"/>
+      <c r="E52" s="12"/>
+      <c r="F52" s="12"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="B53" s="8"/>
-      <c r="C53" s="8"/>
-      <c r="D53" s="8"/>
-      <c r="E53" s="8"/>
-      <c r="F53" s="8"/>
-    </row>
-    <row r="55" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="12"/>
+      <c r="C53" s="12"/>
+      <c r="D53" s="12"/>
+      <c r="E53" s="12"/>
+      <c r="F53" s="12"/>
+    </row>
+    <row r="55" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="8" t="s">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="B56" s="8"/>
-      <c r="C56" s="8"/>
-      <c r="D56" s="8"/>
-      <c r="E56" s="8"/>
-      <c r="F56" s="8"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="8" t="s">
+      <c r="B56" s="12"/>
+      <c r="C56" s="12"/>
+      <c r="D56" s="12"/>
+      <c r="E56" s="12"/>
+      <c r="F56" s="12"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="B57" s="8"/>
-      <c r="C57" s="8"/>
-      <c r="D57" s="8"/>
-      <c r="E57" s="8"/>
-      <c r="F57" s="8"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="8" t="s">
+      <c r="B57" s="12"/>
+      <c r="C57" s="12"/>
+      <c r="D57" s="12"/>
+      <c r="E57" s="12"/>
+      <c r="F57" s="12"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="B58" s="8"/>
-      <c r="C58" s="8"/>
-      <c r="D58" s="8"/>
-      <c r="E58" s="8"/>
-      <c r="F58" s="8"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="8" t="s">
+      <c r="B58" s="12"/>
+      <c r="C58" s="12"/>
+      <c r="D58" s="12"/>
+      <c r="E58" s="12"/>
+      <c r="F58" s="12"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B59" s="8"/>
-      <c r="C59" s="8"/>
-      <c r="D59" s="8"/>
-      <c r="E59" s="8"/>
-      <c r="F59" s="8"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="8" t="s">
+      <c r="B59" s="12"/>
+      <c r="C59" s="12"/>
+      <c r="D59" s="12"/>
+      <c r="E59" s="12"/>
+      <c r="F59" s="12"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="B60" s="8"/>
-      <c r="C60" s="8"/>
-      <c r="D60" s="8"/>
-      <c r="E60" s="8"/>
-      <c r="F60" s="8"/>
-    </row>
-    <row r="62" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B60" s="12"/>
+      <c r="C60" s="12"/>
+      <c r="D60" s="12"/>
+      <c r="E60" s="12"/>
+      <c r="F60" s="12"/>
+    </row>
+    <row r="62" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="8" t="s">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="B63" s="8"/>
-      <c r="C63" s="8"/>
-      <c r="D63" s="8"/>
-      <c r="E63" s="8"/>
-      <c r="F63" s="8"/>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="8" t="s">
+      <c r="B63" s="12"/>
+      <c r="C63" s="12"/>
+      <c r="D63" s="12"/>
+      <c r="E63" s="12"/>
+      <c r="F63" s="12"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="B64" s="8"/>
-      <c r="C64" s="8"/>
-      <c r="D64" s="8"/>
-      <c r="E64" s="8"/>
-      <c r="F64" s="8"/>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="8" t="s">
+      <c r="B64" s="12"/>
+      <c r="C64" s="12"/>
+      <c r="D64" s="12"/>
+      <c r="E64" s="12"/>
+      <c r="F64" s="12"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A65" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="B65" s="8"/>
-      <c r="C65" s="8"/>
-      <c r="D65" s="8"/>
-      <c r="E65" s="8"/>
-      <c r="F65" s="8"/>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="8" t="s">
+      <c r="B65" s="12"/>
+      <c r="C65" s="12"/>
+      <c r="D65" s="12"/>
+      <c r="E65" s="12"/>
+      <c r="F65" s="12"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A66" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="B66" s="8"/>
-      <c r="C66" s="8"/>
-      <c r="D66" s="8"/>
-      <c r="E66" s="8"/>
-      <c r="F66" s="8"/>
+      <c r="B66" s="12"/>
+      <c r="C66" s="12"/>
+      <c r="D66" s="12"/>
+      <c r="E66" s="12"/>
+      <c r="F66" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A16:F16"/>
-    <mergeCell ref="A29:F29"/>
-    <mergeCell ref="A31:F31"/>
-    <mergeCell ref="A32:F32"/>
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="A34:F34"/>
-    <mergeCell ref="A35:F35"/>
-    <mergeCell ref="A36:F36"/>
-    <mergeCell ref="A39:F39"/>
-    <mergeCell ref="A40:F40"/>
-    <mergeCell ref="A41:F41"/>
-    <mergeCell ref="A44:F44"/>
-    <mergeCell ref="A45:F45"/>
-    <mergeCell ref="A46:F46"/>
-    <mergeCell ref="A47:F47"/>
-    <mergeCell ref="A50:F50"/>
-    <mergeCell ref="A51:F51"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="A53:F53"/>
     <mergeCell ref="A63:F63"/>
     <mergeCell ref="A64:F64"/>
     <mergeCell ref="A65:F65"/>
@@ -1349,6 +1330,26 @@
     <mergeCell ref="A58:F58"/>
     <mergeCell ref="A59:F59"/>
     <mergeCell ref="A60:F60"/>
+    <mergeCell ref="A47:F47"/>
+    <mergeCell ref="A50:F50"/>
+    <mergeCell ref="A51:F51"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="A53:F53"/>
+    <mergeCell ref="A40:F40"/>
+    <mergeCell ref="A41:F41"/>
+    <mergeCell ref="A44:F44"/>
+    <mergeCell ref="A45:F45"/>
+    <mergeCell ref="A46:F46"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A34:F34"/>
+    <mergeCell ref="A35:F35"/>
+    <mergeCell ref="A36:F36"/>
+    <mergeCell ref="A39:F39"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A29:F29"/>
+    <mergeCell ref="A31:F31"/>
+    <mergeCell ref="A32:F32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Made sprites for Indra
</commit_message>
<xml_diff>
--- a/Production Documents/To-Do.xlsx
+++ b/Production Documents/To-Do.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Shiva\Production Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmgam\Desktop\Shiva\Production Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E8F4BF3-9A72-41FA-AE19-6785223643EF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D67E314C-A697-4762-BC2E-CBEA92DF23BC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="3996" windowWidth="17280" windowHeight="8964" xr2:uid="{669DCC34-C837-4342-A908-0F87EB315612}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{669DCC34-C837-4342-A908-0F87EB315612}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -363,7 +363,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
@@ -373,14 +373,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -706,34 +707,34 @@
   <dimension ref="A2:F66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="18" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="9" t="s">
+    <row r="3" spans="1:6" ht="18" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-    </row>
-    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -753,7 +754,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>75</v>
       </c>
@@ -773,7 +774,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -793,7 +794,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
@@ -813,7 +814,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
@@ -829,7 +830,7 @@
       </c>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
@@ -845,7 +846,7 @@
       </c>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
@@ -859,7 +860,7 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>13</v>
       </c>
@@ -871,7 +872,7 @@
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
@@ -879,27 +880,27 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C13" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C14" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A16" s="9" t="s">
+    <row r="16" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A16" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-    </row>
-    <row r="17" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
         <v>3</v>
@@ -917,14 +918,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B18" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="9" t="s">
         <v>21</v>
       </c>
       <c r="E18" s="3" t="s">
@@ -934,7 +935,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
@@ -949,7 +950,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
@@ -964,7 +965,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
         <v>18</v>
       </c>
@@ -974,18 +975,18 @@
       <c r="D21" s="4"/>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="9" t="s">
         <v>32</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
         <v>20</v>
       </c>
@@ -996,42 +997,42 @@
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C24" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C25" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C26" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C27" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="10" t="s">
+    <row r="29" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
-    </row>
-    <row r="30" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="13"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+    </row>
+    <row r="30" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
         <v>44</v>
       </c>
@@ -1041,7 +1042,7 @@
       <c r="E31" s="11"/>
       <c r="F31" s="11"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>45</v>
       </c>
@@ -1051,7 +1052,7 @@
       <c r="E32" s="11"/>
       <c r="F32" s="11"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
         <v>74</v>
       </c>
@@ -1061,7 +1062,7 @@
       <c r="E33" s="11"/>
       <c r="F33" s="11"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
         <v>46</v>
       </c>
@@ -1071,7 +1072,7 @@
       <c r="E34" s="11"/>
       <c r="F34" s="11"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>47</v>
       </c>
@@ -1081,7 +1082,7 @@
       <c r="E35" s="11"/>
       <c r="F35" s="11"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
         <v>48</v>
       </c>
@@ -1091,50 +1092,50 @@
       <c r="E36" s="11"/>
       <c r="F36" s="11"/>
     </row>
-    <row r="38" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="12" t="s">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="B39" s="12"/>
-      <c r="C39" s="12"/>
-      <c r="D39" s="12"/>
-      <c r="E39" s="12"/>
-      <c r="F39" s="12"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="12" t="s">
+      <c r="B39" s="10"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="B40" s="12"/>
-      <c r="C40" s="12"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="12"/>
-      <c r="F40" s="12"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" s="12" t="s">
+      <c r="B40" s="10"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="B41" s="12"/>
-      <c r="C41" s="12"/>
-      <c r="D41" s="12"/>
-      <c r="E41" s="12"/>
-      <c r="F41" s="12"/>
-    </row>
-    <row r="42" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B41" s="10"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+    </row>
+    <row r="42" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
     </row>
-    <row r="43" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
         <v>49</v>
       </c>
@@ -1144,7 +1145,7 @@
       <c r="E44" s="11"/>
       <c r="F44" s="11"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
         <v>50</v>
       </c>
@@ -1154,7 +1155,7 @@
       <c r="E45" s="11"/>
       <c r="F45" s="11"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="11" t="s">
         <v>52</v>
       </c>
@@ -1164,7 +1165,7 @@
       <c r="E46" s="11"/>
       <c r="F46" s="11"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="11" t="s">
         <v>53</v>
       </c>
@@ -1174,153 +1175,173 @@
       <c r="E47" s="11"/>
       <c r="F47" s="11"/>
     </row>
-    <row r="49" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" s="12" t="s">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B50" s="12"/>
-      <c r="C50" s="12"/>
-      <c r="D50" s="12"/>
-      <c r="E50" s="12"/>
-      <c r="F50" s="12"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" s="12" t="s">
+      <c r="B50" s="10"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="10"/>
+      <c r="E50" s="10"/>
+      <c r="F50" s="10"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="B51" s="12"/>
-      <c r="C51" s="12"/>
-      <c r="D51" s="12"/>
-      <c r="E51" s="12"/>
-      <c r="F51" s="12"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52" s="12" t="s">
+      <c r="B51" s="10"/>
+      <c r="C51" s="10"/>
+      <c r="D51" s="10"/>
+      <c r="E51" s="10"/>
+      <c r="F51" s="10"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="B52" s="12"/>
-      <c r="C52" s="12"/>
-      <c r="D52" s="12"/>
-      <c r="E52" s="12"/>
-      <c r="F52" s="12"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53" s="12" t="s">
+      <c r="B52" s="10"/>
+      <c r="C52" s="10"/>
+      <c r="D52" s="10"/>
+      <c r="E52" s="10"/>
+      <c r="F52" s="10"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="B53" s="12"/>
-      <c r="C53" s="12"/>
-      <c r="D53" s="12"/>
-      <c r="E53" s="12"/>
-      <c r="F53" s="12"/>
-    </row>
-    <row r="55" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B53" s="10"/>
+      <c r="C53" s="10"/>
+      <c r="D53" s="10"/>
+      <c r="E53" s="10"/>
+      <c r="F53" s="10"/>
+    </row>
+    <row r="55" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A56" s="12" t="s">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="B56" s="12"/>
-      <c r="C56" s="12"/>
-      <c r="D56" s="12"/>
-      <c r="E56" s="12"/>
-      <c r="F56" s="12"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A57" s="12" t="s">
+      <c r="B56" s="10"/>
+      <c r="C56" s="10"/>
+      <c r="D56" s="10"/>
+      <c r="E56" s="10"/>
+      <c r="F56" s="10"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="B57" s="12"/>
-      <c r="C57" s="12"/>
-      <c r="D57" s="12"/>
-      <c r="E57" s="12"/>
-      <c r="F57" s="12"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A58" s="12" t="s">
+      <c r="B57" s="10"/>
+      <c r="C57" s="10"/>
+      <c r="D57" s="10"/>
+      <c r="E57" s="10"/>
+      <c r="F57" s="10"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="B58" s="12"/>
-      <c r="C58" s="12"/>
-      <c r="D58" s="12"/>
-      <c r="E58" s="12"/>
-      <c r="F58" s="12"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A59" s="12" t="s">
+      <c r="B58" s="10"/>
+      <c r="C58" s="10"/>
+      <c r="D58" s="10"/>
+      <c r="E58" s="10"/>
+      <c r="F58" s="10"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="B59" s="12"/>
-      <c r="C59" s="12"/>
-      <c r="D59" s="12"/>
-      <c r="E59" s="12"/>
-      <c r="F59" s="12"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A60" s="12" t="s">
+      <c r="B59" s="10"/>
+      <c r="C59" s="10"/>
+      <c r="D59" s="10"/>
+      <c r="E59" s="10"/>
+      <c r="F59" s="10"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="B60" s="12"/>
-      <c r="C60" s="12"/>
-      <c r="D60" s="12"/>
-      <c r="E60" s="12"/>
-      <c r="F60" s="12"/>
-    </row>
-    <row r="62" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B60" s="10"/>
+      <c r="C60" s="10"/>
+      <c r="D60" s="10"/>
+      <c r="E60" s="10"/>
+      <c r="F60" s="10"/>
+    </row>
+    <row r="62" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A63" s="12" t="s">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="B63" s="12"/>
-      <c r="C63" s="12"/>
-      <c r="D63" s="12"/>
-      <c r="E63" s="12"/>
-      <c r="F63" s="12"/>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A64" s="12" t="s">
+      <c r="B63" s="10"/>
+      <c r="C63" s="10"/>
+      <c r="D63" s="10"/>
+      <c r="E63" s="10"/>
+      <c r="F63" s="10"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="B64" s="12"/>
-      <c r="C64" s="12"/>
-      <c r="D64" s="12"/>
-      <c r="E64" s="12"/>
-      <c r="F64" s="12"/>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A65" s="12" t="s">
+      <c r="B64" s="10"/>
+      <c r="C64" s="10"/>
+      <c r="D64" s="10"/>
+      <c r="E64" s="10"/>
+      <c r="F64" s="10"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="B65" s="12"/>
-      <c r="C65" s="12"/>
-      <c r="D65" s="12"/>
-      <c r="E65" s="12"/>
-      <c r="F65" s="12"/>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A66" s="12" t="s">
+      <c r="B65" s="10"/>
+      <c r="C65" s="10"/>
+      <c r="D65" s="10"/>
+      <c r="E65" s="10"/>
+      <c r="F65" s="10"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="B66" s="12"/>
-      <c r="C66" s="12"/>
-      <c r="D66" s="12"/>
-      <c r="E66" s="12"/>
-      <c r="F66" s="12"/>
+      <c r="B66" s="10"/>
+      <c r="C66" s="10"/>
+      <c r="D66" s="10"/>
+      <c r="E66" s="10"/>
+      <c r="F66" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A29:F29"/>
+    <mergeCell ref="A31:F31"/>
+    <mergeCell ref="A32:F32"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A34:F34"/>
+    <mergeCell ref="A35:F35"/>
+    <mergeCell ref="A36:F36"/>
+    <mergeCell ref="A39:F39"/>
+    <mergeCell ref="A40:F40"/>
+    <mergeCell ref="A41:F41"/>
+    <mergeCell ref="A44:F44"/>
+    <mergeCell ref="A45:F45"/>
+    <mergeCell ref="A46:F46"/>
+    <mergeCell ref="A47:F47"/>
+    <mergeCell ref="A50:F50"/>
+    <mergeCell ref="A51:F51"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="A53:F53"/>
     <mergeCell ref="A63:F63"/>
     <mergeCell ref="A64:F64"/>
     <mergeCell ref="A65:F65"/>
@@ -1330,26 +1351,6 @@
     <mergeCell ref="A58:F58"/>
     <mergeCell ref="A59:F59"/>
     <mergeCell ref="A60:F60"/>
-    <mergeCell ref="A47:F47"/>
-    <mergeCell ref="A50:F50"/>
-    <mergeCell ref="A51:F51"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="A53:F53"/>
-    <mergeCell ref="A40:F40"/>
-    <mergeCell ref="A41:F41"/>
-    <mergeCell ref="A44:F44"/>
-    <mergeCell ref="A45:F45"/>
-    <mergeCell ref="A46:F46"/>
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="A34:F34"/>
-    <mergeCell ref="A35:F35"/>
-    <mergeCell ref="A36:F36"/>
-    <mergeCell ref="A39:F39"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A16:F16"/>
-    <mergeCell ref="A29:F29"/>
-    <mergeCell ref="A31:F31"/>
-    <mergeCell ref="A32:F32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed some bugs regarding having units pick a target to move to. Units shouldn't be moving to the same tile anymore. Made the 'Next Round' button only visable during prep rounds. Killing all enemies on the board ends invasion rounds. The global variable global.enemiesOnBoard keeps track of how many enemies are still left to be killed before the invasion round ends. Implemented the player being able to have a soldier destroy a spawn pod if it is next to it. This is done by clicking the movement button and selecting the spawn pod. Spawn pods that can be destroyed have their tile show a red overlay.
</commit_message>
<xml_diff>
--- a/Production Documents/To-Do.xlsx
+++ b/Production Documents/To-Do.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmgam\Desktop\Shiva\Production Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D67E314C-A697-4762-BC2E-CBEA92DF23BC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C1F7170-44FA-4AD4-BF52-D3AA36BFFCA9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{669DCC34-C837-4342-A908-0F87EB315612}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="81">
   <si>
     <t>Sprites</t>
   </si>
@@ -262,6 +262,18 @@
   </si>
   <si>
     <t>Rudra - Attack</t>
+  </si>
+  <si>
+    <t>Aliens attack walls when neccisary</t>
+  </si>
+  <si>
+    <t>The player may direct soldiers to attack spawn pods during prep rounds</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Spawn pods are generated at the start of invasion rounds</t>
   </si>
 </sst>
 </file>
@@ -301,7 +313,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -317,6 +329,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -363,7 +381,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
@@ -375,13 +393,15 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -704,10 +724,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4D254F2-4E19-40CF-BD85-766CDBA8C5EF}">
-  <dimension ref="A2:F66"/>
+  <dimension ref="A2:F71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="I52" sqref="I52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -725,14 +745,14 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="18" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -891,14 +911,14 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
@@ -1018,14 +1038,14 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="13" t="s">
+      <c r="A29" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="13"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
     </row>
     <row r="30" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
@@ -1033,64 +1053,64 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="11" t="s">
+      <c r="A31" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B31" s="11"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="11" t="s">
+      <c r="A32" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="B32" s="11"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="11" t="s">
+      <c r="A33" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="B33" s="11"/>
-      <c r="C33" s="11"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="11" t="s">
+      <c r="A34" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="B34" s="11"/>
-      <c r="C34" s="11"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="11"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="11" t="s">
+      <c r="A35" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="B35" s="11"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11"/>
-      <c r="E35" s="11"/>
-      <c r="F35" s="11"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="11" t="s">
+      <c r="A36" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="B36" s="11"/>
-      <c r="C36" s="11"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="11"/>
-      <c r="F36" s="11"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
     </row>
     <row r="38" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
@@ -1098,34 +1118,34 @@
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="10" t="s">
+      <c r="A39" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="B39" s="10"/>
-      <c r="C39" s="10"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="10"/>
-      <c r="F39" s="10"/>
+      <c r="B39" s="14"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="14"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="10" t="s">
+      <c r="A40" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="B40" s="10"/>
-      <c r="C40" s="10"/>
-      <c r="D40" s="10"/>
-      <c r="E40" s="10"/>
-      <c r="F40" s="10"/>
+      <c r="B40" s="14"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="10" t="s">
+      <c r="A41" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="B41" s="10"/>
-      <c r="C41" s="10"/>
-      <c r="D41" s="10"/>
-      <c r="E41" s="10"/>
-      <c r="F41" s="10"/>
+      <c r="B41" s="14"/>
+      <c r="C41" s="14"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="14"/>
     </row>
     <row r="42" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
@@ -1136,221 +1156,256 @@
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="11" t="s">
+      <c r="A44" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="B44" s="11"/>
-      <c r="C44" s="11"/>
-      <c r="D44" s="11"/>
-      <c r="E44" s="11"/>
-      <c r="F44" s="11"/>
+      <c r="B44" s="13"/>
+      <c r="C44" s="13"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="13"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="11" t="s">
+      <c r="A45" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="B45" s="11"/>
-      <c r="C45" s="11"/>
-      <c r="D45" s="11"/>
-      <c r="E45" s="11"/>
-      <c r="F45" s="11"/>
+      <c r="B45" s="13"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="13"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="11" t="s">
+      <c r="A46" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="B46" s="11"/>
-      <c r="C46" s="11"/>
-      <c r="D46" s="11"/>
-      <c r="E46" s="11"/>
-      <c r="F46" s="11"/>
+      <c r="B46" s="13"/>
+      <c r="C46" s="13"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="13"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="11" t="s">
+      <c r="A47" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="B47" s="11"/>
-      <c r="C47" s="11"/>
-      <c r="D47" s="11"/>
-      <c r="E47" s="11"/>
-      <c r="F47" s="11"/>
-    </row>
-    <row r="49" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="1" t="s">
+      <c r="B47" s="13"/>
+      <c r="C47" s="13"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="13"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B48" s="10"/>
+      <c r="C48" s="10"/>
+      <c r="D48" s="10"/>
+      <c r="E48" s="10"/>
+      <c r="F48" s="10"/>
+    </row>
+    <row r="50" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="10" t="s">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="B50" s="10"/>
-      <c r="C50" s="10"/>
-      <c r="D50" s="10"/>
-      <c r="E50" s="10"/>
-      <c r="F50" s="10"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="10" t="s">
+      <c r="B51" s="13"/>
+      <c r="C51" s="13"/>
+      <c r="D51" s="13"/>
+      <c r="E51" s="13"/>
+      <c r="F51" s="13"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="B51" s="10"/>
-      <c r="C51" s="10"/>
-      <c r="D51" s="10"/>
-      <c r="E51" s="10"/>
-      <c r="F51" s="10"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="10" t="s">
+      <c r="B52" s="13"/>
+      <c r="C52" s="13"/>
+      <c r="D52" s="13"/>
+      <c r="E52" s="13"/>
+      <c r="F52" s="13"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B52" s="10"/>
-      <c r="C52" s="10"/>
-      <c r="D52" s="10"/>
-      <c r="E52" s="10"/>
-      <c r="F52" s="10"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="10" t="s">
+      <c r="B53" s="13"/>
+      <c r="C53" s="13"/>
+      <c r="D53" s="13"/>
+      <c r="E53" s="13"/>
+      <c r="F53" s="13"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="B53" s="10"/>
-      <c r="C53" s="10"/>
-      <c r="D53" s="10"/>
-      <c r="E53" s="10"/>
-      <c r="F53" s="10"/>
-    </row>
-    <row r="55" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="1" t="s">
+      <c r="B54" s="14"/>
+      <c r="C54" s="14"/>
+      <c r="D54" s="14"/>
+      <c r="E54" s="14"/>
+      <c r="F54" s="14"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B55" s="15"/>
+      <c r="C55" s="15"/>
+      <c r="D55" s="15"/>
+      <c r="E55" s="15"/>
+      <c r="F55" s="15"/>
+    </row>
+    <row r="57" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="10" t="s">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="B56" s="10"/>
-      <c r="C56" s="10"/>
-      <c r="D56" s="10"/>
-      <c r="E56" s="10"/>
-      <c r="F56" s="10"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="10" t="s">
+      <c r="B58" s="14"/>
+      <c r="C58" s="14"/>
+      <c r="D58" s="14"/>
+      <c r="E58" s="14"/>
+      <c r="F58" s="14"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="B57" s="10"/>
-      <c r="C57" s="10"/>
-      <c r="D57" s="10"/>
-      <c r="E57" s="10"/>
-      <c r="F57" s="10"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="10" t="s">
+      <c r="B59" s="14"/>
+      <c r="C59" s="14"/>
+      <c r="D59" s="14"/>
+      <c r="E59" s="14"/>
+      <c r="F59" s="14"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="B58" s="10"/>
-      <c r="C58" s="10"/>
-      <c r="D58" s="10"/>
-      <c r="E58" s="10"/>
-      <c r="F58" s="10"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="10" t="s">
+      <c r="B60" s="14"/>
+      <c r="C60" s="14"/>
+      <c r="D60" s="14"/>
+      <c r="E60" s="14"/>
+      <c r="F60" s="14"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="B59" s="10"/>
-      <c r="C59" s="10"/>
-      <c r="D59" s="10"/>
-      <c r="E59" s="10"/>
-      <c r="F59" s="10"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="10" t="s">
+      <c r="B61" s="14"/>
+      <c r="C61" s="14"/>
+      <c r="D61" s="14"/>
+      <c r="E61" s="14"/>
+      <c r="F61" s="14"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="B60" s="10"/>
-      <c r="C60" s="10"/>
-      <c r="D60" s="10"/>
-      <c r="E60" s="10"/>
-      <c r="F60" s="10"/>
-    </row>
-    <row r="62" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="1" t="s">
+      <c r="B62" s="14"/>
+      <c r="C62" s="14"/>
+      <c r="D62" s="14"/>
+      <c r="E62" s="14"/>
+      <c r="F62" s="14"/>
+    </row>
+    <row r="64" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="10" t="s">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="B63" s="10"/>
-      <c r="C63" s="10"/>
-      <c r="D63" s="10"/>
-      <c r="E63" s="10"/>
-      <c r="F63" s="10"/>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="10" t="s">
+      <c r="B65" s="14"/>
+      <c r="C65" s="14"/>
+      <c r="D65" s="14"/>
+      <c r="E65" s="14"/>
+      <c r="F65" s="14"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="B64" s="10"/>
-      <c r="C64" s="10"/>
-      <c r="D64" s="10"/>
-      <c r="E64" s="10"/>
-      <c r="F64" s="10"/>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="10" t="s">
+      <c r="B66" s="14"/>
+      <c r="C66" s="14"/>
+      <c r="D66" s="14"/>
+      <c r="E66" s="14"/>
+      <c r="F66" s="14"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="B65" s="10"/>
-      <c r="C65" s="10"/>
-      <c r="D65" s="10"/>
-      <c r="E65" s="10"/>
-      <c r="F65" s="10"/>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="10" t="s">
+      <c r="B67" s="14"/>
+      <c r="C67" s="14"/>
+      <c r="D67" s="14"/>
+      <c r="E67" s="14"/>
+      <c r="F67" s="14"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="B66" s="10"/>
-      <c r="C66" s="10"/>
-      <c r="D66" s="10"/>
-      <c r="E66" s="10"/>
-      <c r="F66" s="10"/>
+      <c r="B68" s="14"/>
+      <c r="C68" s="14"/>
+      <c r="D68" s="14"/>
+      <c r="E68" s="14"/>
+      <c r="F68" s="14"/>
+    </row>
+    <row r="70" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B71" s="10"/>
+      <c r="C71" s="10"/>
+      <c r="D71" s="10"/>
+      <c r="E71" s="10"/>
+      <c r="F71" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="A65:F65"/>
+    <mergeCell ref="A66:F66"/>
+    <mergeCell ref="A67:F67"/>
+    <mergeCell ref="A68:F68"/>
+    <mergeCell ref="A58:F58"/>
+    <mergeCell ref="A59:F59"/>
+    <mergeCell ref="A60:F60"/>
+    <mergeCell ref="A61:F61"/>
+    <mergeCell ref="A62:F62"/>
+    <mergeCell ref="A47:F47"/>
+    <mergeCell ref="A51:F51"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="A53:F53"/>
+    <mergeCell ref="A54:F54"/>
+    <mergeCell ref="A40:F40"/>
+    <mergeCell ref="A41:F41"/>
+    <mergeCell ref="A44:F44"/>
+    <mergeCell ref="A45:F45"/>
+    <mergeCell ref="A46:F46"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A34:F34"/>
+    <mergeCell ref="A35:F35"/>
+    <mergeCell ref="A36:F36"/>
+    <mergeCell ref="A39:F39"/>
     <mergeCell ref="A3:F3"/>
     <mergeCell ref="A16:F16"/>
     <mergeCell ref="A29:F29"/>
     <mergeCell ref="A31:F31"/>
     <mergeCell ref="A32:F32"/>
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="A34:F34"/>
-    <mergeCell ref="A35:F35"/>
-    <mergeCell ref="A36:F36"/>
-    <mergeCell ref="A39:F39"/>
-    <mergeCell ref="A40:F40"/>
-    <mergeCell ref="A41:F41"/>
-    <mergeCell ref="A44:F44"/>
-    <mergeCell ref="A45:F45"/>
-    <mergeCell ref="A46:F46"/>
-    <mergeCell ref="A47:F47"/>
-    <mergeCell ref="A50:F50"/>
-    <mergeCell ref="A51:F51"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="A53:F53"/>
-    <mergeCell ref="A63:F63"/>
-    <mergeCell ref="A64:F64"/>
-    <mergeCell ref="A65:F65"/>
-    <mergeCell ref="A66:F66"/>
-    <mergeCell ref="A56:F56"/>
-    <mergeCell ref="A57:F57"/>
-    <mergeCell ref="A58:F58"/>
-    <mergeCell ref="A59:F59"/>
-    <mergeCell ref="A60:F60"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added more planning to todo list
</commit_message>
<xml_diff>
--- a/Production Documents/To-Do.xlsx
+++ b/Production Documents/To-Do.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmgam\Desktop\Shiva\Production Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C1F7170-44FA-4AD4-BF52-D3AA36BFFCA9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{209A94E8-E51F-4E56-BB9F-737DC24BFBDA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{669DCC34-C837-4342-A908-0F87EB315612}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{669DCC34-C837-4342-A908-0F87EB315612}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="100">
   <si>
     <t>Sprites</t>
   </si>
@@ -231,9 +232,6 @@
     <t>When a unit lands on top of the space a popup appears telling them what they found</t>
   </si>
   <si>
-    <t>Items are sent to the inventory and food/research points are counted up top</t>
-  </si>
-  <si>
     <t>Inventory items can be placed on the board</t>
   </si>
   <si>
@@ -274,13 +272,73 @@
   </si>
   <si>
     <t>Spawn pods are generated at the start of invasion rounds</t>
+  </si>
+  <si>
+    <t>Resource Plan:</t>
+  </si>
+  <si>
+    <t>Food</t>
+  </si>
+  <si>
+    <t>Nothing</t>
+  </si>
+  <si>
+    <t>Found humans can be either placed on a tile adjacent to where they were found, or sent back to town</t>
+  </si>
+  <si>
+    <t>Weapons can be given to soldiers through the inventory</t>
+  </si>
+  <si>
+    <t>Soldiers have a button that removes their weapon and sends it back to the inventory</t>
+  </si>
+  <si>
+    <t>Food/research points are counted</t>
+  </si>
+  <si>
+    <t>Items are sent to the inventory</t>
+  </si>
+  <si>
+    <t>Soldier</t>
+  </si>
+  <si>
+    <t>Human</t>
+  </si>
+  <si>
+    <t>Human Weapon</t>
+  </si>
+  <si>
+    <t>Alien Weapon</t>
+  </si>
+  <si>
+    <t>Research</t>
+  </si>
+  <si>
+    <t>Pistol</t>
+  </si>
+  <si>
+    <t>Machine Gun</t>
+  </si>
+  <si>
+    <t>Laser</t>
+  </si>
+  <si>
+    <t>Cannon</t>
+  </si>
+  <si>
+    <t>Laser Turret</t>
+  </si>
+  <si>
+    <t>Cannon Turret</t>
+  </si>
+  <si>
+    <t>Tiles with spawn pods become landing sites</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -308,6 +366,14 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -381,7 +447,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
@@ -393,15 +459,18 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -724,10 +793,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4D254F2-4E19-40CF-BD85-766CDBA8C5EF}">
-  <dimension ref="A2:F71"/>
+  <dimension ref="A2:F76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="I52" sqref="I52"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A77" sqref="A77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -745,14 +814,14 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="18" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -776,7 +845,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>15</v>
@@ -802,7 +871,7 @@
         <v>16</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>22</v>
@@ -911,14 +980,14 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
@@ -960,7 +1029,7 @@
         <v>16</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>22</v>
@@ -1038,14 +1107,14 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="12" t="s">
+      <c r="A29" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="12"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
     </row>
     <row r="30" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
@@ -1053,64 +1122,64 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="13" t="s">
+      <c r="A31" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="B31" s="13"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="13" t="s">
+      <c r="A32" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="B32" s="13"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
+      <c r="B32" s="14"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="B33" s="13"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
+      <c r="A33" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B33" s="14"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="14"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="13" t="s">
+      <c r="A34" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="B34" s="13"/>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="13" t="s">
+      <c r="A35" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="B35" s="13"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="13" t="s">
+      <c r="A36" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="B36" s="13"/>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
     </row>
     <row r="38" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
@@ -1118,34 +1187,34 @@
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="14" t="s">
+      <c r="A39" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="B39" s="14"/>
-      <c r="C39" s="14"/>
-      <c r="D39" s="14"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="14"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="13"/>
+      <c r="F39" s="13"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="14" t="s">
+      <c r="A40" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="B40" s="14"/>
-      <c r="C40" s="14"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="14"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="13"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="14" t="s">
+      <c r="A41" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="B41" s="14"/>
-      <c r="C41" s="14"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="14"/>
+      <c r="B41" s="13"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="13"/>
     </row>
     <row r="42" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
@@ -1156,48 +1225,48 @@
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="13" t="s">
+      <c r="A44" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="B44" s="13"/>
-      <c r="C44" s="13"/>
-      <c r="D44" s="13"/>
-      <c r="E44" s="13"/>
-      <c r="F44" s="13"/>
+      <c r="B44" s="14"/>
+      <c r="C44" s="14"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="14"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="13" t="s">
+      <c r="A45" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="B45" s="13"/>
-      <c r="C45" s="13"/>
-      <c r="D45" s="13"/>
-      <c r="E45" s="13"/>
-      <c r="F45" s="13"/>
+      <c r="B45" s="14"/>
+      <c r="C45" s="14"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="14"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="13" t="s">
+      <c r="A46" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="B46" s="13"/>
-      <c r="C46" s="13"/>
-      <c r="D46" s="13"/>
-      <c r="E46" s="13"/>
-      <c r="F46" s="13"/>
+      <c r="B46" s="14"/>
+      <c r="C46" s="14"/>
+      <c r="D46" s="14"/>
+      <c r="E46" s="14"/>
+      <c r="F46" s="14"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="13" t="s">
+      <c r="A47" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="B47" s="13"/>
-      <c r="C47" s="13"/>
-      <c r="D47" s="13"/>
-      <c r="E47" s="13"/>
-      <c r="F47" s="13"/>
+      <c r="B47" s="14"/>
+      <c r="C47" s="14"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="14"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B48" s="10"/>
       <c r="C48" s="10"/>
@@ -1211,54 +1280,54 @@
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="13" t="s">
+      <c r="A51" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="B51" s="13"/>
-      <c r="C51" s="13"/>
-      <c r="D51" s="13"/>
-      <c r="E51" s="13"/>
-      <c r="F51" s="13"/>
+      <c r="B51" s="14"/>
+      <c r="C51" s="14"/>
+      <c r="D51" s="14"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="14"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="13" t="s">
+      <c r="A52" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="B52" s="13"/>
-      <c r="C52" s="13"/>
-      <c r="D52" s="13"/>
-      <c r="E52" s="13"/>
-      <c r="F52" s="13"/>
+      <c r="B52" s="14"/>
+      <c r="C52" s="14"/>
+      <c r="D52" s="14"/>
+      <c r="E52" s="14"/>
+      <c r="F52" s="14"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="13" t="s">
+      <c r="A53" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="B53" s="13"/>
-      <c r="C53" s="13"/>
-      <c r="D53" s="13"/>
-      <c r="E53" s="13"/>
-      <c r="F53" s="13"/>
+      <c r="B53" s="14"/>
+      <c r="C53" s="14"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="14"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="14" t="s">
+      <c r="A54" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="B54" s="14"/>
-      <c r="C54" s="14"/>
-      <c r="D54" s="14"/>
-      <c r="E54" s="14"/>
-      <c r="F54" s="14"/>
+      <c r="B54" s="13"/>
+      <c r="C54" s="13"/>
+      <c r="D54" s="13"/>
+      <c r="E54" s="13"/>
+      <c r="F54" s="13"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="B55" s="15"/>
-      <c r="C55" s="15"/>
-      <c r="D55" s="15"/>
-      <c r="E55" s="15"/>
-      <c r="F55" s="15"/>
+      <c r="A55" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="B55" s="12"/>
+      <c r="C55" s="12"/>
+      <c r="D55" s="12"/>
+      <c r="E55" s="12"/>
+      <c r="F55" s="12"/>
     </row>
     <row r="57" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
@@ -1266,147 +1335,567 @@
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="14" t="s">
+      <c r="A58" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="B58" s="14"/>
-      <c r="C58" s="14"/>
-      <c r="D58" s="14"/>
-      <c r="E58" s="14"/>
-      <c r="F58" s="14"/>
+      <c r="B58" s="13"/>
+      <c r="C58" s="13"/>
+      <c r="D58" s="13"/>
+      <c r="E58" s="13"/>
+      <c r="F58" s="13"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="14" t="s">
+      <c r="A59" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="B59" s="14"/>
-      <c r="C59" s="14"/>
-      <c r="D59" s="14"/>
-      <c r="E59" s="14"/>
-      <c r="F59" s="14"/>
+      <c r="B59" s="13"/>
+      <c r="C59" s="13"/>
+      <c r="D59" s="13"/>
+      <c r="E59" s="13"/>
+      <c r="F59" s="13"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="14" t="s">
+      <c r="A60" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="B60" s="13"/>
+      <c r="C60" s="13"/>
+      <c r="D60" s="13"/>
+      <c r="E60" s="13"/>
+      <c r="F60" s="13"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="B61" s="11"/>
+      <c r="C61" s="11"/>
+      <c r="D61" s="11"/>
+      <c r="E61" s="11"/>
+      <c r="F61" s="11"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="B60" s="14"/>
-      <c r="C60" s="14"/>
-      <c r="D60" s="14"/>
-      <c r="E60" s="14"/>
-      <c r="F60" s="14"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="14" t="s">
+      <c r="B62" s="13"/>
+      <c r="C62" s="13"/>
+      <c r="D62" s="13"/>
+      <c r="E62" s="13"/>
+      <c r="F62" s="13"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B63" s="11"/>
+      <c r="C63" s="11"/>
+      <c r="D63" s="11"/>
+      <c r="E63" s="11"/>
+      <c r="F63" s="11"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B64" s="11"/>
+      <c r="C64" s="11"/>
+      <c r="D64" s="11"/>
+      <c r="E64" s="11"/>
+      <c r="F64" s="11"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="B65" s="11"/>
+      <c r="C65" s="11"/>
+      <c r="D65" s="11"/>
+      <c r="E65" s="11"/>
+      <c r="F65" s="11"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B66" s="13"/>
+      <c r="C66" s="13"/>
+      <c r="D66" s="13"/>
+      <c r="E66" s="13"/>
+      <c r="F66" s="13"/>
+    </row>
+    <row r="68" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B61" s="14"/>
-      <c r="C61" s="14"/>
-      <c r="D61" s="14"/>
-      <c r="E61" s="14"/>
-      <c r="F61" s="14"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="14" t="s">
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="B62" s="14"/>
-      <c r="C62" s="14"/>
-      <c r="D62" s="14"/>
-      <c r="E62" s="14"/>
-      <c r="F62" s="14"/>
-    </row>
-    <row r="64" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="14" t="s">
+      <c r="B69" s="13"/>
+      <c r="C69" s="13"/>
+      <c r="D69" s="13"/>
+      <c r="E69" s="13"/>
+      <c r="F69" s="13"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="B65" s="14"/>
-      <c r="C65" s="14"/>
-      <c r="D65" s="14"/>
-      <c r="E65" s="14"/>
-      <c r="F65" s="14"/>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="14" t="s">
+      <c r="B70" s="13"/>
+      <c r="C70" s="13"/>
+      <c r="D70" s="13"/>
+      <c r="E70" s="13"/>
+      <c r="F70" s="13"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="B66" s="14"/>
-      <c r="C66" s="14"/>
-      <c r="D66" s="14"/>
-      <c r="E66" s="14"/>
-      <c r="F66" s="14"/>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="14" t="s">
+      <c r="B71" s="13"/>
+      <c r="C71" s="13"/>
+      <c r="D71" s="13"/>
+      <c r="E71" s="13"/>
+      <c r="F71" s="13"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="B67" s="14"/>
-      <c r="C67" s="14"/>
-      <c r="D67" s="14"/>
-      <c r="E67" s="14"/>
-      <c r="F67" s="14"/>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="B68" s="14"/>
-      <c r="C68" s="14"/>
-      <c r="D68" s="14"/>
-      <c r="E68" s="14"/>
-      <c r="F68" s="14"/>
-    </row>
-    <row r="70" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="1" t="s">
+      <c r="B72" s="13"/>
+      <c r="C72" s="13"/>
+      <c r="D72" s="13"/>
+      <c r="E72" s="13"/>
+      <c r="F72" s="13"/>
+    </row>
+    <row r="74" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="10" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="B71" s="10"/>
-      <c r="C71" s="10"/>
-      <c r="D71" s="10"/>
-      <c r="E71" s="10"/>
-      <c r="F71" s="10"/>
+      <c r="B75" s="10"/>
+      <c r="C75" s="10"/>
+      <c r="D75" s="10"/>
+      <c r="E75" s="10"/>
+      <c r="F75" s="10"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="B76" s="11"/>
+      <c r="C76" s="11"/>
+      <c r="D76" s="11"/>
+      <c r="E76" s="11"/>
+      <c r="F76" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="A65:F65"/>
-    <mergeCell ref="A66:F66"/>
-    <mergeCell ref="A67:F67"/>
-    <mergeCell ref="A68:F68"/>
-    <mergeCell ref="A58:F58"/>
-    <mergeCell ref="A59:F59"/>
-    <mergeCell ref="A60:F60"/>
-    <mergeCell ref="A61:F61"/>
-    <mergeCell ref="A62:F62"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A29:F29"/>
+    <mergeCell ref="A31:F31"/>
+    <mergeCell ref="A32:F32"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A34:F34"/>
+    <mergeCell ref="A35:F35"/>
+    <mergeCell ref="A36:F36"/>
+    <mergeCell ref="A39:F39"/>
+    <mergeCell ref="A40:F40"/>
+    <mergeCell ref="A41:F41"/>
+    <mergeCell ref="A44:F44"/>
+    <mergeCell ref="A45:F45"/>
+    <mergeCell ref="A46:F46"/>
     <mergeCell ref="A47:F47"/>
     <mergeCell ref="A51:F51"/>
     <mergeCell ref="A52:F52"/>
     <mergeCell ref="A53:F53"/>
     <mergeCell ref="A54:F54"/>
-    <mergeCell ref="A40:F40"/>
-    <mergeCell ref="A41:F41"/>
-    <mergeCell ref="A44:F44"/>
-    <mergeCell ref="A45:F45"/>
-    <mergeCell ref="A46:F46"/>
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="A34:F34"/>
-    <mergeCell ref="A35:F35"/>
-    <mergeCell ref="A36:F36"/>
-    <mergeCell ref="A39:F39"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A16:F16"/>
-    <mergeCell ref="A29:F29"/>
-    <mergeCell ref="A31:F31"/>
-    <mergeCell ref="A32:F32"/>
+    <mergeCell ref="A69:F69"/>
+    <mergeCell ref="A70:F70"/>
+    <mergeCell ref="A71:F71"/>
+    <mergeCell ref="A72:F72"/>
+    <mergeCell ref="A58:F58"/>
+    <mergeCell ref="A59:F59"/>
+    <mergeCell ref="A60:F60"/>
+    <mergeCell ref="A62:F62"/>
+    <mergeCell ref="A66:F66"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EC65D00-114F-446E-BBDB-199B2CA15EF1}">
+  <dimension ref="A1:N45"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" s="18">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4" s="18">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" s="18">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6" s="18">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" s="18">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B8" s="18">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B9" s="18">
+        <f>SUM(B3:B8)</f>
+        <v>1</v>
+      </c>
+      <c r="J9" t="s">
+        <v>89</v>
+      </c>
+      <c r="K9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J10" t="s">
+        <v>90</v>
+      </c>
+      <c r="K10" t="s">
+        <v>93</v>
+      </c>
+      <c r="L10" t="s">
+        <v>94</v>
+      </c>
+      <c r="M10" t="s">
+        <v>21</v>
+      </c>
+      <c r="N10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="J11" t="s">
+        <v>91</v>
+      </c>
+      <c r="K11" t="s">
+        <v>95</v>
+      </c>
+      <c r="L11" t="s">
+        <v>96</v>
+      </c>
+      <c r="M11" t="s">
+        <v>97</v>
+      </c>
+      <c r="N11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B12" s="18">
+        <v>0</v>
+      </c>
+      <c r="J12" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>89</v>
+      </c>
+      <c r="B13" s="18">
+        <v>0</v>
+      </c>
+      <c r="J13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>90</v>
+      </c>
+      <c r="B14" s="18">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>91</v>
+      </c>
+      <c r="B15" s="18">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>81</v>
+      </c>
+      <c r="B16" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>92</v>
+      </c>
+      <c r="B17" s="18">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="18">
+        <f>SUM(B12:B17)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>82</v>
+      </c>
+      <c r="B21" s="18">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>89</v>
+      </c>
+      <c r="B22" s="18">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>90</v>
+      </c>
+      <c r="B23" s="18">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>91</v>
+      </c>
+      <c r="B24" s="18">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>81</v>
+      </c>
+      <c r="B25" s="18">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>92</v>
+      </c>
+      <c r="B26" s="18">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B27" s="18">
+        <f>SUM(B21:B26)</f>
+        <v>1.0000000000000002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>82</v>
+      </c>
+      <c r="B30" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>89</v>
+      </c>
+      <c r="B31" s="18">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>90</v>
+      </c>
+      <c r="B32" s="18">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>91</v>
+      </c>
+      <c r="B33" s="18">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>81</v>
+      </c>
+      <c r="B34" s="18">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>92</v>
+      </c>
+      <c r="B35" s="18">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B36" s="18">
+        <f>SUM(B30:B35)</f>
+        <v>0.99999999999999989</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>82</v>
+      </c>
+      <c r="B39" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>89</v>
+      </c>
+      <c r="B40" s="18">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>90</v>
+      </c>
+      <c r="B41" s="18">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>91</v>
+      </c>
+      <c r="B42" s="18">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>81</v>
+      </c>
+      <c r="B43" s="18">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>92</v>
+      </c>
+      <c r="B44" s="18">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B45" s="18">
+        <f>SUM(B39:B44)</f>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Working on the resource system. Each explorable tile has a list containing the percentage chance that the player will discover X resource. When a human is placed on or moves to an unexplored tile, then the exploreTile() function is called and picks a resource to give to the player. It currently just updates the dialogText with a basic message until something else is selected. Will be adding more discovered* functions soon to add more functionality to exploration
</commit_message>
<xml_diff>
--- a/Production Documents/To-Do.xlsx
+++ b/Production Documents/To-Do.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmgam\Desktop\Shiva\Production Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{209A94E8-E51F-4E56-BB9F-737DC24BFBDA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2ECE7EB-8D8B-4D2B-98EC-727149331805}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{669DCC34-C837-4342-A908-0F87EB315612}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{669DCC34-C837-4342-A908-0F87EB315612}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="101">
   <si>
     <t>Sprites</t>
   </si>
@@ -283,9 +283,6 @@
     <t>Nothing</t>
   </si>
   <si>
-    <t>Found humans can be either placed on a tile adjacent to where they were found, or sent back to town</t>
-  </si>
-  <si>
     <t>Weapons can be given to soldiers through the inventory</t>
   </si>
   <si>
@@ -332,6 +329,12 @@
   </si>
   <si>
     <t>Tiles with spawn pods become landing sites</t>
+  </si>
+  <si>
+    <t>The player starts the game with a turret outside the base, and a soldier in the base</t>
+  </si>
+  <si>
+    <t>Found humans are placed on an adjacent tile to where they were found</t>
   </si>
 </sst>
 </file>
@@ -379,7 +382,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -395,12 +398,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -447,7 +444,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
@@ -460,17 +457,18 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -793,10 +791,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4D254F2-4E19-40CF-BD85-766CDBA8C5EF}">
-  <dimension ref="A2:F76"/>
+  <dimension ref="A2:F77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A77" sqref="A77"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="I63" sqref="I63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -814,14 +812,14 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="18" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -980,14 +978,14 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
@@ -1107,14 +1105,14 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="16" t="s">
+      <c r="A29" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="16"/>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17"/>
     </row>
     <row r="30" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
@@ -1122,64 +1120,64 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="14" t="s">
+      <c r="A31" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="B31" s="14"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="14" t="s">
+      <c r="A32" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="B32" s="14"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="14" t="s">
+      <c r="A33" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="B33" s="14"/>
-      <c r="C33" s="14"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="14" t="s">
+      <c r="A34" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B34" s="14"/>
-      <c r="C34" s="14"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="14"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="14" t="s">
+      <c r="A35" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="B35" s="14"/>
-      <c r="C35" s="14"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="14"/>
+      <c r="B35" s="18"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="14" t="s">
+      <c r="A36" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="B36" s="14"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="14"/>
+      <c r="B36" s="18"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
     </row>
     <row r="38" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
@@ -1187,34 +1185,34 @@
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="13" t="s">
+      <c r="A39" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="B39" s="13"/>
-      <c r="C39" s="13"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="13"/>
-      <c r="F39" s="13"/>
+      <c r="B39" s="19"/>
+      <c r="C39" s="19"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="19"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="13" t="s">
+      <c r="A40" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="B40" s="13"/>
-      <c r="C40" s="13"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="13"/>
-      <c r="F40" s="13"/>
+      <c r="B40" s="19"/>
+      <c r="C40" s="19"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="19"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="13" t="s">
+      <c r="A41" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="B41" s="13"/>
-      <c r="C41" s="13"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="13"/>
-      <c r="F41" s="13"/>
+      <c r="B41" s="19"/>
+      <c r="C41" s="19"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="19"/>
+      <c r="F41" s="19"/>
     </row>
     <row r="42" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
@@ -1225,44 +1223,44 @@
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="14" t="s">
+      <c r="A44" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="B44" s="14"/>
-      <c r="C44" s="14"/>
-      <c r="D44" s="14"/>
-      <c r="E44" s="14"/>
-      <c r="F44" s="14"/>
+      <c r="B44" s="18"/>
+      <c r="C44" s="18"/>
+      <c r="D44" s="18"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="18"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="14" t="s">
+      <c r="A45" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="B45" s="14"/>
-      <c r="C45" s="14"/>
-      <c r="D45" s="14"/>
-      <c r="E45" s="14"/>
-      <c r="F45" s="14"/>
+      <c r="B45" s="18"/>
+      <c r="C45" s="18"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="18"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="14" t="s">
+      <c r="A46" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="B46" s="14"/>
-      <c r="C46" s="14"/>
-      <c r="D46" s="14"/>
-      <c r="E46" s="14"/>
-      <c r="F46" s="14"/>
+      <c r="B46" s="18"/>
+      <c r="C46" s="18"/>
+      <c r="D46" s="18"/>
+      <c r="E46" s="18"/>
+      <c r="F46" s="18"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="14" t="s">
+      <c r="A47" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="B47" s="14"/>
-      <c r="C47" s="14"/>
-      <c r="D47" s="14"/>
-      <c r="E47" s="14"/>
-      <c r="F47" s="14"/>
+      <c r="B47" s="18"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="18"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="18"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
@@ -1280,54 +1278,54 @@
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="14" t="s">
+      <c r="A51" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="B51" s="14"/>
-      <c r="C51" s="14"/>
-      <c r="D51" s="14"/>
-      <c r="E51" s="14"/>
-      <c r="F51" s="14"/>
+      <c r="B51" s="18"/>
+      <c r="C51" s="18"/>
+      <c r="D51" s="18"/>
+      <c r="E51" s="18"/>
+      <c r="F51" s="18"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="14" t="s">
+      <c r="A52" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="B52" s="14"/>
-      <c r="C52" s="14"/>
-      <c r="D52" s="14"/>
-      <c r="E52" s="14"/>
-      <c r="F52" s="14"/>
+      <c r="B52" s="18"/>
+      <c r="C52" s="18"/>
+      <c r="D52" s="18"/>
+      <c r="E52" s="18"/>
+      <c r="F52" s="18"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="14" t="s">
+      <c r="A53" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B53" s="14"/>
-      <c r="C53" s="14"/>
-      <c r="D53" s="14"/>
-      <c r="E53" s="14"/>
-      <c r="F53" s="14"/>
+      <c r="B53" s="18"/>
+      <c r="C53" s="18"/>
+      <c r="D53" s="18"/>
+      <c r="E53" s="18"/>
+      <c r="F53" s="18"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="13" t="s">
+      <c r="A54" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="B54" s="13"/>
-      <c r="C54" s="13"/>
-      <c r="D54" s="13"/>
-      <c r="E54" s="13"/>
-      <c r="F54" s="13"/>
+      <c r="B54" s="19"/>
+      <c r="C54" s="19"/>
+      <c r="D54" s="19"/>
+      <c r="E54" s="19"/>
+      <c r="F54" s="19"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="12" t="s">
+      <c r="A55" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="B55" s="12"/>
-      <c r="C55" s="12"/>
-      <c r="D55" s="12"/>
-      <c r="E55" s="12"/>
-      <c r="F55" s="12"/>
+      <c r="B55" s="13"/>
+      <c r="C55" s="13"/>
+      <c r="D55" s="13"/>
+      <c r="E55" s="13"/>
+      <c r="F55" s="13"/>
     </row>
     <row r="57" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
@@ -1335,58 +1333,58 @@
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="13" t="s">
+      <c r="A58" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="B58" s="13"/>
-      <c r="C58" s="13"/>
-      <c r="D58" s="13"/>
-      <c r="E58" s="13"/>
-      <c r="F58" s="13"/>
+      <c r="B58" s="18"/>
+      <c r="C58" s="18"/>
+      <c r="D58" s="18"/>
+      <c r="E58" s="18"/>
+      <c r="F58" s="18"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="13" t="s">
+      <c r="A59" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="B59" s="13"/>
-      <c r="C59" s="13"/>
-      <c r="D59" s="13"/>
-      <c r="E59" s="13"/>
-      <c r="F59" s="13"/>
+      <c r="B59" s="19"/>
+      <c r="C59" s="19"/>
+      <c r="D59" s="19"/>
+      <c r="E59" s="19"/>
+      <c r="F59" s="19"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="B60" s="13"/>
-      <c r="C60" s="13"/>
-      <c r="D60" s="13"/>
-      <c r="E60" s="13"/>
-      <c r="F60" s="13"/>
+      <c r="A60" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="B60" s="19"/>
+      <c r="C60" s="19"/>
+      <c r="D60" s="19"/>
+      <c r="E60" s="19"/>
+      <c r="F60" s="19"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="B61" s="11"/>
-      <c r="C61" s="11"/>
-      <c r="D61" s="11"/>
-      <c r="E61" s="11"/>
-      <c r="F61" s="11"/>
+      <c r="A61" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="B61" s="13"/>
+      <c r="C61" s="13"/>
+      <c r="D61" s="13"/>
+      <c r="E61" s="13"/>
+      <c r="F61" s="13"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="13" t="s">
+      <c r="A62" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="B62" s="13"/>
-      <c r="C62" s="13"/>
-      <c r="D62" s="13"/>
-      <c r="E62" s="13"/>
-      <c r="F62" s="13"/>
+      <c r="B62" s="19"/>
+      <c r="C62" s="19"/>
+      <c r="D62" s="19"/>
+      <c r="E62" s="19"/>
+      <c r="F62" s="19"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="11" t="s">
-        <v>83</v>
+        <v>100</v>
       </c>
       <c r="B63" s="11"/>
       <c r="C63" s="11"/>
@@ -1396,7 +1394,7 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B64" s="11"/>
       <c r="C64" s="11"/>
@@ -1406,7 +1404,7 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B65" s="11"/>
       <c r="C65" s="11"/>
@@ -1415,14 +1413,14 @@
       <c r="F65" s="11"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="13" t="s">
+      <c r="A66" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="B66" s="13"/>
-      <c r="C66" s="13"/>
-      <c r="D66" s="13"/>
-      <c r="E66" s="13"/>
-      <c r="F66" s="13"/>
+      <c r="B66" s="19"/>
+      <c r="C66" s="19"/>
+      <c r="D66" s="19"/>
+      <c r="E66" s="19"/>
+      <c r="F66" s="19"/>
     </row>
     <row r="68" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
@@ -1430,44 +1428,44 @@
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="13" t="s">
+      <c r="A69" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="B69" s="13"/>
-      <c r="C69" s="13"/>
-      <c r="D69" s="13"/>
-      <c r="E69" s="13"/>
-      <c r="F69" s="13"/>
+      <c r="B69" s="19"/>
+      <c r="C69" s="19"/>
+      <c r="D69" s="19"/>
+      <c r="E69" s="19"/>
+      <c r="F69" s="19"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="13" t="s">
+      <c r="A70" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="B70" s="13"/>
-      <c r="C70" s="13"/>
-      <c r="D70" s="13"/>
-      <c r="E70" s="13"/>
-      <c r="F70" s="13"/>
+      <c r="B70" s="19"/>
+      <c r="C70" s="19"/>
+      <c r="D70" s="19"/>
+      <c r="E70" s="19"/>
+      <c r="F70" s="19"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="13" t="s">
+      <c r="A71" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="B71" s="13"/>
-      <c r="C71" s="13"/>
-      <c r="D71" s="13"/>
-      <c r="E71" s="13"/>
-      <c r="F71" s="13"/>
+      <c r="B71" s="19"/>
+      <c r="C71" s="19"/>
+      <c r="D71" s="19"/>
+      <c r="E71" s="19"/>
+      <c r="F71" s="19"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="13" t="s">
+      <c r="A72" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="B72" s="13"/>
-      <c r="C72" s="13"/>
-      <c r="D72" s="13"/>
-      <c r="E72" s="13"/>
-      <c r="F72" s="13"/>
+      <c r="B72" s="19"/>
+      <c r="C72" s="19"/>
+      <c r="D72" s="19"/>
+      <c r="E72" s="19"/>
+      <c r="F72" s="19"/>
     </row>
     <row r="74" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
@@ -1486,7 +1484,7 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B76" s="11"/>
       <c r="C76" s="11"/>
@@ -1494,28 +1492,18 @@
       <c r="E76" s="11"/>
       <c r="F76" s="11"/>
     </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="B77" s="12"/>
+      <c r="C77" s="12"/>
+      <c r="D77" s="12"/>
+      <c r="E77" s="12"/>
+      <c r="F77" s="12"/>
+    </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A16:F16"/>
-    <mergeCell ref="A29:F29"/>
-    <mergeCell ref="A31:F31"/>
-    <mergeCell ref="A32:F32"/>
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="A34:F34"/>
-    <mergeCell ref="A35:F35"/>
-    <mergeCell ref="A36:F36"/>
-    <mergeCell ref="A39:F39"/>
-    <mergeCell ref="A40:F40"/>
-    <mergeCell ref="A41:F41"/>
-    <mergeCell ref="A44:F44"/>
-    <mergeCell ref="A45:F45"/>
-    <mergeCell ref="A46:F46"/>
-    <mergeCell ref="A47:F47"/>
-    <mergeCell ref="A51:F51"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="A53:F53"/>
-    <mergeCell ref="A54:F54"/>
     <mergeCell ref="A69:F69"/>
     <mergeCell ref="A70:F70"/>
     <mergeCell ref="A71:F71"/>
@@ -1525,6 +1513,26 @@
     <mergeCell ref="A60:F60"/>
     <mergeCell ref="A62:F62"/>
     <mergeCell ref="A66:F66"/>
+    <mergeCell ref="A47:F47"/>
+    <mergeCell ref="A51:F51"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="A53:F53"/>
+    <mergeCell ref="A54:F54"/>
+    <mergeCell ref="A40:F40"/>
+    <mergeCell ref="A41:F41"/>
+    <mergeCell ref="A44:F44"/>
+    <mergeCell ref="A45:F45"/>
+    <mergeCell ref="A46:F46"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A34:F34"/>
+    <mergeCell ref="A35:F35"/>
+    <mergeCell ref="A36:F36"/>
+    <mergeCell ref="A39:F39"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A29:F29"/>
+    <mergeCell ref="A31:F31"/>
+    <mergeCell ref="A32:F32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1551,12 +1559,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="14" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="14" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1564,31 +1572,31 @@
       <c r="A3" t="s">
         <v>82</v>
       </c>
-      <c r="B3" s="18">
+      <c r="B3" s="15">
         <v>0.75</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>89</v>
-      </c>
-      <c r="B4" s="18">
+        <v>88</v>
+      </c>
+      <c r="B4" s="15">
         <v>0.06</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>90</v>
-      </c>
-      <c r="B5" s="18">
+        <v>89</v>
+      </c>
+      <c r="B5" s="15">
         <v>0.08</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>91</v>
-      </c>
-      <c r="B6" s="18">
+        <v>90</v>
+      </c>
+      <c r="B6" s="15">
         <v>0.02</v>
       </c>
     </row>
@@ -1596,39 +1604,39 @@
       <c r="A7" t="s">
         <v>81</v>
       </c>
-      <c r="B7" s="18">
+      <c r="B7" s="15">
         <v>0.05</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>92</v>
-      </c>
-      <c r="B8" s="18">
+        <v>91</v>
+      </c>
+      <c r="B8" s="15">
         <v>0.04</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="18">
+      <c r="B9" s="15">
         <f>SUM(B3:B8)</f>
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="J10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K10" t="s">
+        <v>92</v>
+      </c>
+      <c r="L10" t="s">
         <v>93</v>
-      </c>
-      <c r="L10" t="s">
-        <v>94</v>
       </c>
       <c r="M10" t="s">
         <v>21</v>
@@ -1638,30 +1646,30 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="14" t="s">
         <v>13</v>
       </c>
       <c r="J11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K11" t="s">
+        <v>94</v>
+      </c>
+      <c r="L11" t="s">
         <v>95</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" t="s">
         <v>96</v>
       </c>
-      <c r="M11" t="s">
+      <c r="N11" t="s">
         <v>97</v>
-      </c>
-      <c r="N11" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>82</v>
       </c>
-      <c r="B12" s="18">
+      <c r="B12" s="15">
         <v>0</v>
       </c>
       <c r="J12" t="s">
@@ -1670,28 +1678,28 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>89</v>
-      </c>
-      <c r="B13" s="18">
+        <v>88</v>
+      </c>
+      <c r="B13" s="15">
         <v>0</v>
       </c>
       <c r="J13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>90</v>
-      </c>
-      <c r="B14" s="18">
+        <v>89</v>
+      </c>
+      <c r="B14" s="15">
         <v>0.05</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>91</v>
-      </c>
-      <c r="B15" s="18">
+        <v>90</v>
+      </c>
+      <c r="B15" s="15">
         <v>0.55000000000000004</v>
       </c>
     </row>
@@ -1699,26 +1707,26 @@
       <c r="A16" t="s">
         <v>81</v>
       </c>
-      <c r="B16" s="18">
+      <c r="B16" s="15">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>92</v>
-      </c>
-      <c r="B17" s="18">
+        <v>91</v>
+      </c>
+      <c r="B17" s="15">
         <v>0.4</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="18">
+      <c r="B18" s="15">
         <f>SUM(B12:B17)</f>
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="17" t="s">
+      <c r="A20" s="14" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1726,31 +1734,31 @@
       <c r="A21" t="s">
         <v>82</v>
       </c>
-      <c r="B21" s="18">
+      <c r="B21" s="15">
         <v>0.3</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>89</v>
-      </c>
-      <c r="B22" s="18">
+        <v>88</v>
+      </c>
+      <c r="B22" s="15">
         <v>0.2</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>90</v>
-      </c>
-      <c r="B23" s="18">
+        <v>89</v>
+      </c>
+      <c r="B23" s="15">
         <v>0.15</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>91</v>
-      </c>
-      <c r="B24" s="18">
+        <v>90</v>
+      </c>
+      <c r="B24" s="15">
         <v>0.05</v>
       </c>
     </row>
@@ -1758,26 +1766,26 @@
       <c r="A25" t="s">
         <v>81</v>
       </c>
-      <c r="B25" s="18">
+      <c r="B25" s="15">
         <v>0.2</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>92</v>
-      </c>
-      <c r="B26" s="18">
+        <v>91</v>
+      </c>
+      <c r="B26" s="15">
         <v>0.1</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B27" s="18">
+      <c r="B27" s="15">
         <f>SUM(B21:B26)</f>
         <v>1.0000000000000002</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="17" t="s">
+      <c r="A29" s="14" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1785,31 +1793,31 @@
       <c r="A30" t="s">
         <v>82</v>
       </c>
-      <c r="B30" s="18">
+      <c r="B30" s="15">
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>89</v>
-      </c>
-      <c r="B31" s="18">
+        <v>88</v>
+      </c>
+      <c r="B31" s="15">
         <v>0.3</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>90</v>
-      </c>
-      <c r="B32" s="18">
+        <v>89</v>
+      </c>
+      <c r="B32" s="15">
         <v>0.15</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>91</v>
-      </c>
-      <c r="B33" s="18">
+        <v>90</v>
+      </c>
+      <c r="B33" s="15">
         <v>0.1</v>
       </c>
     </row>
@@ -1817,26 +1825,26 @@
       <c r="A34" t="s">
         <v>81</v>
       </c>
-      <c r="B34" s="18">
+      <c r="B34" s="15">
         <v>0.3</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>92</v>
-      </c>
-      <c r="B35" s="18">
+        <v>91</v>
+      </c>
+      <c r="B35" s="15">
         <v>0.15</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B36" s="18">
+      <c r="B36" s="15">
         <f>SUM(B30:B35)</f>
         <v>0.99999999999999989</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="17" t="s">
+      <c r="A38" s="14" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1844,31 +1852,31 @@
       <c r="A39" t="s">
         <v>82</v>
       </c>
-      <c r="B39" s="18">
+      <c r="B39" s="15">
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>89</v>
-      </c>
-      <c r="B40" s="18">
+        <v>88</v>
+      </c>
+      <c r="B40" s="15">
         <v>0.2</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>90</v>
-      </c>
-      <c r="B41" s="18">
+        <v>89</v>
+      </c>
+      <c r="B41" s="15">
         <v>0.25</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>91</v>
-      </c>
-      <c r="B42" s="18">
+        <v>90</v>
+      </c>
+      <c r="B42" s="15">
         <v>0.25</v>
       </c>
     </row>
@@ -1876,20 +1884,20 @@
       <c r="A43" t="s">
         <v>81</v>
       </c>
-      <c r="B43" s="18">
+      <c r="B43" s="15">
         <v>0.05</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>92</v>
-      </c>
-      <c r="B44" s="18">
+        <v>91</v>
+      </c>
+      <c r="B44" s="15">
         <v>0.25</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B45" s="18">
+      <c r="B45" s="15">
         <f>SUM(B39:B44)</f>
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Added logic for spawn pods being created at the start of invasion rounds. The maximum pods on the map, minimum pods able to be spawned, and maximum pods able to be spawned are determined through exponential functions. These new scripts can be found in the Game Engine -> Game Flow Folder
</commit_message>
<xml_diff>
--- a/Production Documents/To-Do.xlsx
+++ b/Production Documents/To-Do.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmgam\Desktop\Shiva\Production Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2ECE7EB-8D8B-4D2B-98EC-727149331805}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50FB828B-5144-4480-81ED-F11D44826851}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{669DCC34-C837-4342-A908-0F87EB315612}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="103">
   <si>
     <t>Sprites</t>
   </si>
@@ -335,6 +335,12 @@
   </si>
   <si>
     <t>Found humans are placed on an adjacent tile to where they were found</t>
+  </si>
+  <si>
+    <t>Humans have a 'Feed' button to be given food</t>
+  </si>
+  <si>
+    <t>Only certain tiles are visable</t>
   </si>
 </sst>
 </file>
@@ -444,7 +450,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
@@ -461,14 +467,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -791,10 +799,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4D254F2-4E19-40CF-BD85-766CDBA8C5EF}">
-  <dimension ref="A2:F77"/>
+  <dimension ref="A2:F79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="I63" sqref="I63"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="J69" sqref="J69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -812,14 +820,14 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="18" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -978,14 +986,14 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
@@ -1105,14 +1113,14 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="17" t="s">
+      <c r="A29" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="17"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="17"/>
+      <c r="B29" s="21"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
     </row>
     <row r="30" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
@@ -1120,64 +1128,64 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="18" t="s">
+      <c r="A31" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B31" s="18"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="18" t="s">
+      <c r="A32" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="B32" s="18"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
+      <c r="B32" s="19"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="19"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="18" t="s">
+      <c r="A33" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="B33" s="18"/>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
+      <c r="B33" s="19"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="19"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="18" t="s">
+      <c r="A34" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="B34" s="18"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
+      <c r="B34" s="19"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="19"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="18" t="s">
+      <c r="A35" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="B35" s="18"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
+      <c r="B35" s="19"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="19"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="18" t="s">
+      <c r="A36" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="B36" s="18"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
+      <c r="B36" s="19"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="19"/>
+      <c r="F36" s="19"/>
     </row>
     <row r="38" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
@@ -1185,34 +1193,34 @@
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="19" t="s">
+      <c r="A39" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="B39" s="19"/>
-      <c r="C39" s="19"/>
-      <c r="D39" s="19"/>
-      <c r="E39" s="19"/>
-      <c r="F39" s="19"/>
+      <c r="B39" s="18"/>
+      <c r="C39" s="18"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="18"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="19" t="s">
+      <c r="A40" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="B40" s="19"/>
-      <c r="C40" s="19"/>
-      <c r="D40" s="19"/>
-      <c r="E40" s="19"/>
-      <c r="F40" s="19"/>
+      <c r="B40" s="18"/>
+      <c r="C40" s="18"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="18"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="19" t="s">
+      <c r="A41" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="B41" s="19"/>
-      <c r="C41" s="19"/>
-      <c r="D41" s="19"/>
-      <c r="E41" s="19"/>
-      <c r="F41" s="19"/>
+      <c r="B41" s="18"/>
+      <c r="C41" s="18"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="18"/>
     </row>
     <row r="42" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
@@ -1223,44 +1231,44 @@
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="18" t="s">
+      <c r="A44" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="B44" s="18"/>
-      <c r="C44" s="18"/>
-      <c r="D44" s="18"/>
-      <c r="E44" s="18"/>
-      <c r="F44" s="18"/>
+      <c r="B44" s="19"/>
+      <c r="C44" s="19"/>
+      <c r="D44" s="19"/>
+      <c r="E44" s="19"/>
+      <c r="F44" s="19"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="18" t="s">
+      <c r="A45" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="B45" s="18"/>
-      <c r="C45" s="18"/>
-      <c r="D45" s="18"/>
-      <c r="E45" s="18"/>
-      <c r="F45" s="18"/>
+      <c r="B45" s="19"/>
+      <c r="C45" s="19"/>
+      <c r="D45" s="19"/>
+      <c r="E45" s="19"/>
+      <c r="F45" s="19"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="18" t="s">
+      <c r="A46" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="B46" s="18"/>
-      <c r="C46" s="18"/>
-      <c r="D46" s="18"/>
-      <c r="E46" s="18"/>
-      <c r="F46" s="18"/>
+      <c r="B46" s="19"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="19"/>
+      <c r="E46" s="19"/>
+      <c r="F46" s="19"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="18" t="s">
+      <c r="A47" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="B47" s="18"/>
-      <c r="C47" s="18"/>
-      <c r="D47" s="18"/>
-      <c r="E47" s="18"/>
-      <c r="F47" s="18"/>
+      <c r="B47" s="19"/>
+      <c r="C47" s="19"/>
+      <c r="D47" s="19"/>
+      <c r="E47" s="19"/>
+      <c r="F47" s="19"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
@@ -1278,44 +1286,44 @@
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="18" t="s">
+      <c r="A51" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="B51" s="18"/>
-      <c r="C51" s="18"/>
-      <c r="D51" s="18"/>
-      <c r="E51" s="18"/>
-      <c r="F51" s="18"/>
+      <c r="B51" s="19"/>
+      <c r="C51" s="19"/>
+      <c r="D51" s="19"/>
+      <c r="E51" s="19"/>
+      <c r="F51" s="19"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="18" t="s">
+      <c r="A52" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="B52" s="18"/>
-      <c r="C52" s="18"/>
-      <c r="D52" s="18"/>
-      <c r="E52" s="18"/>
-      <c r="F52" s="18"/>
+      <c r="B52" s="19"/>
+      <c r="C52" s="19"/>
+      <c r="D52" s="19"/>
+      <c r="E52" s="19"/>
+      <c r="F52" s="19"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="18" t="s">
+      <c r="A53" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="B53" s="18"/>
-      <c r="C53" s="18"/>
-      <c r="D53" s="18"/>
-      <c r="E53" s="18"/>
-      <c r="F53" s="18"/>
+      <c r="B53" s="19"/>
+      <c r="C53" s="19"/>
+      <c r="D53" s="19"/>
+      <c r="E53" s="19"/>
+      <c r="F53" s="19"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="19" t="s">
+      <c r="A54" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="B54" s="19"/>
-      <c r="C54" s="19"/>
-      <c r="D54" s="19"/>
-      <c r="E54" s="19"/>
-      <c r="F54" s="19"/>
+      <c r="B54" s="18"/>
+      <c r="C54" s="18"/>
+      <c r="D54" s="18"/>
+      <c r="E54" s="18"/>
+      <c r="F54" s="18"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="13" t="s">
@@ -1333,14 +1341,14 @@
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="18" t="s">
+      <c r="A58" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="B58" s="18"/>
-      <c r="C58" s="18"/>
-      <c r="D58" s="18"/>
-      <c r="E58" s="18"/>
-      <c r="F58" s="18"/>
+      <c r="B58" s="19"/>
+      <c r="C58" s="19"/>
+      <c r="D58" s="19"/>
+      <c r="E58" s="19"/>
+      <c r="F58" s="19"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="19" t="s">
@@ -1353,14 +1361,14 @@
       <c r="F59" s="19"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="19" t="s">
+      <c r="A60" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="B60" s="19"/>
-      <c r="C60" s="19"/>
-      <c r="D60" s="19"/>
-      <c r="E60" s="19"/>
-      <c r="F60" s="19"/>
+      <c r="B60" s="18"/>
+      <c r="C60" s="18"/>
+      <c r="D60" s="18"/>
+      <c r="E60" s="18"/>
+      <c r="F60" s="18"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="13" t="s">
@@ -1373,14 +1381,14 @@
       <c r="F61" s="13"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="19" t="s">
+      <c r="A62" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="B62" s="19"/>
-      <c r="C62" s="19"/>
-      <c r="D62" s="19"/>
-      <c r="E62" s="19"/>
-      <c r="F62" s="19"/>
+      <c r="B62" s="18"/>
+      <c r="C62" s="18"/>
+      <c r="D62" s="18"/>
+      <c r="E62" s="18"/>
+      <c r="F62" s="18"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="11" t="s">
@@ -1413,126 +1421,146 @@
       <c r="F65" s="11"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="19" t="s">
+      <c r="A66" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="B66" s="19"/>
-      <c r="C66" s="19"/>
-      <c r="D66" s="19"/>
-      <c r="E66" s="19"/>
-      <c r="F66" s="19"/>
-    </row>
-    <row r="68" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="1" t="s">
+      <c r="B66" s="18"/>
+      <c r="C66" s="18"/>
+      <c r="D66" s="18"/>
+      <c r="E66" s="18"/>
+      <c r="F66" s="18"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="B67" s="17"/>
+      <c r="C67" s="17"/>
+      <c r="D67" s="17"/>
+      <c r="E67" s="17"/>
+      <c r="F67" s="17"/>
+    </row>
+    <row r="69" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="19" t="s">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="B69" s="19"/>
-      <c r="C69" s="19"/>
-      <c r="D69" s="19"/>
-      <c r="E69" s="19"/>
-      <c r="F69" s="19"/>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="19" t="s">
+      <c r="B70" s="18"/>
+      <c r="C70" s="18"/>
+      <c r="D70" s="18"/>
+      <c r="E70" s="18"/>
+      <c r="F70" s="18"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="B70" s="19"/>
-      <c r="C70" s="19"/>
-      <c r="D70" s="19"/>
-      <c r="E70" s="19"/>
-      <c r="F70" s="19"/>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="19" t="s">
+      <c r="B71" s="18"/>
+      <c r="C71" s="18"/>
+      <c r="D71" s="18"/>
+      <c r="E71" s="18"/>
+      <c r="F71" s="18"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="B71" s="19"/>
-      <c r="C71" s="19"/>
-      <c r="D71" s="19"/>
-      <c r="E71" s="19"/>
-      <c r="F71" s="19"/>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="19" t="s">
+      <c r="B72" s="18"/>
+      <c r="C72" s="18"/>
+      <c r="D72" s="18"/>
+      <c r="E72" s="18"/>
+      <c r="F72" s="18"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="B72" s="19"/>
-      <c r="C72" s="19"/>
-      <c r="D72" s="19"/>
-      <c r="E72" s="19"/>
-      <c r="F72" s="19"/>
-    </row>
-    <row r="74" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="1" t="s">
+      <c r="B73" s="18"/>
+      <c r="C73" s="18"/>
+      <c r="D73" s="18"/>
+      <c r="E73" s="18"/>
+      <c r="F73" s="18"/>
+    </row>
+    <row r="75" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="10" t="s">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="B75" s="10"/>
-      <c r="C75" s="10"/>
-      <c r="D75" s="10"/>
-      <c r="E75" s="10"/>
-      <c r="F75" s="10"/>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="11" t="s">
+      <c r="B76" s="16"/>
+      <c r="C76" s="16"/>
+      <c r="D76" s="16"/>
+      <c r="E76" s="16"/>
+      <c r="F76" s="16"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B76" s="11"/>
-      <c r="C76" s="11"/>
-      <c r="D76" s="11"/>
-      <c r="E76" s="11"/>
-      <c r="F76" s="11"/>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="12" t="s">
+      <c r="B77" s="11"/>
+      <c r="C77" s="11"/>
+      <c r="D77" s="11"/>
+      <c r="E77" s="11"/>
+      <c r="F77" s="11"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="B77" s="12"/>
-      <c r="C77" s="12"/>
-      <c r="D77" s="12"/>
-      <c r="E77" s="12"/>
-      <c r="F77" s="12"/>
+      <c r="B78" s="12"/>
+      <c r="C78" s="12"/>
+      <c r="D78" s="12"/>
+      <c r="E78" s="12"/>
+      <c r="F78" s="12"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="B79" s="17"/>
+      <c r="C79" s="17"/>
+      <c r="D79" s="17"/>
+      <c r="E79" s="17"/>
+      <c r="F79" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="A69:F69"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A29:F29"/>
+    <mergeCell ref="A31:F31"/>
+    <mergeCell ref="A32:F32"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A34:F34"/>
+    <mergeCell ref="A35:F35"/>
+    <mergeCell ref="A36:F36"/>
+    <mergeCell ref="A39:F39"/>
+    <mergeCell ref="A40:F40"/>
+    <mergeCell ref="A41:F41"/>
+    <mergeCell ref="A44:F44"/>
+    <mergeCell ref="A45:F45"/>
+    <mergeCell ref="A46:F46"/>
+    <mergeCell ref="A47:F47"/>
+    <mergeCell ref="A51:F51"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="A53:F53"/>
+    <mergeCell ref="A54:F54"/>
     <mergeCell ref="A70:F70"/>
     <mergeCell ref="A71:F71"/>
     <mergeCell ref="A72:F72"/>
+    <mergeCell ref="A73:F73"/>
     <mergeCell ref="A58:F58"/>
     <mergeCell ref="A59:F59"/>
     <mergeCell ref="A60:F60"/>
     <mergeCell ref="A62:F62"/>
     <mergeCell ref="A66:F66"/>
-    <mergeCell ref="A47:F47"/>
-    <mergeCell ref="A51:F51"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="A53:F53"/>
-    <mergeCell ref="A54:F54"/>
-    <mergeCell ref="A40:F40"/>
-    <mergeCell ref="A41:F41"/>
-    <mergeCell ref="A44:F44"/>
-    <mergeCell ref="A45:F45"/>
-    <mergeCell ref="A46:F46"/>
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="A34:F34"/>
-    <mergeCell ref="A35:F35"/>
-    <mergeCell ref="A36:F36"/>
-    <mergeCell ref="A39:F39"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A16:F16"/>
-    <mergeCell ref="A29:F29"/>
-    <mergeCell ref="A31:F31"/>
-    <mergeCell ref="A32:F32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added more functionality to resource discovery. A random amount of food and research points is given to the player upon discovery. When a human is found, the game tries to place it on the last tile the moving human was on. If there is no previous tile or that tile is already occupied, it finds a surrounding tile that is not the tile the unit is moving to.
</commit_message>
<xml_diff>
--- a/Production Documents/To-Do.xlsx
+++ b/Production Documents/To-Do.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmgam\Desktop\Shiva\Production Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50FB828B-5144-4480-81ED-F11D44826851}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78E595D5-02C4-42EB-B959-7187B73509AC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{669DCC34-C837-4342-A908-0F87EB315612}"/>
   </bookViews>
@@ -450,7 +450,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
@@ -469,7 +469,6 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -477,6 +476,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -801,8 +802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4D254F2-4E19-40CF-BD85-766CDBA8C5EF}">
   <dimension ref="A2:F79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="J69" sqref="J69"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="I65" sqref="I65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -820,14 +821,14 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="18" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -986,14 +987,14 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="20"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
@@ -1113,14 +1114,14 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="21" t="s">
+      <c r="A29" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="21"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
     </row>
     <row r="30" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
@@ -1128,64 +1129,64 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="19" t="s">
+      <c r="A31" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="B31" s="19"/>
-      <c r="C31" s="19"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="19"/>
+      <c r="B31" s="21"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="19" t="s">
+      <c r="A32" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="B32" s="19"/>
-      <c r="C32" s="19"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="19"/>
+      <c r="B32" s="21"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="19" t="s">
+      <c r="A33" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="B33" s="19"/>
-      <c r="C33" s="19"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="19"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="19" t="s">
+      <c r="A34" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="B34" s="19"/>
-      <c r="C34" s="19"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="19"/>
+      <c r="B34" s="21"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="19" t="s">
+      <c r="A35" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="B35" s="19"/>
-      <c r="C35" s="19"/>
-      <c r="D35" s="19"/>
-      <c r="E35" s="19"/>
-      <c r="F35" s="19"/>
+      <c r="B35" s="21"/>
+      <c r="C35" s="21"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="21"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="19" t="s">
+      <c r="A36" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="B36" s="19"/>
-      <c r="C36" s="19"/>
-      <c r="D36" s="19"/>
-      <c r="E36" s="19"/>
-      <c r="F36" s="19"/>
+      <c r="B36" s="21"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
     </row>
     <row r="38" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
@@ -1193,34 +1194,34 @@
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="18" t="s">
+      <c r="A39" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="B39" s="18"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="18"/>
+      <c r="B39" s="22"/>
+      <c r="C39" s="22"/>
+      <c r="D39" s="22"/>
+      <c r="E39" s="22"/>
+      <c r="F39" s="22"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="18" t="s">
+      <c r="A40" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="B40" s="18"/>
-      <c r="C40" s="18"/>
-      <c r="D40" s="18"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="18"/>
+      <c r="B40" s="22"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="18" t="s">
+      <c r="A41" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="B41" s="18"/>
-      <c r="C41" s="18"/>
-      <c r="D41" s="18"/>
-      <c r="E41" s="18"/>
-      <c r="F41" s="18"/>
+      <c r="B41" s="22"/>
+      <c r="C41" s="22"/>
+      <c r="D41" s="22"/>
+      <c r="E41" s="22"/>
+      <c r="F41" s="22"/>
     </row>
     <row r="42" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
@@ -1231,44 +1232,44 @@
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="19" t="s">
+      <c r="A44" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="B44" s="19"/>
-      <c r="C44" s="19"/>
-      <c r="D44" s="19"/>
-      <c r="E44" s="19"/>
-      <c r="F44" s="19"/>
+      <c r="B44" s="21"/>
+      <c r="C44" s="21"/>
+      <c r="D44" s="21"/>
+      <c r="E44" s="21"/>
+      <c r="F44" s="21"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="19" t="s">
+      <c r="A45" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="B45" s="19"/>
-      <c r="C45" s="19"/>
-      <c r="D45" s="19"/>
-      <c r="E45" s="19"/>
-      <c r="F45" s="19"/>
+      <c r="B45" s="21"/>
+      <c r="C45" s="21"/>
+      <c r="D45" s="21"/>
+      <c r="E45" s="21"/>
+      <c r="F45" s="21"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="19" t="s">
+      <c r="A46" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="B46" s="19"/>
-      <c r="C46" s="19"/>
-      <c r="D46" s="19"/>
-      <c r="E46" s="19"/>
-      <c r="F46" s="19"/>
+      <c r="B46" s="21"/>
+      <c r="C46" s="21"/>
+      <c r="D46" s="21"/>
+      <c r="E46" s="21"/>
+      <c r="F46" s="21"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="19" t="s">
+      <c r="A47" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="B47" s="19"/>
-      <c r="C47" s="19"/>
-      <c r="D47" s="19"/>
-      <c r="E47" s="19"/>
-      <c r="F47" s="19"/>
+      <c r="B47" s="21"/>
+      <c r="C47" s="21"/>
+      <c r="D47" s="21"/>
+      <c r="E47" s="21"/>
+      <c r="F47" s="21"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
@@ -1286,44 +1287,44 @@
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="19" t="s">
+      <c r="A51" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="B51" s="19"/>
-      <c r="C51" s="19"/>
-      <c r="D51" s="19"/>
-      <c r="E51" s="19"/>
-      <c r="F51" s="19"/>
+      <c r="B51" s="21"/>
+      <c r="C51" s="21"/>
+      <c r="D51" s="21"/>
+      <c r="E51" s="21"/>
+      <c r="F51" s="21"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="19" t="s">
+      <c r="A52" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="B52" s="19"/>
-      <c r="C52" s="19"/>
-      <c r="D52" s="19"/>
-      <c r="E52" s="19"/>
-      <c r="F52" s="19"/>
+      <c r="B52" s="21"/>
+      <c r="C52" s="21"/>
+      <c r="D52" s="21"/>
+      <c r="E52" s="21"/>
+      <c r="F52" s="21"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="19" t="s">
+      <c r="A53" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="B53" s="19"/>
-      <c r="C53" s="19"/>
-      <c r="D53" s="19"/>
-      <c r="E53" s="19"/>
-      <c r="F53" s="19"/>
+      <c r="B53" s="21"/>
+      <c r="C53" s="21"/>
+      <c r="D53" s="21"/>
+      <c r="E53" s="21"/>
+      <c r="F53" s="21"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="18" t="s">
+      <c r="A54" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="B54" s="18"/>
-      <c r="C54" s="18"/>
-      <c r="D54" s="18"/>
-      <c r="E54" s="18"/>
-      <c r="F54" s="18"/>
+      <c r="B54" s="22"/>
+      <c r="C54" s="22"/>
+      <c r="D54" s="22"/>
+      <c r="E54" s="22"/>
+      <c r="F54" s="22"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="13" t="s">
@@ -1341,34 +1342,34 @@
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="19" t="s">
+      <c r="A58" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="B58" s="19"/>
-      <c r="C58" s="19"/>
-      <c r="D58" s="19"/>
-      <c r="E58" s="19"/>
-      <c r="F58" s="19"/>
+      <c r="B58" s="21"/>
+      <c r="C58" s="21"/>
+      <c r="D58" s="21"/>
+      <c r="E58" s="21"/>
+      <c r="F58" s="21"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="19" t="s">
+      <c r="A59" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="B59" s="19"/>
-      <c r="C59" s="19"/>
-      <c r="D59" s="19"/>
-      <c r="E59" s="19"/>
-      <c r="F59" s="19"/>
+      <c r="B59" s="21"/>
+      <c r="C59" s="21"/>
+      <c r="D59" s="21"/>
+      <c r="E59" s="21"/>
+      <c r="F59" s="21"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="18" t="s">
+      <c r="A60" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="B60" s="18"/>
-      <c r="C60" s="18"/>
-      <c r="D60" s="18"/>
-      <c r="E60" s="18"/>
-      <c r="F60" s="18"/>
+      <c r="B60" s="22"/>
+      <c r="C60" s="22"/>
+      <c r="D60" s="22"/>
+      <c r="E60" s="22"/>
+      <c r="F60" s="22"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="13" t="s">
@@ -1381,24 +1382,24 @@
       <c r="F61" s="13"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="18" t="s">
+      <c r="A62" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="B62" s="18"/>
-      <c r="C62" s="18"/>
-      <c r="D62" s="18"/>
-      <c r="E62" s="18"/>
-      <c r="F62" s="18"/>
+      <c r="B62" s="22"/>
+      <c r="C62" s="22"/>
+      <c r="D62" s="22"/>
+      <c r="E62" s="22"/>
+      <c r="F62" s="22"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="11" t="s">
+      <c r="A63" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="B63" s="11"/>
-      <c r="C63" s="11"/>
-      <c r="D63" s="11"/>
-      <c r="E63" s="11"/>
-      <c r="F63" s="11"/>
+      <c r="B63" s="18"/>
+      <c r="C63" s="18"/>
+      <c r="D63" s="18"/>
+      <c r="E63" s="18"/>
+      <c r="F63" s="18"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="11" t="s">
@@ -1421,14 +1422,14 @@
       <c r="F65" s="11"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="18" t="s">
+      <c r="A66" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="B66" s="18"/>
-      <c r="C66" s="18"/>
-      <c r="D66" s="18"/>
-      <c r="E66" s="18"/>
-      <c r="F66" s="18"/>
+      <c r="B66" s="22"/>
+      <c r="C66" s="22"/>
+      <c r="D66" s="22"/>
+      <c r="E66" s="22"/>
+      <c r="F66" s="22"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="17" t="s">
@@ -1446,44 +1447,44 @@
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="18" t="s">
+      <c r="A70" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="B70" s="18"/>
-      <c r="C70" s="18"/>
-      <c r="D70" s="18"/>
-      <c r="E70" s="18"/>
-      <c r="F70" s="18"/>
+      <c r="B70" s="22"/>
+      <c r="C70" s="22"/>
+      <c r="D70" s="22"/>
+      <c r="E70" s="22"/>
+      <c r="F70" s="22"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="18" t="s">
+      <c r="A71" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="B71" s="18"/>
-      <c r="C71" s="18"/>
-      <c r="D71" s="18"/>
-      <c r="E71" s="18"/>
-      <c r="F71" s="18"/>
+      <c r="B71" s="22"/>
+      <c r="C71" s="22"/>
+      <c r="D71" s="22"/>
+      <c r="E71" s="22"/>
+      <c r="F71" s="22"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="18" t="s">
+      <c r="A72" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="B72" s="18"/>
-      <c r="C72" s="18"/>
-      <c r="D72" s="18"/>
-      <c r="E72" s="18"/>
-      <c r="F72" s="18"/>
+      <c r="B72" s="22"/>
+      <c r="C72" s="22"/>
+      <c r="D72" s="22"/>
+      <c r="E72" s="22"/>
+      <c r="F72" s="22"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="18" t="s">
+      <c r="A73" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="B73" s="18"/>
-      <c r="C73" s="18"/>
-      <c r="D73" s="18"/>
-      <c r="E73" s="18"/>
-      <c r="F73" s="18"/>
+      <c r="B73" s="22"/>
+      <c r="C73" s="22"/>
+      <c r="D73" s="22"/>
+      <c r="E73" s="22"/>
+      <c r="F73" s="22"/>
     </row>
     <row r="75" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
@@ -1532,26 +1533,6 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A16:F16"/>
-    <mergeCell ref="A29:F29"/>
-    <mergeCell ref="A31:F31"/>
-    <mergeCell ref="A32:F32"/>
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="A34:F34"/>
-    <mergeCell ref="A35:F35"/>
-    <mergeCell ref="A36:F36"/>
-    <mergeCell ref="A39:F39"/>
-    <mergeCell ref="A40:F40"/>
-    <mergeCell ref="A41:F41"/>
-    <mergeCell ref="A44:F44"/>
-    <mergeCell ref="A45:F45"/>
-    <mergeCell ref="A46:F46"/>
-    <mergeCell ref="A47:F47"/>
-    <mergeCell ref="A51:F51"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="A53:F53"/>
-    <mergeCell ref="A54:F54"/>
     <mergeCell ref="A70:F70"/>
     <mergeCell ref="A71:F71"/>
     <mergeCell ref="A72:F72"/>
@@ -1561,6 +1542,26 @@
     <mergeCell ref="A60:F60"/>
     <mergeCell ref="A62:F62"/>
     <mergeCell ref="A66:F66"/>
+    <mergeCell ref="A47:F47"/>
+    <mergeCell ref="A51:F51"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="A53:F53"/>
+    <mergeCell ref="A54:F54"/>
+    <mergeCell ref="A40:F40"/>
+    <mergeCell ref="A41:F41"/>
+    <mergeCell ref="A44:F44"/>
+    <mergeCell ref="A45:F45"/>
+    <mergeCell ref="A46:F46"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A34:F34"/>
+    <mergeCell ref="A35:F35"/>
+    <mergeCell ref="A36:F36"/>
+    <mergeCell ref="A39:F39"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A29:F29"/>
+    <mergeCell ref="A31:F31"/>
+    <mergeCell ref="A32:F32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Made directional sprites for soldiers with machine gun, laser, and cannon. Created icon sprites to be used for the inventory. Updated wall sprite
</commit_message>
<xml_diff>
--- a/Production Documents/To-Do.xlsx
+++ b/Production Documents/To-Do.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmgam\Desktop\Shiva\Production Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78E595D5-02C4-42EB-B959-7187B73509AC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF2C2D0B-F1B8-4846-A5F4-172CB97D7AC4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{669DCC34-C837-4342-A908-0F87EB315612}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{669DCC34-C837-4342-A908-0F87EB315612}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="112">
   <si>
     <t>Sprites</t>
   </si>
@@ -341,6 +341,33 @@
   </si>
   <si>
     <t>Only certain tiles are visable</t>
+  </si>
+  <si>
+    <t>Inventory</t>
+  </si>
+  <si>
+    <t>Pistol Icon</t>
+  </si>
+  <si>
+    <t>Machine Gun Icon</t>
+  </si>
+  <si>
+    <t>Laser Icon</t>
+  </si>
+  <si>
+    <t>Rocket Icon</t>
+  </si>
+  <si>
+    <t>Manual Turret Icon</t>
+  </si>
+  <si>
+    <t>Manual Cannon Turret Icon</t>
+  </si>
+  <si>
+    <t>Automatic Alien Laser Turret Icon</t>
+  </si>
+  <si>
+    <t>Wall Icon</t>
   </si>
 </sst>
 </file>
@@ -450,7 +477,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
@@ -470,6 +497,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -800,10 +830,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4D254F2-4E19-40CF-BD85-766CDBA8C5EF}">
-  <dimension ref="A2:F79"/>
+  <dimension ref="A2:G79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="I65" sqref="I65"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -813,24 +843,25 @@
     <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="18" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="19" t="s">
+    <row r="3" spans="1:7" ht="18" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -849,8 +880,11 @@
       <c r="F4" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="21" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>74</v>
       </c>
@@ -869,8 +903,11 @@
       <c r="F5" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="19" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -889,8 +926,11 @@
       <c r="F6" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" s="19" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
@@ -909,8 +949,11 @@
       <c r="F7" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
@@ -925,8 +968,11 @@
         <v>27</v>
       </c>
       <c r="F8" s="4"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" s="19" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
@@ -941,8 +987,11 @@
         <v>28</v>
       </c>
       <c r="F9" s="4"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
@@ -955,8 +1004,11 @@
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" s="19" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>13</v>
       </c>
@@ -967,34 +1019,40 @@
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" s="19" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12" s="19" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C13" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C14" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A16" s="19" t="s">
+    <row r="16" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A16" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="19"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
@@ -1062,7 +1120,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="20" t="s">
         <v>18</v>
       </c>
       <c r="C21" s="3" t="s">
@@ -1072,7 +1130,7 @@
       <c r="F21" s="4"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="20" t="s">
         <v>19</v>
       </c>
       <c r="C22" s="9" t="s">
@@ -1083,7 +1141,7 @@
       <c r="F22" s="4"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="20" t="s">
         <v>20</v>
       </c>
       <c r="C23" s="3" t="s">
@@ -1114,14 +1172,14 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="20" t="s">
+      <c r="A29" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="20"/>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
+      <c r="B29" s="23"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="23"/>
     </row>
     <row r="30" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
@@ -1129,64 +1187,64 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="21" t="s">
+      <c r="A31" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="B31" s="21"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="21" t="s">
+      <c r="A32" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="B32" s="21"/>
-      <c r="C32" s="21"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="21"/>
-      <c r="F32" s="21"/>
+      <c r="B32" s="24"/>
+      <c r="C32" s="24"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="24"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="21" t="s">
+      <c r="A33" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="B33" s="21"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
-      <c r="F33" s="21"/>
+      <c r="B33" s="24"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="24"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="21" t="s">
+      <c r="A34" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="B34" s="21"/>
-      <c r="C34" s="21"/>
-      <c r="D34" s="21"/>
-      <c r="E34" s="21"/>
-      <c r="F34" s="21"/>
+      <c r="B34" s="24"/>
+      <c r="C34" s="24"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="24"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="21" t="s">
+      <c r="A35" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="B35" s="21"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
-      <c r="E35" s="21"/>
-      <c r="F35" s="21"/>
+      <c r="B35" s="24"/>
+      <c r="C35" s="24"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="21" t="s">
+      <c r="A36" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="B36" s="21"/>
-      <c r="C36" s="21"/>
-      <c r="D36" s="21"/>
-      <c r="E36" s="21"/>
-      <c r="F36" s="21"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="24"/>
+      <c r="D36" s="24"/>
+      <c r="E36" s="24"/>
+      <c r="F36" s="24"/>
     </row>
     <row r="38" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
@@ -1194,34 +1252,34 @@
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="22" t="s">
+      <c r="A39" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="B39" s="22"/>
-      <c r="C39" s="22"/>
-      <c r="D39" s="22"/>
-      <c r="E39" s="22"/>
-      <c r="F39" s="22"/>
+      <c r="B39" s="25"/>
+      <c r="C39" s="25"/>
+      <c r="D39" s="25"/>
+      <c r="E39" s="25"/>
+      <c r="F39" s="25"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="22" t="s">
+      <c r="A40" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="B40" s="22"/>
-      <c r="C40" s="22"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="22"/>
+      <c r="B40" s="25"/>
+      <c r="C40" s="25"/>
+      <c r="D40" s="25"/>
+      <c r="E40" s="25"/>
+      <c r="F40" s="25"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="22" t="s">
+      <c r="A41" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="B41" s="22"/>
-      <c r="C41" s="22"/>
-      <c r="D41" s="22"/>
-      <c r="E41" s="22"/>
-      <c r="F41" s="22"/>
+      <c r="B41" s="25"/>
+      <c r="C41" s="25"/>
+      <c r="D41" s="25"/>
+      <c r="E41" s="25"/>
+      <c r="F41" s="25"/>
     </row>
     <row r="42" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
@@ -1232,44 +1290,44 @@
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="21" t="s">
+      <c r="A44" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="B44" s="21"/>
-      <c r="C44" s="21"/>
-      <c r="D44" s="21"/>
-      <c r="E44" s="21"/>
-      <c r="F44" s="21"/>
+      <c r="B44" s="24"/>
+      <c r="C44" s="24"/>
+      <c r="D44" s="24"/>
+      <c r="E44" s="24"/>
+      <c r="F44" s="24"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="21" t="s">
+      <c r="A45" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="B45" s="21"/>
-      <c r="C45" s="21"/>
-      <c r="D45" s="21"/>
-      <c r="E45" s="21"/>
-      <c r="F45" s="21"/>
+      <c r="B45" s="24"/>
+      <c r="C45" s="24"/>
+      <c r="D45" s="24"/>
+      <c r="E45" s="24"/>
+      <c r="F45" s="24"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="21" t="s">
+      <c r="A46" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="B46" s="21"/>
-      <c r="C46" s="21"/>
-      <c r="D46" s="21"/>
-      <c r="E46" s="21"/>
-      <c r="F46" s="21"/>
+      <c r="B46" s="24"/>
+      <c r="C46" s="24"/>
+      <c r="D46" s="24"/>
+      <c r="E46" s="24"/>
+      <c r="F46" s="24"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="21" t="s">
+      <c r="A47" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="B47" s="21"/>
-      <c r="C47" s="21"/>
-      <c r="D47" s="21"/>
-      <c r="E47" s="21"/>
-      <c r="F47" s="21"/>
+      <c r="B47" s="24"/>
+      <c r="C47" s="24"/>
+      <c r="D47" s="24"/>
+      <c r="E47" s="24"/>
+      <c r="F47" s="24"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
@@ -1287,44 +1345,44 @@
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="21" t="s">
+      <c r="A51" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="B51" s="21"/>
-      <c r="C51" s="21"/>
-      <c r="D51" s="21"/>
-      <c r="E51" s="21"/>
-      <c r="F51" s="21"/>
+      <c r="B51" s="24"/>
+      <c r="C51" s="24"/>
+      <c r="D51" s="24"/>
+      <c r="E51" s="24"/>
+      <c r="F51" s="24"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="21" t="s">
+      <c r="A52" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="B52" s="21"/>
-      <c r="C52" s="21"/>
-      <c r="D52" s="21"/>
-      <c r="E52" s="21"/>
-      <c r="F52" s="21"/>
+      <c r="B52" s="24"/>
+      <c r="C52" s="24"/>
+      <c r="D52" s="24"/>
+      <c r="E52" s="24"/>
+      <c r="F52" s="24"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="21" t="s">
+      <c r="A53" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="B53" s="21"/>
-      <c r="C53" s="21"/>
-      <c r="D53" s="21"/>
-      <c r="E53" s="21"/>
-      <c r="F53" s="21"/>
+      <c r="B53" s="24"/>
+      <c r="C53" s="24"/>
+      <c r="D53" s="24"/>
+      <c r="E53" s="24"/>
+      <c r="F53" s="24"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="22" t="s">
+      <c r="A54" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="B54" s="22"/>
-      <c r="C54" s="22"/>
-      <c r="D54" s="22"/>
-      <c r="E54" s="22"/>
-      <c r="F54" s="22"/>
+      <c r="B54" s="25"/>
+      <c r="C54" s="25"/>
+      <c r="D54" s="25"/>
+      <c r="E54" s="25"/>
+      <c r="F54" s="25"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="13" t="s">
@@ -1342,34 +1400,34 @@
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="21" t="s">
+      <c r="A58" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="B58" s="21"/>
-      <c r="C58" s="21"/>
-      <c r="D58" s="21"/>
-      <c r="E58" s="21"/>
-      <c r="F58" s="21"/>
+      <c r="B58" s="24"/>
+      <c r="C58" s="24"/>
+      <c r="D58" s="24"/>
+      <c r="E58" s="24"/>
+      <c r="F58" s="24"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="21" t="s">
+      <c r="A59" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="B59" s="21"/>
-      <c r="C59" s="21"/>
-      <c r="D59" s="21"/>
-      <c r="E59" s="21"/>
-      <c r="F59" s="21"/>
+      <c r="B59" s="24"/>
+      <c r="C59" s="24"/>
+      <c r="D59" s="24"/>
+      <c r="E59" s="24"/>
+      <c r="F59" s="24"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="22" t="s">
+      <c r="A60" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="B60" s="22"/>
-      <c r="C60" s="22"/>
-      <c r="D60" s="22"/>
-      <c r="E60" s="22"/>
-      <c r="F60" s="22"/>
+      <c r="B60" s="25"/>
+      <c r="C60" s="25"/>
+      <c r="D60" s="25"/>
+      <c r="E60" s="25"/>
+      <c r="F60" s="25"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="13" t="s">
@@ -1382,14 +1440,14 @@
       <c r="F61" s="13"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="22" t="s">
+      <c r="A62" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="B62" s="22"/>
-      <c r="C62" s="22"/>
-      <c r="D62" s="22"/>
-      <c r="E62" s="22"/>
-      <c r="F62" s="22"/>
+      <c r="B62" s="25"/>
+      <c r="C62" s="25"/>
+      <c r="D62" s="25"/>
+      <c r="E62" s="25"/>
+      <c r="F62" s="25"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="18" t="s">
@@ -1422,14 +1480,14 @@
       <c r="F65" s="11"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="22" t="s">
+      <c r="A66" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="B66" s="22"/>
-      <c r="C66" s="22"/>
-      <c r="D66" s="22"/>
-      <c r="E66" s="22"/>
-      <c r="F66" s="22"/>
+      <c r="B66" s="25"/>
+      <c r="C66" s="25"/>
+      <c r="D66" s="25"/>
+      <c r="E66" s="25"/>
+      <c r="F66" s="25"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="17" t="s">
@@ -1447,44 +1505,44 @@
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="22" t="s">
+      <c r="A70" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="B70" s="22"/>
-      <c r="C70" s="22"/>
-      <c r="D70" s="22"/>
-      <c r="E70" s="22"/>
-      <c r="F70" s="22"/>
+      <c r="B70" s="25"/>
+      <c r="C70" s="25"/>
+      <c r="D70" s="25"/>
+      <c r="E70" s="25"/>
+      <c r="F70" s="25"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="22" t="s">
+      <c r="A71" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="B71" s="22"/>
-      <c r="C71" s="22"/>
-      <c r="D71" s="22"/>
-      <c r="E71" s="22"/>
-      <c r="F71" s="22"/>
+      <c r="B71" s="25"/>
+      <c r="C71" s="25"/>
+      <c r="D71" s="25"/>
+      <c r="E71" s="25"/>
+      <c r="F71" s="25"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="22" t="s">
+      <c r="A72" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="B72" s="22"/>
-      <c r="C72" s="22"/>
-      <c r="D72" s="22"/>
-      <c r="E72" s="22"/>
-      <c r="F72" s="22"/>
+      <c r="B72" s="25"/>
+      <c r="C72" s="25"/>
+      <c r="D72" s="25"/>
+      <c r="E72" s="25"/>
+      <c r="F72" s="25"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="22" t="s">
+      <c r="A73" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="B73" s="22"/>
-      <c r="C73" s="22"/>
-      <c r="D73" s="22"/>
-      <c r="E73" s="22"/>
-      <c r="F73" s="22"/>
+      <c r="B73" s="25"/>
+      <c r="C73" s="25"/>
+      <c r="D73" s="25"/>
+      <c r="E73" s="25"/>
+      <c r="F73" s="25"/>
     </row>
     <row r="75" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">

</xml_diff>

<commit_message>
Added not being able to walk on water or mountains. Working on inventory
</commit_message>
<xml_diff>
--- a/Production Documents/To-Do.xlsx
+++ b/Production Documents/To-Do.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Shiva\Production Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmgam\Desktop\Shiva\Production Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{090A6648-4C80-44A2-8670-F699C92FFCF7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1712D335-CCD6-4793-A5BD-6A9620B9BCD4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{669DCC34-C837-4342-A908-0F87EB315612}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{669DCC34-C837-4342-A908-0F87EB315612}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="117">
   <si>
     <t>Sprites</t>
   </si>
@@ -498,7 +498,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
@@ -522,15 +522,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="3" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="3" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -855,26 +856,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4D254F2-4E19-40CF-BD85-766CDBA8C5EF}">
   <dimension ref="A2:G84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="H56" sqref="H56"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="G57" sqref="G57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="18" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="18" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A3" s="25" t="s">
         <v>1</v>
       </c>
@@ -884,7 +885,7 @@
       <c r="E3" s="25"/>
       <c r="F3" s="25"/>
     </row>
-    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -907,7 +908,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>74</v>
       </c>
@@ -930,7 +931,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -953,7 +954,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
@@ -976,7 +977,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
@@ -995,7 +996,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
@@ -1014,7 +1015,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
@@ -1031,7 +1032,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>13</v>
       </c>
@@ -1046,7 +1047,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
@@ -1057,17 +1058,17 @@
         <v>111</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C13" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C14" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A16" s="25" t="s">
         <v>34</v>
       </c>
@@ -1077,7 +1078,7 @@
       <c r="E16" s="25"/>
       <c r="F16" s="25"/>
     </row>
-    <row r="17" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
         <v>3</v>
@@ -1095,7 +1096,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B18" s="8" t="s">
         <v>15</v>
       </c>
@@ -1112,7 +1113,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
@@ -1127,7 +1128,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
@@ -1142,7 +1143,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B21" s="20" t="s">
         <v>18</v>
       </c>
@@ -1152,7 +1153,7 @@
       <c r="D21" s="4"/>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" s="20" t="s">
         <v>19</v>
       </c>
@@ -1163,7 +1164,7 @@
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" s="20" t="s">
         <v>20</v>
       </c>
@@ -1174,27 +1175,27 @@
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C24" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C25" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C26" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C27" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="26" t="s">
         <v>42</v>
       </c>
@@ -1204,165 +1205,168 @@
       <c r="E29" s="26"/>
       <c r="F29" s="26"/>
     </row>
-    <row r="30" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="24" t="s">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="B31" s="24"/>
-      <c r="C31" s="24"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="24"/>
-      <c r="F31" s="24"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="24" t="s">
+      <c r="B31" s="27"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="27"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="B32" s="24"/>
-      <c r="C32" s="24"/>
-      <c r="D32" s="24"/>
-      <c r="E32" s="24"/>
-      <c r="F32" s="24"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="24" t="s">
+      <c r="B32" s="27"/>
+      <c r="C32" s="27"/>
+      <c r="D32" s="27"/>
+      <c r="E32" s="27"/>
+      <c r="F32" s="27"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="B33" s="24"/>
-      <c r="C33" s="24"/>
-      <c r="D33" s="24"/>
-      <c r="E33" s="24"/>
-      <c r="F33" s="24"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="24" t="s">
+      <c r="B33" s="27"/>
+      <c r="C33" s="27"/>
+      <c r="D33" s="27"/>
+      <c r="E33" s="27"/>
+      <c r="F33" s="27"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="B34" s="24"/>
-      <c r="C34" s="24"/>
-      <c r="D34" s="24"/>
-      <c r="E34" s="24"/>
-      <c r="F34" s="24"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" s="24" t="s">
+      <c r="B34" s="27"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="27"/>
+      <c r="E34" s="27"/>
+      <c r="F34" s="27"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="B35" s="24"/>
-      <c r="C35" s="24"/>
-      <c r="D35" s="24"/>
-      <c r="E35" s="24"/>
-      <c r="F35" s="24"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="24" t="s">
+      <c r="B35" s="27"/>
+      <c r="C35" s="27"/>
+      <c r="D35" s="27"/>
+      <c r="E35" s="27"/>
+      <c r="F35" s="27"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="B36" s="24"/>
-      <c r="C36" s="24"/>
-      <c r="D36" s="24"/>
-      <c r="E36" s="24"/>
-      <c r="F36" s="24"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="22" t="s">
+      <c r="B36" s="27"/>
+      <c r="C36" s="27"/>
+      <c r="D36" s="27"/>
+      <c r="E36" s="27"/>
+      <c r="F36" s="27"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="B37" s="22"/>
-      <c r="C37" s="22"/>
-      <c r="D37" s="22"/>
-      <c r="E37" s="22"/>
-      <c r="F37" s="22"/>
-    </row>
-    <row r="39" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B37" s="23"/>
+      <c r="C37" s="23"/>
+      <c r="D37" s="23"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="23"/>
+      <c r="G37" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="23" t="s">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="B40" s="23"/>
-      <c r="C40" s="23"/>
-      <c r="D40" s="23"/>
-      <c r="E40" s="23"/>
-      <c r="F40" s="23"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" s="23" t="s">
+      <c r="B40" s="28"/>
+      <c r="C40" s="28"/>
+      <c r="D40" s="28"/>
+      <c r="E40" s="28"/>
+      <c r="F40" s="28"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="B41" s="23"/>
-      <c r="C41" s="23"/>
-      <c r="D41" s="23"/>
-      <c r="E41" s="23"/>
-      <c r="F41" s="23"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" s="23" t="s">
+      <c r="B41" s="28"/>
+      <c r="C41" s="28"/>
+      <c r="D41" s="28"/>
+      <c r="E41" s="28"/>
+      <c r="F41" s="28"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="B42" s="23"/>
-      <c r="C42" s="23"/>
-      <c r="D42" s="23"/>
-      <c r="E42" s="23"/>
-      <c r="F42" s="23"/>
-    </row>
-    <row r="43" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B42" s="28"/>
+      <c r="C42" s="28"/>
+      <c r="D42" s="28"/>
+      <c r="E42" s="28"/>
+      <c r="F42" s="28"/>
+    </row>
+    <row r="43" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
     </row>
-    <row r="44" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45" s="24" t="s">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="B45" s="24"/>
-      <c r="C45" s="24"/>
-      <c r="D45" s="24"/>
-      <c r="E45" s="24"/>
-      <c r="F45" s="24"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" s="24" t="s">
+      <c r="B45" s="27"/>
+      <c r="C45" s="27"/>
+      <c r="D45" s="27"/>
+      <c r="E45" s="27"/>
+      <c r="F45" s="27"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="B46" s="24"/>
-      <c r="C46" s="24"/>
-      <c r="D46" s="24"/>
-      <c r="E46" s="24"/>
-      <c r="F46" s="24"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" s="24" t="s">
+      <c r="B46" s="27"/>
+      <c r="C46" s="27"/>
+      <c r="D46" s="27"/>
+      <c r="E46" s="27"/>
+      <c r="F46" s="27"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="B47" s="24"/>
-      <c r="C47" s="24"/>
-      <c r="D47" s="24"/>
-      <c r="E47" s="24"/>
-      <c r="F47" s="24"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A48" s="24" t="s">
+      <c r="B47" s="27"/>
+      <c r="C47" s="27"/>
+      <c r="D47" s="27"/>
+      <c r="E47" s="27"/>
+      <c r="F47" s="27"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="B48" s="24"/>
-      <c r="C48" s="24"/>
-      <c r="D48" s="24"/>
-      <c r="E48" s="24"/>
-      <c r="F48" s="24"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B48" s="27"/>
+      <c r="C48" s="27"/>
+      <c r="D48" s="27"/>
+      <c r="E48" s="27"/>
+      <c r="F48" s="27"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
         <v>76</v>
       </c>
@@ -1372,52 +1376,52 @@
       <c r="E49" s="10"/>
       <c r="F49" s="10"/>
     </row>
-    <row r="51" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A52" s="24" t="s">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="B52" s="24"/>
-      <c r="C52" s="24"/>
-      <c r="D52" s="24"/>
-      <c r="E52" s="24"/>
-      <c r="F52" s="24"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A53" s="24" t="s">
+      <c r="B52" s="27"/>
+      <c r="C52" s="27"/>
+      <c r="D52" s="27"/>
+      <c r="E52" s="27"/>
+      <c r="F52" s="27"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="B53" s="24"/>
-      <c r="C53" s="24"/>
-      <c r="D53" s="24"/>
-      <c r="E53" s="24"/>
-      <c r="F53" s="24"/>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A54" s="24" t="s">
+      <c r="B53" s="27"/>
+      <c r="C53" s="27"/>
+      <c r="D53" s="27"/>
+      <c r="E53" s="27"/>
+      <c r="F53" s="27"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="B54" s="24"/>
-      <c r="C54" s="24"/>
-      <c r="D54" s="24"/>
-      <c r="E54" s="24"/>
-      <c r="F54" s="24"/>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A55" s="23" t="s">
+      <c r="B54" s="27"/>
+      <c r="C54" s="27"/>
+      <c r="D54" s="27"/>
+      <c r="E54" s="27"/>
+      <c r="F54" s="27"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="B55" s="23"/>
-      <c r="C55" s="23"/>
-      <c r="D55" s="23"/>
-      <c r="E55" s="23"/>
-      <c r="F55" s="23"/>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B55" s="28"/>
+      <c r="C55" s="28"/>
+      <c r="D55" s="28"/>
+      <c r="E55" s="28"/>
+      <c r="F55" s="28"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="13" t="s">
         <v>77</v>
       </c>
@@ -1427,45 +1431,45 @@
       <c r="E56" s="13"/>
       <c r="F56" s="13"/>
     </row>
-    <row r="58" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A59" s="24" t="s">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="B59" s="24"/>
-      <c r="C59" s="24"/>
-      <c r="D59" s="24"/>
-      <c r="E59" s="24"/>
-      <c r="F59" s="24"/>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A60" s="24" t="s">
+      <c r="B59" s="27"/>
+      <c r="C59" s="27"/>
+      <c r="D59" s="27"/>
+      <c r="E59" s="27"/>
+      <c r="F59" s="27"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="B60" s="24"/>
-      <c r="C60" s="24"/>
-      <c r="D60" s="24"/>
-      <c r="E60" s="24"/>
-      <c r="F60" s="24"/>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A61" s="23" t="s">
+      <c r="B60" s="27"/>
+      <c r="C60" s="27"/>
+      <c r="D60" s="27"/>
+      <c r="E60" s="27"/>
+      <c r="F60" s="27"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="B61" s="23"/>
-      <c r="C61" s="23"/>
-      <c r="D61" s="23"/>
-      <c r="E61" s="23"/>
-      <c r="F61" s="23"/>
+      <c r="B61" s="28"/>
+      <c r="C61" s="28"/>
+      <c r="D61" s="28"/>
+      <c r="E61" s="28"/>
+      <c r="F61" s="28"/>
       <c r="G61" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="13" t="s">
         <v>85</v>
       </c>
@@ -1475,20 +1479,20 @@
       <c r="E62" s="13"/>
       <c r="F62" s="13"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A63" s="23" t="s">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="B63" s="23"/>
-      <c r="C63" s="23"/>
-      <c r="D63" s="23"/>
-      <c r="E63" s="23"/>
-      <c r="F63" s="23"/>
+      <c r="B63" s="28"/>
+      <c r="C63" s="28"/>
+      <c r="D63" s="28"/>
+      <c r="E63" s="28"/>
+      <c r="F63" s="28"/>
       <c r="G63" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="18" t="s">
         <v>100</v>
       </c>
@@ -1498,7 +1502,7 @@
       <c r="E64" s="18"/>
       <c r="F64" s="18"/>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="11" t="s">
         <v>83</v>
       </c>
@@ -1511,7 +1515,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="11" t="s">
         <v>84</v>
       </c>
@@ -1524,17 +1528,17 @@
         <v>115</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A67" s="23" t="s">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="B67" s="23"/>
-      <c r="C67" s="23"/>
-      <c r="D67" s="23"/>
-      <c r="E67" s="23"/>
-      <c r="F67" s="23"/>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B67" s="28"/>
+      <c r="C67" s="28"/>
+      <c r="D67" s="28"/>
+      <c r="E67" s="28"/>
+      <c r="F67" s="28"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="17" t="s">
         <v>101</v>
       </c>
@@ -1547,57 +1551,57 @@
         <v>115</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A71" s="23" t="s">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="B71" s="23"/>
-      <c r="C71" s="23"/>
-      <c r="D71" s="23"/>
-      <c r="E71" s="23"/>
-      <c r="F71" s="23"/>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A72" s="23" t="s">
+      <c r="B71" s="28"/>
+      <c r="C71" s="28"/>
+      <c r="D71" s="28"/>
+      <c r="E71" s="28"/>
+      <c r="F71" s="28"/>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="B72" s="23"/>
-      <c r="C72" s="23"/>
-      <c r="D72" s="23"/>
-      <c r="E72" s="23"/>
-      <c r="F72" s="23"/>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A73" s="23" t="s">
+      <c r="B72" s="28"/>
+      <c r="C72" s="28"/>
+      <c r="D72" s="28"/>
+      <c r="E72" s="28"/>
+      <c r="F72" s="28"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="B73" s="23"/>
-      <c r="C73" s="23"/>
-      <c r="D73" s="23"/>
-      <c r="E73" s="23"/>
-      <c r="F73" s="23"/>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A74" s="23" t="s">
+      <c r="B73" s="28"/>
+      <c r="C73" s="28"/>
+      <c r="D73" s="28"/>
+      <c r="E73" s="28"/>
+      <c r="F73" s="28"/>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="B74" s="23"/>
-      <c r="C74" s="23"/>
-      <c r="D74" s="23"/>
-      <c r="E74" s="23"/>
-      <c r="F74" s="23"/>
-    </row>
-    <row r="76" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B74" s="28"/>
+      <c r="C74" s="28"/>
+      <c r="D74" s="28"/>
+      <c r="E74" s="28"/>
+      <c r="F74" s="28"/>
+    </row>
+    <row r="76" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="16" t="s">
         <v>79</v>
       </c>
@@ -1607,7 +1611,7 @@
       <c r="E77" s="16"/>
       <c r="F77" s="16"/>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="11" t="s">
         <v>98</v>
       </c>
@@ -1617,7 +1621,7 @@
       <c r="E78" s="11"/>
       <c r="F78" s="11"/>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="12" t="s">
         <v>99</v>
       </c>
@@ -1627,12 +1631,12 @@
       <c r="E79" s="12"/>
       <c r="F79" s="12"/>
     </row>
-    <row r="81" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="27" t="s">
+    <row r="81" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="24" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="22" t="s">
         <v>113</v>
       </c>
@@ -1645,7 +1649,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="22" t="s">
         <v>114</v>
       </c>
@@ -1658,7 +1662,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="17" t="s">
         <v>102</v>
       </c>
@@ -1670,26 +1674,6 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A16:F16"/>
-    <mergeCell ref="A29:F29"/>
-    <mergeCell ref="A31:F31"/>
-    <mergeCell ref="A32:F32"/>
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="A34:F34"/>
-    <mergeCell ref="A35:F35"/>
-    <mergeCell ref="A36:F36"/>
-    <mergeCell ref="A40:F40"/>
-    <mergeCell ref="A41:F41"/>
-    <mergeCell ref="A42:F42"/>
-    <mergeCell ref="A45:F45"/>
-    <mergeCell ref="A46:F46"/>
-    <mergeCell ref="A47:F47"/>
-    <mergeCell ref="A48:F48"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="A53:F53"/>
-    <mergeCell ref="A54:F54"/>
-    <mergeCell ref="A55:F55"/>
     <mergeCell ref="A71:F71"/>
     <mergeCell ref="A72:F72"/>
     <mergeCell ref="A73:F73"/>
@@ -1699,6 +1683,26 @@
     <mergeCell ref="A61:F61"/>
     <mergeCell ref="A63:F63"/>
     <mergeCell ref="A67:F67"/>
+    <mergeCell ref="A48:F48"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="A53:F53"/>
+    <mergeCell ref="A54:F54"/>
+    <mergeCell ref="A55:F55"/>
+    <mergeCell ref="A41:F41"/>
+    <mergeCell ref="A42:F42"/>
+    <mergeCell ref="A45:F45"/>
+    <mergeCell ref="A46:F46"/>
+    <mergeCell ref="A47:F47"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A34:F34"/>
+    <mergeCell ref="A35:F35"/>
+    <mergeCell ref="A36:F36"/>
+    <mergeCell ref="A40:F40"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A29:F29"/>
+    <mergeCell ref="A31:F31"/>
+    <mergeCell ref="A32:F32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1712,29 +1716,29 @@
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.109375" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>82</v>
       </c>
@@ -1742,7 +1746,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>88</v>
       </c>
@@ -1750,7 +1754,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>89</v>
       </c>
@@ -1758,7 +1762,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>90</v>
       </c>
@@ -1766,7 +1770,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>81</v>
       </c>
@@ -1774,7 +1778,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>91</v>
       </c>
@@ -1782,7 +1786,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B9" s="15">
         <f>SUM(B3:B8)</f>
         <v>1</v>
@@ -1794,7 +1798,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="J10" t="s">
         <v>89</v>
       </c>
@@ -1811,7 +1815,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>13</v>
       </c>
@@ -1831,7 +1835,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>82</v>
       </c>
@@ -1842,7 +1846,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>88</v>
       </c>
@@ -1853,7 +1857,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>89</v>
       </c>
@@ -1861,7 +1865,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>90</v>
       </c>
@@ -1869,7 +1873,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>81</v>
       </c>
@@ -1877,7 +1881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>91</v>
       </c>
@@ -1885,18 +1889,18 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B18" s="15">
         <f>SUM(B12:B17)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>82</v>
       </c>
@@ -1904,7 +1908,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>88</v>
       </c>
@@ -1912,7 +1916,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>89</v>
       </c>
@@ -1920,7 +1924,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>90</v>
       </c>
@@ -1928,7 +1932,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>81</v>
       </c>
@@ -1936,7 +1940,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>91</v>
       </c>
@@ -1944,18 +1948,18 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B27" s="15">
         <f>SUM(B21:B26)</f>
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>82</v>
       </c>
@@ -1963,7 +1967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>88</v>
       </c>
@@ -1971,7 +1975,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>89</v>
       </c>
@@ -1979,7 +1983,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>90</v>
       </c>
@@ -1987,7 +1991,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>81</v>
       </c>
@@ -1995,7 +1999,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>91</v>
       </c>
@@ -2003,18 +2007,18 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B36" s="15">
         <f>SUM(B30:B35)</f>
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>82</v>
       </c>
@@ -2022,7 +2026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>88</v>
       </c>
@@ -2030,7 +2034,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>89</v>
       </c>
@@ -2038,7 +2042,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>90</v>
       </c>
@@ -2046,7 +2050,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>81</v>
       </c>
@@ -2054,7 +2058,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>91</v>
       </c>
@@ -2062,7 +2066,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B45" s="15">
         <f>SUM(B39:B44)</f>
         <v>1</v>

</xml_diff>

<commit_message>
Inventory working for weapons
</commit_message>
<xml_diff>
--- a/Production Documents/To-Do.xlsx
+++ b/Production Documents/To-Do.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmgam\Desktop\Shiva\Production Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1712D335-CCD6-4793-A5BD-6A9620B9BCD4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC12BB23-80BA-4D1D-B477-89DD5EBD1FFC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{669DCC34-C837-4342-A908-0F87EB315612}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="117">
   <si>
     <t>Sprites</t>
   </si>
@@ -498,7 +498,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
@@ -524,14 +524,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="3" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -857,7 +858,7 @@
   <dimension ref="A2:G84"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="G57" sqref="G57"/>
+      <selection activeCell="G65" sqref="G65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -876,14 +877,14 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="18" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -1069,14 +1070,14 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A16" s="25" t="s">
+      <c r="A16" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
@@ -1196,14 +1197,14 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="26" t="s">
+      <c r="A29" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
     </row>
     <row r="30" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
@@ -1289,34 +1290,34 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="28" t="s">
+      <c r="A40" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="B40" s="28"/>
-      <c r="C40" s="28"/>
-      <c r="D40" s="28"/>
-      <c r="E40" s="28"/>
-      <c r="F40" s="28"/>
+      <c r="B40" s="26"/>
+      <c r="C40" s="26"/>
+      <c r="D40" s="26"/>
+      <c r="E40" s="26"/>
+      <c r="F40" s="26"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="28" t="s">
+      <c r="A41" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="B41" s="28"/>
-      <c r="C41" s="28"/>
-      <c r="D41" s="28"/>
-      <c r="E41" s="28"/>
-      <c r="F41" s="28"/>
+      <c r="B41" s="26"/>
+      <c r="C41" s="26"/>
+      <c r="D41" s="26"/>
+      <c r="E41" s="26"/>
+      <c r="F41" s="26"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="28" t="s">
+      <c r="A42" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="B42" s="28"/>
-      <c r="C42" s="28"/>
-      <c r="D42" s="28"/>
-      <c r="E42" s="28"/>
-      <c r="F42" s="28"/>
+      <c r="B42" s="26"/>
+      <c r="C42" s="26"/>
+      <c r="D42" s="26"/>
+      <c r="E42" s="26"/>
+      <c r="F42" s="26"/>
     </row>
     <row r="43" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
@@ -1412,14 +1413,14 @@
       <c r="F54" s="27"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="28" t="s">
+      <c r="A55" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="B55" s="28"/>
-      <c r="C55" s="28"/>
-      <c r="D55" s="28"/>
-      <c r="E55" s="28"/>
-      <c r="F55" s="28"/>
+      <c r="B55" s="26"/>
+      <c r="C55" s="26"/>
+      <c r="D55" s="26"/>
+      <c r="E55" s="26"/>
+      <c r="F55" s="26"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="13" t="s">
@@ -1457,14 +1458,14 @@
       <c r="F60" s="27"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="28" t="s">
+      <c r="A61" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="B61" s="28"/>
-      <c r="C61" s="28"/>
-      <c r="D61" s="28"/>
-      <c r="E61" s="28"/>
-      <c r="F61" s="28"/>
+      <c r="B61" s="26"/>
+      <c r="C61" s="26"/>
+      <c r="D61" s="26"/>
+      <c r="E61" s="26"/>
+      <c r="F61" s="26"/>
       <c r="G61" t="s">
         <v>115</v>
       </c>
@@ -1480,14 +1481,14 @@
       <c r="F62" s="13"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="28" t="s">
+      <c r="A63" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="B63" s="28"/>
-      <c r="C63" s="28"/>
-      <c r="D63" s="28"/>
-      <c r="E63" s="28"/>
-      <c r="F63" s="28"/>
+      <c r="B63" s="26"/>
+      <c r="C63" s="26"/>
+      <c r="D63" s="26"/>
+      <c r="E63" s="26"/>
+      <c r="F63" s="26"/>
       <c r="G63" t="s">
         <v>115</v>
       </c>
@@ -1503,17 +1504,14 @@
       <c r="F64" s="18"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="11" t="s">
+      <c r="A65" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="B65" s="11"/>
-      <c r="C65" s="11"/>
-      <c r="D65" s="11"/>
-      <c r="E65" s="11"/>
-      <c r="F65" s="11"/>
-      <c r="G65" t="s">
-        <v>115</v>
-      </c>
+      <c r="B65" s="25"/>
+      <c r="C65" s="25"/>
+      <c r="D65" s="25"/>
+      <c r="E65" s="25"/>
+      <c r="F65" s="25"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="11" t="s">
@@ -1529,14 +1527,14 @@
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67" s="28" t="s">
+      <c r="A67" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="B67" s="28"/>
-      <c r="C67" s="28"/>
-      <c r="D67" s="28"/>
-      <c r="E67" s="28"/>
-      <c r="F67" s="28"/>
+      <c r="B67" s="26"/>
+      <c r="C67" s="26"/>
+      <c r="D67" s="26"/>
+      <c r="E67" s="26"/>
+      <c r="F67" s="26"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="17" t="s">
@@ -1557,44 +1555,44 @@
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" s="28" t="s">
+      <c r="A71" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="B71" s="28"/>
-      <c r="C71" s="28"/>
-      <c r="D71" s="28"/>
-      <c r="E71" s="28"/>
-      <c r="F71" s="28"/>
+      <c r="B71" s="26"/>
+      <c r="C71" s="26"/>
+      <c r="D71" s="26"/>
+      <c r="E71" s="26"/>
+      <c r="F71" s="26"/>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" s="28" t="s">
+      <c r="A72" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="B72" s="28"/>
-      <c r="C72" s="28"/>
-      <c r="D72" s="28"/>
-      <c r="E72" s="28"/>
-      <c r="F72" s="28"/>
+      <c r="B72" s="26"/>
+      <c r="C72" s="26"/>
+      <c r="D72" s="26"/>
+      <c r="E72" s="26"/>
+      <c r="F72" s="26"/>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" s="28" t="s">
+      <c r="A73" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="B73" s="28"/>
-      <c r="C73" s="28"/>
-      <c r="D73" s="28"/>
-      <c r="E73" s="28"/>
-      <c r="F73" s="28"/>
+      <c r="B73" s="26"/>
+      <c r="C73" s="26"/>
+      <c r="D73" s="26"/>
+      <c r="E73" s="26"/>
+      <c r="F73" s="26"/>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" s="28" t="s">
+      <c r="A74" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="B74" s="28"/>
-      <c r="C74" s="28"/>
-      <c r="D74" s="28"/>
-      <c r="E74" s="28"/>
-      <c r="F74" s="28"/>
+      <c r="B74" s="26"/>
+      <c r="C74" s="26"/>
+      <c r="D74" s="26"/>
+      <c r="E74" s="26"/>
+      <c r="F74" s="26"/>
     </row>
     <row r="76" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
@@ -1674,6 +1672,26 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A29:F29"/>
+    <mergeCell ref="A31:F31"/>
+    <mergeCell ref="A32:F32"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A34:F34"/>
+    <mergeCell ref="A35:F35"/>
+    <mergeCell ref="A36:F36"/>
+    <mergeCell ref="A40:F40"/>
+    <mergeCell ref="A41:F41"/>
+    <mergeCell ref="A42:F42"/>
+    <mergeCell ref="A45:F45"/>
+    <mergeCell ref="A46:F46"/>
+    <mergeCell ref="A47:F47"/>
+    <mergeCell ref="A48:F48"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="A53:F53"/>
+    <mergeCell ref="A54:F54"/>
+    <mergeCell ref="A55:F55"/>
     <mergeCell ref="A71:F71"/>
     <mergeCell ref="A72:F72"/>
     <mergeCell ref="A73:F73"/>
@@ -1683,26 +1701,6 @@
     <mergeCell ref="A61:F61"/>
     <mergeCell ref="A63:F63"/>
     <mergeCell ref="A67:F67"/>
-    <mergeCell ref="A48:F48"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="A53:F53"/>
-    <mergeCell ref="A54:F54"/>
-    <mergeCell ref="A55:F55"/>
-    <mergeCell ref="A41:F41"/>
-    <mergeCell ref="A42:F42"/>
-    <mergeCell ref="A45:F45"/>
-    <mergeCell ref="A46:F46"/>
-    <mergeCell ref="A47:F47"/>
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="A34:F34"/>
-    <mergeCell ref="A35:F35"/>
-    <mergeCell ref="A36:F36"/>
-    <mergeCell ref="A40:F40"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A16:F16"/>
-    <mergeCell ref="A29:F29"/>
-    <mergeCell ref="A31:F31"/>
-    <mergeCell ref="A32:F32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Implemented discovering weapons incrementing the item quantity in the inventory. Implemented a food button for humans that feeds humans. Button only shows up when the human is clicked on and not at 0 hunger
</commit_message>
<xml_diff>
--- a/Production Documents/To-Do.xlsx
+++ b/Production Documents/To-Do.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmgam\Desktop\Shiva\Production Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC12BB23-80BA-4D1D-B477-89DD5EBD1FFC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E62AFA16-EBDF-4EFA-8487-EE2B46D2EE4C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{669DCC34-C837-4342-A908-0F87EB315612}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="117">
   <si>
     <t>Sprites</t>
   </si>
@@ -498,7 +498,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
@@ -522,7 +522,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="3" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -533,6 +532,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -858,7 +859,7 @@
   <dimension ref="A2:G84"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="G65" sqref="G65"/>
+      <selection activeCell="H57" sqref="H57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -877,14 +878,14 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="18" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -1070,14 +1071,14 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A16" s="28" t="s">
+      <c r="A16" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="28"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
@@ -1197,14 +1198,14 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="29" t="s">
+      <c r="A29" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="29"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="29"/>
-      <c r="F29" s="29"/>
+      <c r="B29" s="28"/>
+      <c r="C29" s="28"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="28"/>
     </row>
     <row r="30" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
@@ -1212,74 +1213,74 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="27" t="s">
+      <c r="A31" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="B31" s="27"/>
-      <c r="C31" s="27"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="27"/>
-      <c r="F31" s="27"/>
+      <c r="B31" s="29"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="29"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="27" t="s">
+      <c r="A32" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="B32" s="27"/>
-      <c r="C32" s="27"/>
-      <c r="D32" s="27"/>
-      <c r="E32" s="27"/>
-      <c r="F32" s="27"/>
+      <c r="B32" s="29"/>
+      <c r="C32" s="29"/>
+      <c r="D32" s="29"/>
+      <c r="E32" s="29"/>
+      <c r="F32" s="29"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="27" t="s">
+      <c r="A33" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="B33" s="27"/>
-      <c r="C33" s="27"/>
-      <c r="D33" s="27"/>
-      <c r="E33" s="27"/>
-      <c r="F33" s="27"/>
+      <c r="B33" s="29"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="29"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="27" t="s">
+      <c r="A34" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="B34" s="27"/>
-      <c r="C34" s="27"/>
-      <c r="D34" s="27"/>
-      <c r="E34" s="27"/>
-      <c r="F34" s="27"/>
+      <c r="B34" s="29"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="29"/>
+      <c r="E34" s="29"/>
+      <c r="F34" s="29"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="27" t="s">
+      <c r="A35" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="B35" s="27"/>
-      <c r="C35" s="27"/>
-      <c r="D35" s="27"/>
-      <c r="E35" s="27"/>
-      <c r="F35" s="27"/>
+      <c r="B35" s="29"/>
+      <c r="C35" s="29"/>
+      <c r="D35" s="29"/>
+      <c r="E35" s="29"/>
+      <c r="F35" s="29"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="27" t="s">
+      <c r="A36" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="B36" s="27"/>
-      <c r="C36" s="27"/>
-      <c r="D36" s="27"/>
-      <c r="E36" s="27"/>
-      <c r="F36" s="27"/>
+      <c r="B36" s="29"/>
+      <c r="C36" s="29"/>
+      <c r="D36" s="29"/>
+      <c r="E36" s="29"/>
+      <c r="F36" s="29"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="23" t="s">
+      <c r="A37" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="B37" s="23"/>
-      <c r="C37" s="23"/>
-      <c r="D37" s="23"/>
-      <c r="E37" s="23"/>
-      <c r="F37" s="23"/>
+      <c r="B37" s="25"/>
+      <c r="C37" s="25"/>
+      <c r="D37" s="25"/>
+      <c r="E37" s="25"/>
+      <c r="F37" s="25"/>
       <c r="G37" t="s">
         <v>115</v>
       </c>
@@ -1290,34 +1291,34 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="26" t="s">
+      <c r="A40" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="B40" s="26"/>
-      <c r="C40" s="26"/>
-      <c r="D40" s="26"/>
-      <c r="E40" s="26"/>
-      <c r="F40" s="26"/>
+      <c r="B40" s="30"/>
+      <c r="C40" s="30"/>
+      <c r="D40" s="30"/>
+      <c r="E40" s="30"/>
+      <c r="F40" s="30"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="26" t="s">
+      <c r="A41" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="B41" s="26"/>
-      <c r="C41" s="26"/>
-      <c r="D41" s="26"/>
-      <c r="E41" s="26"/>
-      <c r="F41" s="26"/>
+      <c r="B41" s="30"/>
+      <c r="C41" s="30"/>
+      <c r="D41" s="30"/>
+      <c r="E41" s="30"/>
+      <c r="F41" s="30"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="26" t="s">
+      <c r="A42" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="B42" s="26"/>
-      <c r="C42" s="26"/>
-      <c r="D42" s="26"/>
-      <c r="E42" s="26"/>
-      <c r="F42" s="26"/>
+      <c r="B42" s="30"/>
+      <c r="C42" s="30"/>
+      <c r="D42" s="30"/>
+      <c r="E42" s="30"/>
+      <c r="F42" s="30"/>
     </row>
     <row r="43" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
@@ -1328,44 +1329,44 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="27" t="s">
+      <c r="A45" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="B45" s="27"/>
-      <c r="C45" s="27"/>
-      <c r="D45" s="27"/>
-      <c r="E45" s="27"/>
-      <c r="F45" s="27"/>
+      <c r="B45" s="29"/>
+      <c r="C45" s="29"/>
+      <c r="D45" s="29"/>
+      <c r="E45" s="29"/>
+      <c r="F45" s="29"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="27" t="s">
+      <c r="A46" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="B46" s="27"/>
-      <c r="C46" s="27"/>
-      <c r="D46" s="27"/>
-      <c r="E46" s="27"/>
-      <c r="F46" s="27"/>
+      <c r="B46" s="29"/>
+      <c r="C46" s="29"/>
+      <c r="D46" s="29"/>
+      <c r="E46" s="29"/>
+      <c r="F46" s="29"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="27" t="s">
+      <c r="A47" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="B47" s="27"/>
-      <c r="C47" s="27"/>
-      <c r="D47" s="27"/>
-      <c r="E47" s="27"/>
-      <c r="F47" s="27"/>
+      <c r="B47" s="29"/>
+      <c r="C47" s="29"/>
+      <c r="D47" s="29"/>
+      <c r="E47" s="29"/>
+      <c r="F47" s="29"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="27" t="s">
+      <c r="A48" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="B48" s="27"/>
-      <c r="C48" s="27"/>
-      <c r="D48" s="27"/>
-      <c r="E48" s="27"/>
-      <c r="F48" s="27"/>
+      <c r="B48" s="29"/>
+      <c r="C48" s="29"/>
+      <c r="D48" s="29"/>
+      <c r="E48" s="29"/>
+      <c r="F48" s="29"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
@@ -1383,44 +1384,44 @@
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="27" t="s">
+      <c r="A52" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="B52" s="27"/>
-      <c r="C52" s="27"/>
-      <c r="D52" s="27"/>
-      <c r="E52" s="27"/>
-      <c r="F52" s="27"/>
+      <c r="B52" s="29"/>
+      <c r="C52" s="29"/>
+      <c r="D52" s="29"/>
+      <c r="E52" s="29"/>
+      <c r="F52" s="29"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="27" t="s">
+      <c r="A53" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="B53" s="27"/>
-      <c r="C53" s="27"/>
-      <c r="D53" s="27"/>
-      <c r="E53" s="27"/>
-      <c r="F53" s="27"/>
+      <c r="B53" s="29"/>
+      <c r="C53" s="29"/>
+      <c r="D53" s="29"/>
+      <c r="E53" s="29"/>
+      <c r="F53" s="29"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="27" t="s">
+      <c r="A54" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="B54" s="27"/>
-      <c r="C54" s="27"/>
-      <c r="D54" s="27"/>
-      <c r="E54" s="27"/>
-      <c r="F54" s="27"/>
+      <c r="B54" s="29"/>
+      <c r="C54" s="29"/>
+      <c r="D54" s="29"/>
+      <c r="E54" s="29"/>
+      <c r="F54" s="29"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="26" t="s">
+      <c r="A55" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="B55" s="26"/>
-      <c r="C55" s="26"/>
-      <c r="D55" s="26"/>
-      <c r="E55" s="26"/>
-      <c r="F55" s="26"/>
+      <c r="B55" s="30"/>
+      <c r="C55" s="30"/>
+      <c r="D55" s="30"/>
+      <c r="E55" s="30"/>
+      <c r="F55" s="30"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="13" t="s">
@@ -1438,37 +1439,34 @@
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="27" t="s">
+      <c r="A59" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="B59" s="27"/>
-      <c r="C59" s="27"/>
-      <c r="D59" s="27"/>
-      <c r="E59" s="27"/>
-      <c r="F59" s="27"/>
+      <c r="B59" s="29"/>
+      <c r="C59" s="29"/>
+      <c r="D59" s="29"/>
+      <c r="E59" s="29"/>
+      <c r="F59" s="29"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="27" t="s">
+      <c r="A60" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="B60" s="27"/>
-      <c r="C60" s="27"/>
-      <c r="D60" s="27"/>
-      <c r="E60" s="27"/>
-      <c r="F60" s="27"/>
+      <c r="B60" s="29"/>
+      <c r="C60" s="29"/>
+      <c r="D60" s="29"/>
+      <c r="E60" s="29"/>
+      <c r="F60" s="29"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="26" t="s">
+      <c r="A61" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="B61" s="26"/>
-      <c r="C61" s="26"/>
-      <c r="D61" s="26"/>
-      <c r="E61" s="26"/>
-      <c r="F61" s="26"/>
-      <c r="G61" t="s">
-        <v>115</v>
-      </c>
+      <c r="B61" s="29"/>
+      <c r="C61" s="29"/>
+      <c r="D61" s="29"/>
+      <c r="E61" s="29"/>
+      <c r="F61" s="29"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="13" t="s">
@@ -1481,14 +1479,14 @@
       <c r="F62" s="13"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="26" t="s">
+      <c r="A63" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="B63" s="26"/>
-      <c r="C63" s="26"/>
-      <c r="D63" s="26"/>
-      <c r="E63" s="26"/>
-      <c r="F63" s="26"/>
+      <c r="B63" s="30"/>
+      <c r="C63" s="30"/>
+      <c r="D63" s="30"/>
+      <c r="E63" s="30"/>
+      <c r="F63" s="30"/>
       <c r="G63" t="s">
         <v>115</v>
       </c>
@@ -1504,14 +1502,14 @@
       <c r="F64" s="18"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="25" t="s">
+      <c r="A65" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="B65" s="25"/>
-      <c r="C65" s="25"/>
-      <c r="D65" s="25"/>
-      <c r="E65" s="25"/>
-      <c r="F65" s="25"/>
+      <c r="B65" s="24"/>
+      <c r="C65" s="24"/>
+      <c r="D65" s="24"/>
+      <c r="E65" s="24"/>
+      <c r="F65" s="24"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="11" t="s">
@@ -1527,24 +1525,24 @@
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67" s="26" t="s">
+      <c r="A67" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="B67" s="26"/>
-      <c r="C67" s="26"/>
-      <c r="D67" s="26"/>
-      <c r="E67" s="26"/>
-      <c r="F67" s="26"/>
+      <c r="B67" s="30"/>
+      <c r="C67" s="30"/>
+      <c r="D67" s="30"/>
+      <c r="E67" s="30"/>
+      <c r="F67" s="30"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68" s="17" t="s">
+      <c r="A68" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="B68" s="17"/>
-      <c r="C68" s="17"/>
-      <c r="D68" s="17"/>
-      <c r="E68" s="17"/>
-      <c r="F68" s="17"/>
+      <c r="B68" s="26"/>
+      <c r="C68" s="26"/>
+      <c r="D68" s="26"/>
+      <c r="E68" s="26"/>
+      <c r="F68" s="26"/>
       <c r="G68" t="s">
         <v>115</v>
       </c>
@@ -1555,44 +1553,44 @@
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" s="26" t="s">
+      <c r="A71" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="B71" s="26"/>
-      <c r="C71" s="26"/>
-      <c r="D71" s="26"/>
-      <c r="E71" s="26"/>
-      <c r="F71" s="26"/>
+      <c r="B71" s="30"/>
+      <c r="C71" s="30"/>
+      <c r="D71" s="30"/>
+      <c r="E71" s="30"/>
+      <c r="F71" s="30"/>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" s="26" t="s">
+      <c r="A72" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="B72" s="26"/>
-      <c r="C72" s="26"/>
-      <c r="D72" s="26"/>
-      <c r="E72" s="26"/>
-      <c r="F72" s="26"/>
+      <c r="B72" s="30"/>
+      <c r="C72" s="30"/>
+      <c r="D72" s="30"/>
+      <c r="E72" s="30"/>
+      <c r="F72" s="30"/>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" s="26" t="s">
+      <c r="A73" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="B73" s="26"/>
-      <c r="C73" s="26"/>
-      <c r="D73" s="26"/>
-      <c r="E73" s="26"/>
-      <c r="F73" s="26"/>
+      <c r="B73" s="30"/>
+      <c r="C73" s="30"/>
+      <c r="D73" s="30"/>
+      <c r="E73" s="30"/>
+      <c r="F73" s="30"/>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" s="26" t="s">
+      <c r="A74" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="B74" s="26"/>
-      <c r="C74" s="26"/>
-      <c r="D74" s="26"/>
-      <c r="E74" s="26"/>
-      <c r="F74" s="26"/>
+      <c r="B74" s="30"/>
+      <c r="C74" s="30"/>
+      <c r="D74" s="30"/>
+      <c r="E74" s="30"/>
+      <c r="F74" s="30"/>
     </row>
     <row r="76" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
@@ -1630,7 +1628,7 @@
       <c r="F79" s="12"/>
     </row>
     <row r="81" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="24" t="s">
+      <c r="A81" s="23" t="s">
         <v>112</v>
       </c>
     </row>
@@ -1672,26 +1670,6 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A16:F16"/>
-    <mergeCell ref="A29:F29"/>
-    <mergeCell ref="A31:F31"/>
-    <mergeCell ref="A32:F32"/>
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="A34:F34"/>
-    <mergeCell ref="A35:F35"/>
-    <mergeCell ref="A36:F36"/>
-    <mergeCell ref="A40:F40"/>
-    <mergeCell ref="A41:F41"/>
-    <mergeCell ref="A42:F42"/>
-    <mergeCell ref="A45:F45"/>
-    <mergeCell ref="A46:F46"/>
-    <mergeCell ref="A47:F47"/>
-    <mergeCell ref="A48:F48"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="A53:F53"/>
-    <mergeCell ref="A54:F54"/>
-    <mergeCell ref="A55:F55"/>
     <mergeCell ref="A71:F71"/>
     <mergeCell ref="A72:F72"/>
     <mergeCell ref="A73:F73"/>
@@ -1701,6 +1679,26 @@
     <mergeCell ref="A61:F61"/>
     <mergeCell ref="A63:F63"/>
     <mergeCell ref="A67:F67"/>
+    <mergeCell ref="A48:F48"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="A53:F53"/>
+    <mergeCell ref="A54:F54"/>
+    <mergeCell ref="A55:F55"/>
+    <mergeCell ref="A41:F41"/>
+    <mergeCell ref="A42:F42"/>
+    <mergeCell ref="A45:F45"/>
+    <mergeCell ref="A46:F46"/>
+    <mergeCell ref="A47:F47"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A34:F34"/>
+    <mergeCell ref="A35:F35"/>
+    <mergeCell ref="A36:F36"/>
+    <mergeCell ref="A40:F40"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A29:F29"/>
+    <mergeCell ref="A31:F31"/>
+    <mergeCell ref="A32:F32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added disarm button with functionality to soldiers. Added some quality of life changes to human buttons
</commit_message>
<xml_diff>
--- a/Production Documents/To-Do.xlsx
+++ b/Production Documents/To-Do.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmgam\Desktop\Shiva\Production Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E62AFA16-EBDF-4EFA-8487-EE2B46D2EE4C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47EE2914-5868-4F3B-A582-961514FF187B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{669DCC34-C837-4342-A908-0F87EB315612}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="119">
   <si>
     <t>Sprites</t>
   </si>
@@ -232,9 +232,6 @@
     <t>When a unit lands on top of the space a popup appears telling them what they found</t>
   </si>
   <si>
-    <t>Inventory items can be placed on the board</t>
-  </si>
-  <si>
     <t>Vehicles</t>
   </si>
   <si>
@@ -331,9 +328,6 @@
     <t>Tiles with spawn pods become landing sites</t>
   </si>
   <si>
-    <t>The player starts the game with a turret outside the base, and a soldier in the base</t>
-  </si>
-  <si>
     <t>Found humans are placed on an adjacent tile to where they were found</t>
   </si>
   <si>
@@ -383,6 +377,18 @@
   </si>
   <si>
     <t>Ground units cannot move to water or mountain tiles</t>
+  </si>
+  <si>
+    <t>Change the way directional sprites are being determined so that human buttons don't get flipped</t>
+  </si>
+  <si>
+    <t>The player starts the game with two soldiers outside the base</t>
+  </si>
+  <si>
+    <t>Resources cannot be found within 2 tiles of the home base</t>
+  </si>
+  <si>
+    <t>Inventory items can be placed on the board on tiles adjacent to the home base or humans</t>
   </si>
 </sst>
 </file>
@@ -498,7 +504,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
@@ -526,14 +532,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -856,10 +864,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4D254F2-4E19-40CF-BD85-766CDBA8C5EF}">
-  <dimension ref="A2:G84"/>
+  <dimension ref="A2:G86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="H57" sqref="H57"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="G67" sqref="G67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -878,14 +886,14 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="18" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -907,12 +915,12 @@
         <v>7</v>
       </c>
       <c r="G4" s="21" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>15</v>
@@ -930,7 +938,7 @@
         <v>29</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -941,7 +949,7 @@
         <v>16</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>22</v>
@@ -953,7 +961,7 @@
         <v>30</v>
       </c>
       <c r="G6" s="19" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -976,7 +984,7 @@
         <v>31</v>
       </c>
       <c r="G7" s="19" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -995,7 +1003,7 @@
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="19" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1014,7 +1022,7 @@
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="19" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1031,7 +1039,7 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="19" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1046,7 +1054,7 @@
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="19" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1057,7 +1065,7 @@
         <v>37</v>
       </c>
       <c r="G12" s="19" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1071,14 +1079,14 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A16" s="27" t="s">
+      <c r="A16" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="27"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="31"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
@@ -1120,7 +1128,7 @@
         <v>16</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>22</v>
@@ -1198,14 +1206,14 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="28" t="s">
+      <c r="A29" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="28"/>
-      <c r="C29" s="28"/>
-      <c r="D29" s="28"/>
-      <c r="E29" s="28"/>
-      <c r="F29" s="28"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="32"/>
     </row>
     <row r="30" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
@@ -1213,68 +1221,68 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="29" t="s">
+      <c r="A31" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="B31" s="29"/>
-      <c r="C31" s="29"/>
-      <c r="D31" s="29"/>
-      <c r="E31" s="29"/>
-      <c r="F31" s="29"/>
+      <c r="B31" s="30"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="30"/>
+      <c r="F31" s="30"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="29" t="s">
+      <c r="A32" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="B32" s="29"/>
-      <c r="C32" s="29"/>
-      <c r="D32" s="29"/>
-      <c r="E32" s="29"/>
-      <c r="F32" s="29"/>
+      <c r="B32" s="30"/>
+      <c r="C32" s="30"/>
+      <c r="D32" s="30"/>
+      <c r="E32" s="30"/>
+      <c r="F32" s="30"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="29" t="s">
-        <v>73</v>
-      </c>
-      <c r="B33" s="29"/>
-      <c r="C33" s="29"/>
-      <c r="D33" s="29"/>
-      <c r="E33" s="29"/>
-      <c r="F33" s="29"/>
+      <c r="A33" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="B33" s="30"/>
+      <c r="C33" s="30"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="30"/>
+      <c r="F33" s="30"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="29" t="s">
+      <c r="A34" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="B34" s="29"/>
-      <c r="C34" s="29"/>
-      <c r="D34" s="29"/>
-      <c r="E34" s="29"/>
-      <c r="F34" s="29"/>
+      <c r="B34" s="30"/>
+      <c r="C34" s="30"/>
+      <c r="D34" s="30"/>
+      <c r="E34" s="30"/>
+      <c r="F34" s="30"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="29" t="s">
+      <c r="A35" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="B35" s="29"/>
-      <c r="C35" s="29"/>
-      <c r="D35" s="29"/>
-      <c r="E35" s="29"/>
-      <c r="F35" s="29"/>
+      <c r="B35" s="30"/>
+      <c r="C35" s="30"/>
+      <c r="D35" s="30"/>
+      <c r="E35" s="30"/>
+      <c r="F35" s="30"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="29" t="s">
+      <c r="A36" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="B36" s="29"/>
-      <c r="C36" s="29"/>
-      <c r="D36" s="29"/>
-      <c r="E36" s="29"/>
-      <c r="F36" s="29"/>
+      <c r="B36" s="30"/>
+      <c r="C36" s="30"/>
+      <c r="D36" s="30"/>
+      <c r="E36" s="30"/>
+      <c r="F36" s="30"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="25" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B37" s="25"/>
       <c r="C37" s="25"/>
@@ -1282,7 +1290,7 @@
       <c r="E37" s="25"/>
       <c r="F37" s="25"/>
       <c r="G37" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1291,34 +1299,34 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="30" t="s">
+      <c r="A40" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="B40" s="30"/>
-      <c r="C40" s="30"/>
-      <c r="D40" s="30"/>
-      <c r="E40" s="30"/>
-      <c r="F40" s="30"/>
+      <c r="B40" s="29"/>
+      <c r="C40" s="29"/>
+      <c r="D40" s="29"/>
+      <c r="E40" s="29"/>
+      <c r="F40" s="29"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="30" t="s">
+      <c r="A41" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="B41" s="30"/>
-      <c r="C41" s="30"/>
-      <c r="D41" s="30"/>
-      <c r="E41" s="30"/>
-      <c r="F41" s="30"/>
+      <c r="B41" s="29"/>
+      <c r="C41" s="29"/>
+      <c r="D41" s="29"/>
+      <c r="E41" s="29"/>
+      <c r="F41" s="29"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="30" t="s">
+      <c r="A42" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="B42" s="30"/>
-      <c r="C42" s="30"/>
-      <c r="D42" s="30"/>
-      <c r="E42" s="30"/>
-      <c r="F42" s="30"/>
+      <c r="B42" s="29"/>
+      <c r="C42" s="29"/>
+      <c r="D42" s="29"/>
+      <c r="E42" s="29"/>
+      <c r="F42" s="29"/>
     </row>
     <row r="43" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
@@ -1329,48 +1337,48 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="29" t="s">
+      <c r="A45" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="B45" s="29"/>
-      <c r="C45" s="29"/>
-      <c r="D45" s="29"/>
-      <c r="E45" s="29"/>
-      <c r="F45" s="29"/>
+      <c r="B45" s="30"/>
+      <c r="C45" s="30"/>
+      <c r="D45" s="30"/>
+      <c r="E45" s="30"/>
+      <c r="F45" s="30"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="29" t="s">
+      <c r="A46" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="B46" s="29"/>
-      <c r="C46" s="29"/>
-      <c r="D46" s="29"/>
-      <c r="E46" s="29"/>
-      <c r="F46" s="29"/>
+      <c r="B46" s="30"/>
+      <c r="C46" s="30"/>
+      <c r="D46" s="30"/>
+      <c r="E46" s="30"/>
+      <c r="F46" s="30"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="29" t="s">
+      <c r="A47" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="B47" s="29"/>
-      <c r="C47" s="29"/>
-      <c r="D47" s="29"/>
-      <c r="E47" s="29"/>
-      <c r="F47" s="29"/>
+      <c r="B47" s="30"/>
+      <c r="C47" s="30"/>
+      <c r="D47" s="30"/>
+      <c r="E47" s="30"/>
+      <c r="F47" s="30"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="29" t="s">
+      <c r="A48" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="B48" s="29"/>
-      <c r="C48" s="29"/>
-      <c r="D48" s="29"/>
-      <c r="E48" s="29"/>
-      <c r="F48" s="29"/>
+      <c r="B48" s="30"/>
+      <c r="C48" s="30"/>
+      <c r="D48" s="30"/>
+      <c r="E48" s="30"/>
+      <c r="F48" s="30"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B49" s="10"/>
       <c r="C49" s="10"/>
@@ -1384,48 +1392,48 @@
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="29" t="s">
+      <c r="A52" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="B52" s="29"/>
-      <c r="C52" s="29"/>
-      <c r="D52" s="29"/>
-      <c r="E52" s="29"/>
-      <c r="F52" s="29"/>
+      <c r="B52" s="30"/>
+      <c r="C52" s="30"/>
+      <c r="D52" s="30"/>
+      <c r="E52" s="30"/>
+      <c r="F52" s="30"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="29" t="s">
+      <c r="A53" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="B53" s="29"/>
-      <c r="C53" s="29"/>
-      <c r="D53" s="29"/>
-      <c r="E53" s="29"/>
-      <c r="F53" s="29"/>
+      <c r="B53" s="30"/>
+      <c r="C53" s="30"/>
+      <c r="D53" s="30"/>
+      <c r="E53" s="30"/>
+      <c r="F53" s="30"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="29" t="s">
+      <c r="A54" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="B54" s="29"/>
-      <c r="C54" s="29"/>
-      <c r="D54" s="29"/>
-      <c r="E54" s="29"/>
-      <c r="F54" s="29"/>
+      <c r="B54" s="30"/>
+      <c r="C54" s="30"/>
+      <c r="D54" s="30"/>
+      <c r="E54" s="30"/>
+      <c r="F54" s="30"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="30" t="s">
+      <c r="A55" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="B55" s="30"/>
-      <c r="C55" s="30"/>
-      <c r="D55" s="30"/>
-      <c r="E55" s="30"/>
-      <c r="F55" s="30"/>
+      <c r="B55" s="29"/>
+      <c r="C55" s="29"/>
+      <c r="D55" s="29"/>
+      <c r="E55" s="29"/>
+      <c r="F55" s="29"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B56" s="13"/>
       <c r="C56" s="13"/>
@@ -1439,38 +1447,38 @@
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="29" t="s">
+      <c r="A59" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="B59" s="29"/>
-      <c r="C59" s="29"/>
-      <c r="D59" s="29"/>
-      <c r="E59" s="29"/>
-      <c r="F59" s="29"/>
+      <c r="B59" s="30"/>
+      <c r="C59" s="30"/>
+      <c r="D59" s="30"/>
+      <c r="E59" s="30"/>
+      <c r="F59" s="30"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="29" t="s">
+      <c r="A60" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="B60" s="29"/>
-      <c r="C60" s="29"/>
-      <c r="D60" s="29"/>
-      <c r="E60" s="29"/>
-      <c r="F60" s="29"/>
+      <c r="B60" s="30"/>
+      <c r="C60" s="30"/>
+      <c r="D60" s="30"/>
+      <c r="E60" s="30"/>
+      <c r="F60" s="30"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="29" t="s">
-        <v>86</v>
-      </c>
-      <c r="B61" s="29"/>
-      <c r="C61" s="29"/>
-      <c r="D61" s="29"/>
-      <c r="E61" s="29"/>
-      <c r="F61" s="29"/>
+      <c r="A61" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="B61" s="30"/>
+      <c r="C61" s="30"/>
+      <c r="D61" s="30"/>
+      <c r="E61" s="30"/>
+      <c r="F61" s="30"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B62" s="13"/>
       <c r="C62" s="13"/>
@@ -1479,21 +1487,21 @@
       <c r="F62" s="13"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="B63" s="30"/>
-      <c r="C63" s="30"/>
-      <c r="D63" s="30"/>
-      <c r="E63" s="30"/>
-      <c r="F63" s="30"/>
+      <c r="A63" s="29" t="s">
+        <v>118</v>
+      </c>
+      <c r="B63" s="29"/>
+      <c r="C63" s="29"/>
+      <c r="D63" s="29"/>
+      <c r="E63" s="29"/>
+      <c r="F63" s="29"/>
       <c r="G63" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="18" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B64" s="18"/>
       <c r="C64" s="18"/>
@@ -1503,7 +1511,7 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B65" s="24"/>
       <c r="C65" s="24"/>
@@ -1512,193 +1520,210 @@
       <c r="F65" s="24"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="B66" s="11"/>
-      <c r="C66" s="11"/>
-      <c r="D66" s="11"/>
-      <c r="E66" s="11"/>
-      <c r="F66" s="11"/>
-      <c r="G66" t="s">
-        <v>115</v>
-      </c>
+      <c r="A66" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="B66" s="27"/>
+      <c r="C66" s="27"/>
+      <c r="D66" s="27"/>
+      <c r="E66" s="27"/>
+      <c r="F66" s="27"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67" s="30" t="s">
-        <v>68</v>
-      </c>
-      <c r="B67" s="30"/>
-      <c r="C67" s="30"/>
-      <c r="D67" s="30"/>
-      <c r="E67" s="30"/>
-      <c r="F67" s="30"/>
+      <c r="A67" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="B67" s="29"/>
+      <c r="C67" s="29"/>
+      <c r="D67" s="29"/>
+      <c r="E67" s="29"/>
+      <c r="F67" s="29"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="26" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B68" s="26"/>
       <c r="C68" s="26"/>
       <c r="D68" s="26"/>
       <c r="E68" s="26"/>
       <c r="F68" s="26"/>
-      <c r="G68" t="s">
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="B69" s="28"/>
+      <c r="C69" s="28"/>
+      <c r="D69" s="28"/>
+      <c r="E69" s="28"/>
+      <c r="F69" s="28"/>
+      <c r="G69" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="B72" s="29"/>
+      <c r="C72" s="29"/>
+      <c r="D72" s="29"/>
+      <c r="E72" s="29"/>
+      <c r="F72" s="29"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="B73" s="29"/>
+      <c r="C73" s="29"/>
+      <c r="D73" s="29"/>
+      <c r="E73" s="29"/>
+      <c r="F73" s="29"/>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="B74" s="29"/>
+      <c r="C74" s="29"/>
+      <c r="D74" s="29"/>
+      <c r="E74" s="29"/>
+      <c r="F74" s="29"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="B75" s="29"/>
+      <c r="C75" s="29"/>
+      <c r="D75" s="29"/>
+      <c r="E75" s="29"/>
+      <c r="F75" s="29"/>
+    </row>
+    <row r="77" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="B78" s="16"/>
+      <c r="C78" s="16"/>
+      <c r="D78" s="16"/>
+      <c r="E78" s="16"/>
+      <c r="F78" s="16"/>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="B79" s="11"/>
+      <c r="C79" s="11"/>
+      <c r="D79" s="11"/>
+      <c r="E79" s="11"/>
+      <c r="F79" s="11"/>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="B80" s="12"/>
+      <c r="C80" s="12"/>
+      <c r="D80" s="12"/>
+      <c r="E80" s="12"/>
+      <c r="F80" s="12"/>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" s="28" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" s="30" t="s">
-        <v>69</v>
-      </c>
-      <c r="B71" s="30"/>
-      <c r="C71" s="30"/>
-      <c r="D71" s="30"/>
-      <c r="E71" s="30"/>
-      <c r="F71" s="30"/>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="B72" s="30"/>
-      <c r="C72" s="30"/>
-      <c r="D72" s="30"/>
-      <c r="E72" s="30"/>
-      <c r="F72" s="30"/>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="B73" s="30"/>
-      <c r="C73" s="30"/>
-      <c r="D73" s="30"/>
-      <c r="E73" s="30"/>
-      <c r="F73" s="30"/>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="B74" s="30"/>
-      <c r="C74" s="30"/>
-      <c r="D74" s="30"/>
-      <c r="E74" s="30"/>
-      <c r="F74" s="30"/>
-    </row>
-    <row r="76" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="B77" s="16"/>
-      <c r="C77" s="16"/>
-      <c r="D77" s="16"/>
-      <c r="E77" s="16"/>
-      <c r="F77" s="16"/>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="B78" s="11"/>
-      <c r="C78" s="11"/>
-      <c r="D78" s="11"/>
-      <c r="E78" s="11"/>
-      <c r="F78" s="11"/>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="B79" s="12"/>
-      <c r="C79" s="12"/>
-      <c r="D79" s="12"/>
-      <c r="E79" s="12"/>
-      <c r="F79" s="12"/>
-    </row>
-    <row r="81" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="23" t="s">
+      <c r="B81" s="28"/>
+      <c r="C81" s="28"/>
+      <c r="D81" s="28"/>
+      <c r="E81" s="28"/>
+      <c r="F81" s="28"/>
+    </row>
+    <row r="83" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="23" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="B84" s="22"/>
+      <c r="C84" s="22"/>
+      <c r="D84" s="22"/>
+      <c r="E84" s="22"/>
+      <c r="F84" s="22"/>
+      <c r="G84" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85" s="22" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82" s="22" t="s">
+      <c r="B85" s="22"/>
+      <c r="C85" s="22"/>
+      <c r="D85" s="22"/>
+      <c r="E85" s="22"/>
+      <c r="F85" s="22"/>
+      <c r="G85" t="s">
         <v>113</v>
       </c>
-      <c r="B82" s="22"/>
-      <c r="C82" s="22"/>
-      <c r="D82" s="22"/>
-      <c r="E82" s="22"/>
-      <c r="F82" s="22"/>
-      <c r="G82" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A83" s="22" t="s">
-        <v>114</v>
-      </c>
-      <c r="B83" s="22"/>
-      <c r="C83" s="22"/>
-      <c r="D83" s="22"/>
-      <c r="E83" s="22"/>
-      <c r="F83" s="22"/>
-      <c r="G83" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="B84" s="17"/>
-      <c r="C84" s="17"/>
-      <c r="D84" s="17"/>
-      <c r="E84" s="17"/>
-      <c r="F84" s="17"/>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="B86" s="17"/>
+      <c r="C86" s="17"/>
+      <c r="D86" s="17"/>
+      <c r="E86" s="17"/>
+      <c r="F86" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="A71:F71"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A29:F29"/>
+    <mergeCell ref="A31:F31"/>
+    <mergeCell ref="A32:F32"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A34:F34"/>
+    <mergeCell ref="A35:F35"/>
+    <mergeCell ref="A36:F36"/>
+    <mergeCell ref="A40:F40"/>
+    <mergeCell ref="A41:F41"/>
+    <mergeCell ref="A42:F42"/>
+    <mergeCell ref="A45:F45"/>
+    <mergeCell ref="A46:F46"/>
+    <mergeCell ref="A47:F47"/>
+    <mergeCell ref="A48:F48"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="A53:F53"/>
+    <mergeCell ref="A54:F54"/>
+    <mergeCell ref="A55:F55"/>
     <mergeCell ref="A72:F72"/>
     <mergeCell ref="A73:F73"/>
     <mergeCell ref="A74:F74"/>
+    <mergeCell ref="A75:F75"/>
     <mergeCell ref="A59:F59"/>
     <mergeCell ref="A60:F60"/>
     <mergeCell ref="A61:F61"/>
     <mergeCell ref="A63:F63"/>
     <mergeCell ref="A67:F67"/>
-    <mergeCell ref="A48:F48"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="A53:F53"/>
-    <mergeCell ref="A54:F54"/>
-    <mergeCell ref="A55:F55"/>
-    <mergeCell ref="A41:F41"/>
-    <mergeCell ref="A42:F42"/>
-    <mergeCell ref="A45:F45"/>
-    <mergeCell ref="A46:F46"/>
-    <mergeCell ref="A47:F47"/>
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="A34:F34"/>
-    <mergeCell ref="A35:F35"/>
-    <mergeCell ref="A36:F36"/>
-    <mergeCell ref="A40:F40"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A16:F16"/>
-    <mergeCell ref="A29:F29"/>
-    <mergeCell ref="A31:F31"/>
-    <mergeCell ref="A32:F32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1726,7 +1751,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -1736,7 +1761,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B3" s="15">
         <v>0.75</v>
@@ -1744,7 +1769,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B4" s="15">
         <v>0.06</v>
@@ -1752,7 +1777,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B5" s="15">
         <v>0.08</v>
@@ -1760,7 +1785,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B6" s="15">
         <v>0.02</v>
@@ -1768,7 +1793,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B7" s="15">
         <v>0.05</v>
@@ -1776,7 +1801,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B8" s="15">
         <v>0.04</v>
@@ -1788,21 +1813,21 @@
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="J10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K10" t="s">
+        <v>91</v>
+      </c>
+      <c r="L10" t="s">
         <v>92</v>
-      </c>
-      <c r="L10" t="s">
-        <v>93</v>
       </c>
       <c r="M10" t="s">
         <v>21</v>
@@ -1816,46 +1841,46 @@
         <v>13</v>
       </c>
       <c r="J11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K11" t="s">
+        <v>93</v>
+      </c>
+      <c r="L11" t="s">
         <v>94</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" t="s">
         <v>95</v>
       </c>
-      <c r="M11" t="s">
+      <c r="N11" t="s">
         <v>96</v>
-      </c>
-      <c r="N11" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B12" s="15">
         <v>0</v>
       </c>
       <c r="J12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B13" s="15">
         <v>0</v>
       </c>
       <c r="J13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B14" s="15">
         <v>0.05</v>
@@ -1863,7 +1888,7 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B15" s="15">
         <v>0.55000000000000004</v>
@@ -1871,7 +1896,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B16" s="15">
         <v>0</v>
@@ -1879,7 +1904,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B17" s="15">
         <v>0.4</v>
@@ -1898,7 +1923,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B21" s="15">
         <v>0.3</v>
@@ -1906,7 +1931,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B22" s="15">
         <v>0.2</v>
@@ -1914,7 +1939,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B23" s="15">
         <v>0.15</v>
@@ -1922,7 +1947,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B24" s="15">
         <v>0.05</v>
@@ -1930,7 +1955,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B25" s="15">
         <v>0.2</v>
@@ -1938,7 +1963,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B26" s="15">
         <v>0.1</v>
@@ -1957,7 +1982,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B30" s="15">
         <v>0</v>
@@ -1965,7 +1990,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B31" s="15">
         <v>0.3</v>
@@ -1973,7 +1998,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B32" s="15">
         <v>0.15</v>
@@ -1981,7 +2006,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B33" s="15">
         <v>0.1</v>
@@ -1989,7 +2014,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B34" s="15">
         <v>0.3</v>
@@ -1997,7 +2022,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B35" s="15">
         <v>0.15</v>
@@ -2016,7 +2041,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B39" s="15">
         <v>0</v>
@@ -2024,7 +2049,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B40" s="15">
         <v>0.2</v>
@@ -2032,7 +2057,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B41" s="15">
         <v>0.25</v>
@@ -2040,7 +2065,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B42" s="15">
         <v>0.25</v>
@@ -2048,7 +2073,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B43" s="15">
         <v>0.05</v>
@@ -2056,7 +2081,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B44" s="15">
         <v>0.25</v>

</xml_diff>

<commit_message>
Added a global list keeping track of the tiles within the macro variable SAFE_RADIUS to the home base. Currently the list is used to set the surrounding area to 'explored'. This will also be used in the future to determine where buildings can be placed. Also fixed a couple bugs that came up when calcTargets started avoiding water and mountain tiles
</commit_message>
<xml_diff>
--- a/Production Documents/To-Do.xlsx
+++ b/Production Documents/To-Do.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmgam\Desktop\Shiva\Production Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47EE2914-5868-4F3B-A582-961514FF187B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{350E26E2-F3AF-41BB-A1D2-DC0AF8802499}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{669DCC34-C837-4342-A908-0F87EB315612}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="119">
   <si>
     <t>Sprites</t>
   </si>
@@ -530,10 +530,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="3" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
@@ -542,6 +540,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -866,8 +866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4D254F2-4E19-40CF-BD85-766CDBA8C5EF}">
   <dimension ref="A2:G86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="G67" sqref="G67"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -886,14 +886,14 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="18" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -1079,14 +1079,14 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A16" s="31" t="s">
+      <c r="A16" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="31"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="31"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
@@ -1206,14 +1206,14 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="32" t="s">
+      <c r="A29" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="32"/>
-      <c r="C29" s="32"/>
-      <c r="D29" s="32"/>
-      <c r="E29" s="32"/>
-      <c r="F29" s="32"/>
+      <c r="B29" s="30"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="30"/>
     </row>
     <row r="30" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
@@ -1221,160 +1221,157 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="30" t="s">
+      <c r="A31" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="B31" s="30"/>
-      <c r="C31" s="30"/>
-      <c r="D31" s="30"/>
-      <c r="E31" s="30"/>
-      <c r="F31" s="30"/>
+      <c r="B31" s="31"/>
+      <c r="C31" s="31"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="31"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="30" t="s">
+      <c r="A32" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="B32" s="30"/>
-      <c r="C32" s="30"/>
-      <c r="D32" s="30"/>
-      <c r="E32" s="30"/>
-      <c r="F32" s="30"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="30" t="s">
+      <c r="B32" s="31"/>
+      <c r="C32" s="31"/>
+      <c r="D32" s="31"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="31"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="B33" s="30"/>
-      <c r="C33" s="30"/>
-      <c r="D33" s="30"/>
-      <c r="E33" s="30"/>
-      <c r="F33" s="30"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="30" t="s">
+      <c r="B33" s="31"/>
+      <c r="C33" s="31"/>
+      <c r="D33" s="31"/>
+      <c r="E33" s="31"/>
+      <c r="F33" s="31"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="B34" s="30"/>
-      <c r="C34" s="30"/>
-      <c r="D34" s="30"/>
-      <c r="E34" s="30"/>
-      <c r="F34" s="30"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="30" t="s">
+      <c r="B34" s="31"/>
+      <c r="C34" s="31"/>
+      <c r="D34" s="31"/>
+      <c r="E34" s="31"/>
+      <c r="F34" s="31"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="B35" s="30"/>
-      <c r="C35" s="30"/>
-      <c r="D35" s="30"/>
-      <c r="E35" s="30"/>
-      <c r="F35" s="30"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="30" t="s">
+      <c r="B35" s="31"/>
+      <c r="C35" s="31"/>
+      <c r="D35" s="31"/>
+      <c r="E35" s="31"/>
+      <c r="F35" s="31"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="B36" s="30"/>
-      <c r="C36" s="30"/>
-      <c r="D36" s="30"/>
-      <c r="E36" s="30"/>
-      <c r="F36" s="30"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="25" t="s">
+      <c r="B36" s="31"/>
+      <c r="C36" s="31"/>
+      <c r="D36" s="31"/>
+      <c r="E36" s="31"/>
+      <c r="F36" s="31"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="28" t="s">
         <v>114</v>
       </c>
-      <c r="B37" s="25"/>
-      <c r="C37" s="25"/>
-      <c r="D37" s="25"/>
-      <c r="E37" s="25"/>
-      <c r="F37" s="25"/>
-      <c r="G37" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="28"/>
+      <c r="C37" s="28"/>
+      <c r="D37" s="28"/>
+      <c r="E37" s="28"/>
+      <c r="F37" s="28"/>
+    </row>
+    <row r="39" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="29" t="s">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="B40" s="29"/>
-      <c r="C40" s="29"/>
-      <c r="D40" s="29"/>
-      <c r="E40" s="29"/>
-      <c r="F40" s="29"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="29" t="s">
+      <c r="B40" s="32"/>
+      <c r="C40" s="32"/>
+      <c r="D40" s="32"/>
+      <c r="E40" s="32"/>
+      <c r="F40" s="32"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="B41" s="29"/>
-      <c r="C41" s="29"/>
-      <c r="D41" s="29"/>
-      <c r="E41" s="29"/>
-      <c r="F41" s="29"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="29" t="s">
+      <c r="B41" s="32"/>
+      <c r="C41" s="32"/>
+      <c r="D41" s="32"/>
+      <c r="E41" s="32"/>
+      <c r="F41" s="32"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="B42" s="29"/>
-      <c r="C42" s="29"/>
-      <c r="D42" s="29"/>
-      <c r="E42" s="29"/>
-      <c r="F42" s="29"/>
-    </row>
-    <row r="43" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="32"/>
+      <c r="C42" s="32"/>
+      <c r="D42" s="32"/>
+      <c r="E42" s="32"/>
+      <c r="F42" s="32"/>
+    </row>
+    <row r="43" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
     </row>
-    <row r="44" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="30" t="s">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="B45" s="30"/>
-      <c r="C45" s="30"/>
-      <c r="D45" s="30"/>
-      <c r="E45" s="30"/>
-      <c r="F45" s="30"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="30" t="s">
+      <c r="B45" s="31"/>
+      <c r="C45" s="31"/>
+      <c r="D45" s="31"/>
+      <c r="E45" s="31"/>
+      <c r="F45" s="31"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="B46" s="30"/>
-      <c r="C46" s="30"/>
-      <c r="D46" s="30"/>
-      <c r="E46" s="30"/>
-      <c r="F46" s="30"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="30" t="s">
+      <c r="B46" s="31"/>
+      <c r="C46" s="31"/>
+      <c r="D46" s="31"/>
+      <c r="E46" s="31"/>
+      <c r="F46" s="31"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="B47" s="30"/>
-      <c r="C47" s="30"/>
-      <c r="D47" s="30"/>
-      <c r="E47" s="30"/>
-      <c r="F47" s="30"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="30" t="s">
+      <c r="B47" s="31"/>
+      <c r="C47" s="31"/>
+      <c r="D47" s="31"/>
+      <c r="E47" s="31"/>
+      <c r="F47" s="31"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="B48" s="30"/>
-      <c r="C48" s="30"/>
-      <c r="D48" s="30"/>
-      <c r="E48" s="30"/>
-      <c r="F48" s="30"/>
+      <c r="B48" s="31"/>
+      <c r="C48" s="31"/>
+      <c r="D48" s="31"/>
+      <c r="E48" s="31"/>
+      <c r="F48" s="31"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
@@ -1392,44 +1389,44 @@
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="30" t="s">
+      <c r="A52" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="B52" s="30"/>
-      <c r="C52" s="30"/>
-      <c r="D52" s="30"/>
-      <c r="E52" s="30"/>
-      <c r="F52" s="30"/>
+      <c r="B52" s="31"/>
+      <c r="C52" s="31"/>
+      <c r="D52" s="31"/>
+      <c r="E52" s="31"/>
+      <c r="F52" s="31"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="30" t="s">
+      <c r="A53" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="B53" s="30"/>
-      <c r="C53" s="30"/>
-      <c r="D53" s="30"/>
-      <c r="E53" s="30"/>
-      <c r="F53" s="30"/>
+      <c r="B53" s="31"/>
+      <c r="C53" s="31"/>
+      <c r="D53" s="31"/>
+      <c r="E53" s="31"/>
+      <c r="F53" s="31"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="30" t="s">
+      <c r="A54" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="B54" s="30"/>
-      <c r="C54" s="30"/>
-      <c r="D54" s="30"/>
-      <c r="E54" s="30"/>
-      <c r="F54" s="30"/>
+      <c r="B54" s="31"/>
+      <c r="C54" s="31"/>
+      <c r="D54" s="31"/>
+      <c r="E54" s="31"/>
+      <c r="F54" s="31"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="29" t="s">
+      <c r="A55" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="B55" s="29"/>
-      <c r="C55" s="29"/>
-      <c r="D55" s="29"/>
-      <c r="E55" s="29"/>
-      <c r="F55" s="29"/>
+      <c r="B55" s="32"/>
+      <c r="C55" s="32"/>
+      <c r="D55" s="32"/>
+      <c r="E55" s="32"/>
+      <c r="F55" s="32"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="13" t="s">
@@ -1447,34 +1444,34 @@
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="30" t="s">
+      <c r="A59" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="B59" s="30"/>
-      <c r="C59" s="30"/>
-      <c r="D59" s="30"/>
-      <c r="E59" s="30"/>
-      <c r="F59" s="30"/>
+      <c r="B59" s="31"/>
+      <c r="C59" s="31"/>
+      <c r="D59" s="31"/>
+      <c r="E59" s="31"/>
+      <c r="F59" s="31"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="30" t="s">
+      <c r="A60" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="B60" s="30"/>
-      <c r="C60" s="30"/>
-      <c r="D60" s="30"/>
-      <c r="E60" s="30"/>
-      <c r="F60" s="30"/>
+      <c r="B60" s="31"/>
+      <c r="C60" s="31"/>
+      <c r="D60" s="31"/>
+      <c r="E60" s="31"/>
+      <c r="F60" s="31"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="30" t="s">
+      <c r="A61" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="B61" s="30"/>
-      <c r="C61" s="30"/>
-      <c r="D61" s="30"/>
-      <c r="E61" s="30"/>
-      <c r="F61" s="30"/>
+      <c r="B61" s="31"/>
+      <c r="C61" s="31"/>
+      <c r="D61" s="31"/>
+      <c r="E61" s="31"/>
+      <c r="F61" s="31"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="13" t="s">
@@ -1487,14 +1484,14 @@
       <c r="F62" s="13"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="29" t="s">
+      <c r="A63" s="32" t="s">
         <v>118</v>
       </c>
-      <c r="B63" s="29"/>
-      <c r="C63" s="29"/>
-      <c r="D63" s="29"/>
-      <c r="E63" s="29"/>
-      <c r="F63" s="29"/>
+      <c r="B63" s="32"/>
+      <c r="C63" s="32"/>
+      <c r="D63" s="32"/>
+      <c r="E63" s="32"/>
+      <c r="F63" s="32"/>
       <c r="G63" t="s">
         <v>113</v>
       </c>
@@ -1509,7 +1506,7 @@
       <c r="E64" s="18"/>
       <c r="F64" s="18"/>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="24" t="s">
         <v>82</v>
       </c>
@@ -1519,37 +1516,37 @@
       <c r="E65" s="24"/>
       <c r="F65" s="24"/>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="27" t="s">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="B66" s="27"/>
-      <c r="C66" s="27"/>
-      <c r="D66" s="27"/>
-      <c r="E66" s="27"/>
-      <c r="F66" s="27"/>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67" s="29" t="s">
+      <c r="B66" s="26"/>
+      <c r="C66" s="26"/>
+      <c r="D66" s="26"/>
+      <c r="E66" s="26"/>
+      <c r="F66" s="26"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="B67" s="29"/>
-      <c r="C67" s="29"/>
-      <c r="D67" s="29"/>
-      <c r="E67" s="29"/>
-      <c r="F67" s="29"/>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68" s="26" t="s">
+      <c r="B67" s="32"/>
+      <c r="C67" s="32"/>
+      <c r="D67" s="32"/>
+      <c r="E67" s="32"/>
+      <c r="F67" s="32"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="B68" s="26"/>
-      <c r="C68" s="26"/>
-      <c r="D68" s="26"/>
-      <c r="E68" s="26"/>
-      <c r="F68" s="26"/>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B68" s="25"/>
+      <c r="C68" s="25"/>
+      <c r="D68" s="25"/>
+      <c r="E68" s="25"/>
+      <c r="F68" s="25"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="28" t="s">
         <v>117</v>
       </c>
@@ -1558,61 +1555,58 @@
       <c r="D69" s="28"/>
       <c r="E69" s="28"/>
       <c r="F69" s="28"/>
-      <c r="G69" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="71" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" s="29" t="s">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="B72" s="29"/>
-      <c r="C72" s="29"/>
-      <c r="D72" s="29"/>
-      <c r="E72" s="29"/>
-      <c r="F72" s="29"/>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" s="29" t="s">
+      <c r="B72" s="32"/>
+      <c r="C72" s="32"/>
+      <c r="D72" s="32"/>
+      <c r="E72" s="32"/>
+      <c r="F72" s="32"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="B73" s="29"/>
-      <c r="C73" s="29"/>
-      <c r="D73" s="29"/>
-      <c r="E73" s="29"/>
-      <c r="F73" s="29"/>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" s="29" t="s">
+      <c r="B73" s="32"/>
+      <c r="C73" s="32"/>
+      <c r="D73" s="32"/>
+      <c r="E73" s="32"/>
+      <c r="F73" s="32"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="B74" s="29"/>
-      <c r="C74" s="29"/>
-      <c r="D74" s="29"/>
-      <c r="E74" s="29"/>
-      <c r="F74" s="29"/>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75" s="29" t="s">
+      <c r="B74" s="32"/>
+      <c r="C74" s="32"/>
+      <c r="D74" s="32"/>
+      <c r="E74" s="32"/>
+      <c r="F74" s="32"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="B75" s="29"/>
-      <c r="C75" s="29"/>
-      <c r="D75" s="29"/>
-      <c r="E75" s="29"/>
-      <c r="F75" s="29"/>
-    </row>
-    <row r="77" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B75" s="32"/>
+      <c r="C75" s="32"/>
+      <c r="D75" s="32"/>
+      <c r="E75" s="32"/>
+      <c r="F75" s="32"/>
+    </row>
+    <row r="77" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="16" t="s">
         <v>78</v>
       </c>
@@ -1622,7 +1616,7 @@
       <c r="E78" s="16"/>
       <c r="F78" s="16"/>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="11" t="s">
         <v>97</v>
       </c>
@@ -1632,7 +1626,7 @@
       <c r="E79" s="11"/>
       <c r="F79" s="11"/>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="12" t="s">
         <v>116</v>
       </c>
@@ -1643,14 +1637,14 @@
       <c r="F80" s="12"/>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" s="28" t="s">
+      <c r="A81" s="27" t="s">
         <v>115</v>
       </c>
-      <c r="B81" s="28"/>
-      <c r="C81" s="28"/>
-      <c r="D81" s="28"/>
-      <c r="E81" s="28"/>
-      <c r="F81" s="28"/>
+      <c r="B81" s="27"/>
+      <c r="C81" s="27"/>
+      <c r="D81" s="27"/>
+      <c r="E81" s="27"/>
+      <c r="F81" s="27"/>
     </row>
     <row r="83" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="23" t="s">
@@ -1695,26 +1689,6 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A16:F16"/>
-    <mergeCell ref="A29:F29"/>
-    <mergeCell ref="A31:F31"/>
-    <mergeCell ref="A32:F32"/>
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="A34:F34"/>
-    <mergeCell ref="A35:F35"/>
-    <mergeCell ref="A36:F36"/>
-    <mergeCell ref="A40:F40"/>
-    <mergeCell ref="A41:F41"/>
-    <mergeCell ref="A42:F42"/>
-    <mergeCell ref="A45:F45"/>
-    <mergeCell ref="A46:F46"/>
-    <mergeCell ref="A47:F47"/>
-    <mergeCell ref="A48:F48"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="A53:F53"/>
-    <mergeCell ref="A54:F54"/>
-    <mergeCell ref="A55:F55"/>
     <mergeCell ref="A72:F72"/>
     <mergeCell ref="A73:F73"/>
     <mergeCell ref="A74:F74"/>
@@ -1724,6 +1698,26 @@
     <mergeCell ref="A61:F61"/>
     <mergeCell ref="A63:F63"/>
     <mergeCell ref="A67:F67"/>
+    <mergeCell ref="A48:F48"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="A53:F53"/>
+    <mergeCell ref="A54:F54"/>
+    <mergeCell ref="A55:F55"/>
+    <mergeCell ref="A41:F41"/>
+    <mergeCell ref="A42:F42"/>
+    <mergeCell ref="A45:F45"/>
+    <mergeCell ref="A46:F46"/>
+    <mergeCell ref="A47:F47"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A34:F34"/>
+    <mergeCell ref="A35:F35"/>
+    <mergeCell ref="A36:F36"/>
+    <mergeCell ref="A40:F40"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A29:F29"/>
+    <mergeCell ref="A31:F31"/>
+    <mergeCell ref="A32:F32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Spawning 2 soldiers on random tiles in the global.homeBaseNearbyTiles list at the start of the game
</commit_message>
<xml_diff>
--- a/Production Documents/To-Do.xlsx
+++ b/Production Documents/To-Do.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmgam\Desktop\Shiva\Production Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{350E26E2-F3AF-41BB-A1D2-DC0AF8802499}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{937AACA8-ECCC-433A-A978-949871D842F9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{669DCC34-C837-4342-A908-0F87EB315612}"/>
   </bookViews>
@@ -517,7 +517,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -534,14 +533,15 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -866,8 +866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4D254F2-4E19-40CF-BD85-766CDBA8C5EF}">
   <dimension ref="A2:G86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="G77" sqref="G77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -886,14 +886,14 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="18" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -914,7 +914,7 @@
       <c r="F4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="21" t="s">
+      <c r="G4" s="20" t="s">
         <v>101</v>
       </c>
     </row>
@@ -937,7 +937,7 @@
       <c r="F5" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="G5" s="18" t="s">
         <v>102</v>
       </c>
     </row>
@@ -960,7 +960,7 @@
       <c r="F6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="19" t="s">
+      <c r="G6" s="18" t="s">
         <v>103</v>
       </c>
     </row>
@@ -983,7 +983,7 @@
       <c r="F7" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="19" t="s">
+      <c r="G7" s="18" t="s">
         <v>104</v>
       </c>
     </row>
@@ -1002,7 +1002,7 @@
         <v>27</v>
       </c>
       <c r="F8" s="4"/>
-      <c r="G8" s="19" t="s">
+      <c r="G8" s="18" t="s">
         <v>105</v>
       </c>
     </row>
@@ -1021,7 +1021,7 @@
         <v>28</v>
       </c>
       <c r="F9" s="4"/>
-      <c r="G9" s="19" t="s">
+      <c r="G9" s="18" t="s">
         <v>106</v>
       </c>
     </row>
@@ -1038,7 +1038,7 @@
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
-      <c r="G10" s="19" t="s">
+      <c r="G10" s="18" t="s">
         <v>107</v>
       </c>
     </row>
@@ -1053,7 +1053,7 @@
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
-      <c r="G11" s="19" t="s">
+      <c r="G11" s="18" t="s">
         <v>108</v>
       </c>
     </row>
@@ -1064,7 +1064,7 @@
       <c r="C12" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="G12" s="19" t="s">
+      <c r="G12" s="18" t="s">
         <v>109</v>
       </c>
     </row>
@@ -1079,14 +1079,14 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="29"/>
-      <c r="C16" s="29"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="31"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
@@ -1154,7 +1154,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="19" t="s">
         <v>18</v>
       </c>
       <c r="C21" s="3" t="s">
@@ -1164,7 +1164,7 @@
       <c r="F21" s="4"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="20" t="s">
+      <c r="B22" s="19" t="s">
         <v>19</v>
       </c>
       <c r="C22" s="9" t="s">
@@ -1175,7 +1175,7 @@
       <c r="F22" s="4"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="20" t="s">
+      <c r="B23" s="19" t="s">
         <v>20</v>
       </c>
       <c r="C23" s="3" t="s">
@@ -1206,14 +1206,14 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="30" t="s">
+      <c r="A29" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="30"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="30"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="32"/>
     </row>
     <row r="30" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
@@ -1221,74 +1221,74 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="31" t="s">
+      <c r="A31" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="B31" s="31"/>
-      <c r="C31" s="31"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="31"/>
-      <c r="F31" s="31"/>
+      <c r="B31" s="30"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="30"/>
+      <c r="F31" s="30"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="31" t="s">
+      <c r="A32" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="B32" s="31"/>
-      <c r="C32" s="31"/>
-      <c r="D32" s="31"/>
-      <c r="E32" s="31"/>
-      <c r="F32" s="31"/>
+      <c r="B32" s="30"/>
+      <c r="C32" s="30"/>
+      <c r="D32" s="30"/>
+      <c r="E32" s="30"/>
+      <c r="F32" s="30"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="31" t="s">
+      <c r="A33" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="B33" s="31"/>
-      <c r="C33" s="31"/>
-      <c r="D33" s="31"/>
-      <c r="E33" s="31"/>
-      <c r="F33" s="31"/>
+      <c r="B33" s="30"/>
+      <c r="C33" s="30"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="30"/>
+      <c r="F33" s="30"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="31" t="s">
+      <c r="A34" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="B34" s="31"/>
-      <c r="C34" s="31"/>
-      <c r="D34" s="31"/>
-      <c r="E34" s="31"/>
-      <c r="F34" s="31"/>
+      <c r="B34" s="30"/>
+      <c r="C34" s="30"/>
+      <c r="D34" s="30"/>
+      <c r="E34" s="30"/>
+      <c r="F34" s="30"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="31" t="s">
+      <c r="A35" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="B35" s="31"/>
-      <c r="C35" s="31"/>
-      <c r="D35" s="31"/>
-      <c r="E35" s="31"/>
-      <c r="F35" s="31"/>
+      <c r="B35" s="30"/>
+      <c r="C35" s="30"/>
+      <c r="D35" s="30"/>
+      <c r="E35" s="30"/>
+      <c r="F35" s="30"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="31" t="s">
+      <c r="A36" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="B36" s="31"/>
-      <c r="C36" s="31"/>
-      <c r="D36" s="31"/>
-      <c r="E36" s="31"/>
-      <c r="F36" s="31"/>
+      <c r="B36" s="30"/>
+      <c r="C36" s="30"/>
+      <c r="D36" s="30"/>
+      <c r="E36" s="30"/>
+      <c r="F36" s="30"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="28" t="s">
+      <c r="A37" s="27" t="s">
         <v>114</v>
       </c>
-      <c r="B37" s="28"/>
-      <c r="C37" s="28"/>
-      <c r="D37" s="28"/>
-      <c r="E37" s="28"/>
-      <c r="F37" s="28"/>
+      <c r="B37" s="27"/>
+      <c r="C37" s="27"/>
+      <c r="D37" s="27"/>
+      <c r="E37" s="27"/>
+      <c r="F37" s="27"/>
     </row>
     <row r="39" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
@@ -1296,34 +1296,34 @@
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="32" t="s">
+      <c r="A40" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="B40" s="32"/>
-      <c r="C40" s="32"/>
-      <c r="D40" s="32"/>
-      <c r="E40" s="32"/>
-      <c r="F40" s="32"/>
+      <c r="B40" s="29"/>
+      <c r="C40" s="29"/>
+      <c r="D40" s="29"/>
+      <c r="E40" s="29"/>
+      <c r="F40" s="29"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="32" t="s">
+      <c r="A41" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="B41" s="32"/>
-      <c r="C41" s="32"/>
-      <c r="D41" s="32"/>
-      <c r="E41" s="32"/>
-      <c r="F41" s="32"/>
+      <c r="B41" s="29"/>
+      <c r="C41" s="29"/>
+      <c r="D41" s="29"/>
+      <c r="E41" s="29"/>
+      <c r="F41" s="29"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="32" t="s">
+      <c r="A42" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="B42" s="32"/>
-      <c r="C42" s="32"/>
-      <c r="D42" s="32"/>
-      <c r="E42" s="32"/>
-      <c r="F42" s="32"/>
+      <c r="B42" s="29"/>
+      <c r="C42" s="29"/>
+      <c r="D42" s="29"/>
+      <c r="E42" s="29"/>
+      <c r="F42" s="29"/>
     </row>
     <row r="43" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
@@ -1334,44 +1334,44 @@
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="31" t="s">
+      <c r="A45" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="B45" s="31"/>
-      <c r="C45" s="31"/>
-      <c r="D45" s="31"/>
-      <c r="E45" s="31"/>
-      <c r="F45" s="31"/>
+      <c r="B45" s="30"/>
+      <c r="C45" s="30"/>
+      <c r="D45" s="30"/>
+      <c r="E45" s="30"/>
+      <c r="F45" s="30"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="31" t="s">
+      <c r="A46" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="B46" s="31"/>
-      <c r="C46" s="31"/>
-      <c r="D46" s="31"/>
-      <c r="E46" s="31"/>
-      <c r="F46" s="31"/>
+      <c r="B46" s="30"/>
+      <c r="C46" s="30"/>
+      <c r="D46" s="30"/>
+      <c r="E46" s="30"/>
+      <c r="F46" s="30"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="31" t="s">
+      <c r="A47" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="B47" s="31"/>
-      <c r="C47" s="31"/>
-      <c r="D47" s="31"/>
-      <c r="E47" s="31"/>
-      <c r="F47" s="31"/>
+      <c r="B47" s="30"/>
+      <c r="C47" s="30"/>
+      <c r="D47" s="30"/>
+      <c r="E47" s="30"/>
+      <c r="F47" s="30"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="31" t="s">
+      <c r="A48" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="B48" s="31"/>
-      <c r="C48" s="31"/>
-      <c r="D48" s="31"/>
-      <c r="E48" s="31"/>
-      <c r="F48" s="31"/>
+      <c r="B48" s="30"/>
+      <c r="C48" s="30"/>
+      <c r="D48" s="30"/>
+      <c r="E48" s="30"/>
+      <c r="F48" s="30"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
@@ -1389,54 +1389,54 @@
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="31" t="s">
+      <c r="A52" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="B52" s="31"/>
-      <c r="C52" s="31"/>
-      <c r="D52" s="31"/>
-      <c r="E52" s="31"/>
-      <c r="F52" s="31"/>
+      <c r="B52" s="30"/>
+      <c r="C52" s="30"/>
+      <c r="D52" s="30"/>
+      <c r="E52" s="30"/>
+      <c r="F52" s="30"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="31" t="s">
+      <c r="A53" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="B53" s="31"/>
-      <c r="C53" s="31"/>
-      <c r="D53" s="31"/>
-      <c r="E53" s="31"/>
-      <c r="F53" s="31"/>
+      <c r="B53" s="30"/>
+      <c r="C53" s="30"/>
+      <c r="D53" s="30"/>
+      <c r="E53" s="30"/>
+      <c r="F53" s="30"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="31" t="s">
+      <c r="A54" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="B54" s="31"/>
-      <c r="C54" s="31"/>
-      <c r="D54" s="31"/>
-      <c r="E54" s="31"/>
-      <c r="F54" s="31"/>
+      <c r="B54" s="30"/>
+      <c r="C54" s="30"/>
+      <c r="D54" s="30"/>
+      <c r="E54" s="30"/>
+      <c r="F54" s="30"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="32" t="s">
+      <c r="A55" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="B55" s="32"/>
-      <c r="C55" s="32"/>
-      <c r="D55" s="32"/>
-      <c r="E55" s="32"/>
-      <c r="F55" s="32"/>
+      <c r="B55" s="29"/>
+      <c r="C55" s="29"/>
+      <c r="D55" s="29"/>
+      <c r="E55" s="29"/>
+      <c r="F55" s="29"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="13" t="s">
+      <c r="A56" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="B56" s="13"/>
-      <c r="C56" s="13"/>
-      <c r="D56" s="13"/>
-      <c r="E56" s="13"/>
-      <c r="F56" s="13"/>
+      <c r="B56" s="12"/>
+      <c r="C56" s="12"/>
+      <c r="D56" s="12"/>
+      <c r="E56" s="12"/>
+      <c r="F56" s="12"/>
     </row>
     <row r="58" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
@@ -1444,117 +1444,117 @@
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="31" t="s">
+      <c r="A59" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="B59" s="31"/>
-      <c r="C59" s="31"/>
-      <c r="D59" s="31"/>
-      <c r="E59" s="31"/>
-      <c r="F59" s="31"/>
+      <c r="B59" s="30"/>
+      <c r="C59" s="30"/>
+      <c r="D59" s="30"/>
+      <c r="E59" s="30"/>
+      <c r="F59" s="30"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="31" t="s">
+      <c r="A60" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="B60" s="31"/>
-      <c r="C60" s="31"/>
-      <c r="D60" s="31"/>
-      <c r="E60" s="31"/>
-      <c r="F60" s="31"/>
+      <c r="B60" s="30"/>
+      <c r="C60" s="30"/>
+      <c r="D60" s="30"/>
+      <c r="E60" s="30"/>
+      <c r="F60" s="30"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="31" t="s">
+      <c r="A61" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="B61" s="31"/>
-      <c r="C61" s="31"/>
-      <c r="D61" s="31"/>
-      <c r="E61" s="31"/>
-      <c r="F61" s="31"/>
+      <c r="B61" s="30"/>
+      <c r="C61" s="30"/>
+      <c r="D61" s="30"/>
+      <c r="E61" s="30"/>
+      <c r="F61" s="30"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="13" t="s">
+      <c r="A62" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="B62" s="13"/>
-      <c r="C62" s="13"/>
-      <c r="D62" s="13"/>
-      <c r="E62" s="13"/>
-      <c r="F62" s="13"/>
+      <c r="B62" s="12"/>
+      <c r="C62" s="12"/>
+      <c r="D62" s="12"/>
+      <c r="E62" s="12"/>
+      <c r="F62" s="12"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="32" t="s">
+      <c r="A63" s="29" t="s">
         <v>118</v>
       </c>
-      <c r="B63" s="32"/>
-      <c r="C63" s="32"/>
-      <c r="D63" s="32"/>
-      <c r="E63" s="32"/>
-      <c r="F63" s="32"/>
+      <c r="B63" s="29"/>
+      <c r="C63" s="29"/>
+      <c r="D63" s="29"/>
+      <c r="E63" s="29"/>
+      <c r="F63" s="29"/>
       <c r="G63" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="18" t="s">
+      <c r="A64" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="B64" s="18"/>
-      <c r="C64" s="18"/>
-      <c r="D64" s="18"/>
-      <c r="E64" s="18"/>
-      <c r="F64" s="18"/>
+      <c r="B64" s="17"/>
+      <c r="C64" s="17"/>
+      <c r="D64" s="17"/>
+      <c r="E64" s="17"/>
+      <c r="F64" s="17"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="24" t="s">
+      <c r="A65" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="B65" s="24"/>
-      <c r="C65" s="24"/>
-      <c r="D65" s="24"/>
-      <c r="E65" s="24"/>
-      <c r="F65" s="24"/>
+      <c r="B65" s="23"/>
+      <c r="C65" s="23"/>
+      <c r="D65" s="23"/>
+      <c r="E65" s="23"/>
+      <c r="F65" s="23"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="26" t="s">
+      <c r="A66" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="B66" s="26"/>
-      <c r="C66" s="26"/>
-      <c r="D66" s="26"/>
-      <c r="E66" s="26"/>
-      <c r="F66" s="26"/>
+      <c r="B66" s="25"/>
+      <c r="C66" s="25"/>
+      <c r="D66" s="25"/>
+      <c r="E66" s="25"/>
+      <c r="F66" s="25"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="32" t="s">
+      <c r="A67" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="B67" s="32"/>
-      <c r="C67" s="32"/>
-      <c r="D67" s="32"/>
-      <c r="E67" s="32"/>
-      <c r="F67" s="32"/>
+      <c r="B67" s="29"/>
+      <c r="C67" s="29"/>
+      <c r="D67" s="29"/>
+      <c r="E67" s="29"/>
+      <c r="F67" s="29"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="25" t="s">
+      <c r="A68" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="B68" s="25"/>
-      <c r="C68" s="25"/>
-      <c r="D68" s="25"/>
-      <c r="E68" s="25"/>
-      <c r="F68" s="25"/>
+      <c r="B68" s="24"/>
+      <c r="C68" s="24"/>
+      <c r="D68" s="24"/>
+      <c r="E68" s="24"/>
+      <c r="F68" s="24"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="28" t="s">
+      <c r="A69" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="B69" s="28"/>
-      <c r="C69" s="28"/>
-      <c r="D69" s="28"/>
-      <c r="E69" s="28"/>
-      <c r="F69" s="28"/>
+      <c r="B69" s="27"/>
+      <c r="C69" s="27"/>
+      <c r="D69" s="27"/>
+      <c r="E69" s="27"/>
+      <c r="F69" s="27"/>
     </row>
     <row r="71" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
@@ -1562,44 +1562,44 @@
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="32" t="s">
+      <c r="A72" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="B72" s="32"/>
-      <c r="C72" s="32"/>
-      <c r="D72" s="32"/>
-      <c r="E72" s="32"/>
-      <c r="F72" s="32"/>
+      <c r="B72" s="29"/>
+      <c r="C72" s="29"/>
+      <c r="D72" s="29"/>
+      <c r="E72" s="29"/>
+      <c r="F72" s="29"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="32" t="s">
+      <c r="A73" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="B73" s="32"/>
-      <c r="C73" s="32"/>
-      <c r="D73" s="32"/>
-      <c r="E73" s="32"/>
-      <c r="F73" s="32"/>
+      <c r="B73" s="29"/>
+      <c r="C73" s="29"/>
+      <c r="D73" s="29"/>
+      <c r="E73" s="29"/>
+      <c r="F73" s="29"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="32" t="s">
+      <c r="A74" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="B74" s="32"/>
-      <c r="C74" s="32"/>
-      <c r="D74" s="32"/>
-      <c r="E74" s="32"/>
-      <c r="F74" s="32"/>
+      <c r="B74" s="29"/>
+      <c r="C74" s="29"/>
+      <c r="D74" s="29"/>
+      <c r="E74" s="29"/>
+      <c r="F74" s="29"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="32" t="s">
+      <c r="A75" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="B75" s="32"/>
-      <c r="C75" s="32"/>
-      <c r="D75" s="32"/>
-      <c r="E75" s="32"/>
-      <c r="F75" s="32"/>
+      <c r="B75" s="29"/>
+      <c r="C75" s="29"/>
+      <c r="D75" s="29"/>
+      <c r="E75" s="29"/>
+      <c r="F75" s="29"/>
     </row>
     <row r="77" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
@@ -1607,14 +1607,14 @@
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="16" t="s">
+      <c r="A78" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="B78" s="16"/>
-      <c r="C78" s="16"/>
-      <c r="D78" s="16"/>
-      <c r="E78" s="16"/>
-      <c r="F78" s="16"/>
+      <c r="B78" s="15"/>
+      <c r="C78" s="15"/>
+      <c r="D78" s="15"/>
+      <c r="E78" s="15"/>
+      <c r="F78" s="15"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="11" t="s">
@@ -1627,68 +1627,88 @@
       <c r="F79" s="11"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="12" t="s">
+      <c r="A80" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="B80" s="12"/>
-      <c r="C80" s="12"/>
-      <c r="D80" s="12"/>
-      <c r="E80" s="12"/>
-      <c r="F80" s="12"/>
+      <c r="B80" s="28"/>
+      <c r="C80" s="28"/>
+      <c r="D80" s="28"/>
+      <c r="E80" s="28"/>
+      <c r="F80" s="28"/>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" s="27" t="s">
+      <c r="A81" s="26" t="s">
         <v>115</v>
       </c>
-      <c r="B81" s="27"/>
-      <c r="C81" s="27"/>
-      <c r="D81" s="27"/>
-      <c r="E81" s="27"/>
-      <c r="F81" s="27"/>
+      <c r="B81" s="26"/>
+      <c r="C81" s="26"/>
+      <c r="D81" s="26"/>
+      <c r="E81" s="26"/>
+      <c r="F81" s="26"/>
     </row>
     <row r="83" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="23" t="s">
+      <c r="A83" s="22" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84" s="22" t="s">
+      <c r="A84" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="B84" s="22"/>
-      <c r="C84" s="22"/>
-      <c r="D84" s="22"/>
-      <c r="E84" s="22"/>
-      <c r="F84" s="22"/>
+      <c r="B84" s="21"/>
+      <c r="C84" s="21"/>
+      <c r="D84" s="21"/>
+      <c r="E84" s="21"/>
+      <c r="F84" s="21"/>
       <c r="G84" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A85" s="22" t="s">
+      <c r="A85" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="B85" s="22"/>
-      <c r="C85" s="22"/>
-      <c r="D85" s="22"/>
-      <c r="E85" s="22"/>
-      <c r="F85" s="22"/>
+      <c r="B85" s="21"/>
+      <c r="C85" s="21"/>
+      <c r="D85" s="21"/>
+      <c r="E85" s="21"/>
+      <c r="F85" s="21"/>
       <c r="G85" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A86" s="17" t="s">
+      <c r="A86" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="B86" s="17"/>
-      <c r="C86" s="17"/>
-      <c r="D86" s="17"/>
-      <c r="E86" s="17"/>
-      <c r="F86" s="17"/>
+      <c r="B86" s="16"/>
+      <c r="C86" s="16"/>
+      <c r="D86" s="16"/>
+      <c r="E86" s="16"/>
+      <c r="F86" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A29:F29"/>
+    <mergeCell ref="A31:F31"/>
+    <mergeCell ref="A32:F32"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A34:F34"/>
+    <mergeCell ref="A35:F35"/>
+    <mergeCell ref="A36:F36"/>
+    <mergeCell ref="A40:F40"/>
+    <mergeCell ref="A41:F41"/>
+    <mergeCell ref="A42:F42"/>
+    <mergeCell ref="A45:F45"/>
+    <mergeCell ref="A46:F46"/>
+    <mergeCell ref="A47:F47"/>
+    <mergeCell ref="A48:F48"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="A53:F53"/>
+    <mergeCell ref="A54:F54"/>
+    <mergeCell ref="A55:F55"/>
     <mergeCell ref="A72:F72"/>
     <mergeCell ref="A73:F73"/>
     <mergeCell ref="A74:F74"/>
@@ -1698,26 +1718,6 @@
     <mergeCell ref="A61:F61"/>
     <mergeCell ref="A63:F63"/>
     <mergeCell ref="A67:F67"/>
-    <mergeCell ref="A48:F48"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="A53:F53"/>
-    <mergeCell ref="A54:F54"/>
-    <mergeCell ref="A55:F55"/>
-    <mergeCell ref="A41:F41"/>
-    <mergeCell ref="A42:F42"/>
-    <mergeCell ref="A45:F45"/>
-    <mergeCell ref="A46:F46"/>
-    <mergeCell ref="A47:F47"/>
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="A34:F34"/>
-    <mergeCell ref="A35:F35"/>
-    <mergeCell ref="A36:F36"/>
-    <mergeCell ref="A40:F40"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A16:F16"/>
-    <mergeCell ref="A29:F29"/>
-    <mergeCell ref="A31:F31"/>
-    <mergeCell ref="A32:F32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1744,12 +1744,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1757,7 +1757,7 @@
       <c r="A3" t="s">
         <v>81</v>
       </c>
-      <c r="B3" s="15">
+      <c r="B3" s="14">
         <v>0.75</v>
       </c>
     </row>
@@ -1765,7 +1765,7 @@
       <c r="A4" t="s">
         <v>87</v>
       </c>
-      <c r="B4" s="15">
+      <c r="B4" s="14">
         <v>0.06</v>
       </c>
     </row>
@@ -1773,7 +1773,7 @@
       <c r="A5" t="s">
         <v>88</v>
       </c>
-      <c r="B5" s="15">
+      <c r="B5" s="14">
         <v>0.08</v>
       </c>
     </row>
@@ -1781,7 +1781,7 @@
       <c r="A6" t="s">
         <v>89</v>
       </c>
-      <c r="B6" s="15">
+      <c r="B6" s="14">
         <v>0.02</v>
       </c>
     </row>
@@ -1789,7 +1789,7 @@
       <c r="A7" t="s">
         <v>80</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="14">
         <v>0.05</v>
       </c>
     </row>
@@ -1797,12 +1797,12 @@
       <c r="A8" t="s">
         <v>90</v>
       </c>
-      <c r="B8" s="15">
+      <c r="B8" s="14">
         <v>0.04</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="15">
+      <c r="B9" s="14">
         <f>SUM(B3:B8)</f>
         <v>1</v>
       </c>
@@ -1831,7 +1831,7 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="13" t="s">
         <v>13</v>
       </c>
       <c r="J11" t="s">
@@ -1854,7 +1854,7 @@
       <c r="A12" t="s">
         <v>81</v>
       </c>
-      <c r="B12" s="15">
+      <c r="B12" s="14">
         <v>0</v>
       </c>
       <c r="J12" t="s">
@@ -1865,7 +1865,7 @@
       <c r="A13" t="s">
         <v>87</v>
       </c>
-      <c r="B13" s="15">
+      <c r="B13" s="14">
         <v>0</v>
       </c>
       <c r="J13" t="s">
@@ -1876,7 +1876,7 @@
       <c r="A14" t="s">
         <v>88</v>
       </c>
-      <c r="B14" s="15">
+      <c r="B14" s="14">
         <v>0.05</v>
       </c>
     </row>
@@ -1884,7 +1884,7 @@
       <c r="A15" t="s">
         <v>89</v>
       </c>
-      <c r="B15" s="15">
+      <c r="B15" s="14">
         <v>0.55000000000000004</v>
       </c>
     </row>
@@ -1892,7 +1892,7 @@
       <c r="A16" t="s">
         <v>80</v>
       </c>
-      <c r="B16" s="15">
+      <c r="B16" s="14">
         <v>0</v>
       </c>
     </row>
@@ -1900,18 +1900,18 @@
       <c r="A17" t="s">
         <v>90</v>
       </c>
-      <c r="B17" s="15">
+      <c r="B17" s="14">
         <v>0.4</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="15">
+      <c r="B18" s="14">
         <f>SUM(B12:B17)</f>
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="13" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1919,7 +1919,7 @@
       <c r="A21" t="s">
         <v>81</v>
       </c>
-      <c r="B21" s="15">
+      <c r="B21" s="14">
         <v>0.3</v>
       </c>
     </row>
@@ -1927,7 +1927,7 @@
       <c r="A22" t="s">
         <v>87</v>
       </c>
-      <c r="B22" s="15">
+      <c r="B22" s="14">
         <v>0.2</v>
       </c>
     </row>
@@ -1935,7 +1935,7 @@
       <c r="A23" t="s">
         <v>88</v>
       </c>
-      <c r="B23" s="15">
+      <c r="B23" s="14">
         <v>0.15</v>
       </c>
     </row>
@@ -1943,7 +1943,7 @@
       <c r="A24" t="s">
         <v>89</v>
       </c>
-      <c r="B24" s="15">
+      <c r="B24" s="14">
         <v>0.05</v>
       </c>
     </row>
@@ -1951,7 +1951,7 @@
       <c r="A25" t="s">
         <v>80</v>
       </c>
-      <c r="B25" s="15">
+      <c r="B25" s="14">
         <v>0.2</v>
       </c>
     </row>
@@ -1959,18 +1959,18 @@
       <c r="A26" t="s">
         <v>90</v>
       </c>
-      <c r="B26" s="15">
+      <c r="B26" s="14">
         <v>0.1</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B27" s="15">
+      <c r="B27" s="14">
         <f>SUM(B21:B26)</f>
         <v>1.0000000000000002</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="14" t="s">
+      <c r="A29" s="13" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1978,7 +1978,7 @@
       <c r="A30" t="s">
         <v>81</v>
       </c>
-      <c r="B30" s="15">
+      <c r="B30" s="14">
         <v>0</v>
       </c>
     </row>
@@ -1986,7 +1986,7 @@
       <c r="A31" t="s">
         <v>87</v>
       </c>
-      <c r="B31" s="15">
+      <c r="B31" s="14">
         <v>0.3</v>
       </c>
     </row>
@@ -1994,7 +1994,7 @@
       <c r="A32" t="s">
         <v>88</v>
       </c>
-      <c r="B32" s="15">
+      <c r="B32" s="14">
         <v>0.15</v>
       </c>
     </row>
@@ -2002,7 +2002,7 @@
       <c r="A33" t="s">
         <v>89</v>
       </c>
-      <c r="B33" s="15">
+      <c r="B33" s="14">
         <v>0.1</v>
       </c>
     </row>
@@ -2010,7 +2010,7 @@
       <c r="A34" t="s">
         <v>80</v>
       </c>
-      <c r="B34" s="15">
+      <c r="B34" s="14">
         <v>0.3</v>
       </c>
     </row>
@@ -2018,18 +2018,18 @@
       <c r="A35" t="s">
         <v>90</v>
       </c>
-      <c r="B35" s="15">
+      <c r="B35" s="14">
         <v>0.15</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B36" s="15">
+      <c r="B36" s="14">
         <f>SUM(B30:B35)</f>
         <v>0.99999999999999989</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="14" t="s">
+      <c r="A38" s="13" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2037,7 +2037,7 @@
       <c r="A39" t="s">
         <v>81</v>
       </c>
-      <c r="B39" s="15">
+      <c r="B39" s="14">
         <v>0</v>
       </c>
     </row>
@@ -2045,7 +2045,7 @@
       <c r="A40" t="s">
         <v>87</v>
       </c>
-      <c r="B40" s="15">
+      <c r="B40" s="14">
         <v>0.2</v>
       </c>
     </row>
@@ -2053,7 +2053,7 @@
       <c r="A41" t="s">
         <v>88</v>
       </c>
-      <c r="B41" s="15">
+      <c r="B41" s="14">
         <v>0.25</v>
       </c>
     </row>
@@ -2061,7 +2061,7 @@
       <c r="A42" t="s">
         <v>89</v>
       </c>
-      <c r="B42" s="15">
+      <c r="B42" s="14">
         <v>0.25</v>
       </c>
     </row>
@@ -2069,7 +2069,7 @@
       <c r="A43" t="s">
         <v>80</v>
       </c>
-      <c r="B43" s="15">
+      <c r="B43" s="14">
         <v>0.05</v>
       </c>
     </row>
@@ -2077,12 +2077,12 @@
       <c r="A44" t="s">
         <v>90</v>
       </c>
-      <c r="B44" s="15">
+      <c r="B44" s="14">
         <v>0.25</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B45" s="15">
+      <c r="B45" s="14">
         <f>SUM(B39:B44)</f>
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
removed a test script I addcidently left in the last commit
</commit_message>
<xml_diff>
--- a/Production Documents/To-Do.xlsx
+++ b/Production Documents/To-Do.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmgam\Desktop\Shiva\Production Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18ACBBC2-90C5-49C0-A79F-ECEFA2190A20}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7940FB70-7D0C-46EF-ACD5-D1FFBE09FF42}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{669DCC34-C837-4342-A908-0F87EB315612}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="122">
   <si>
     <t>Sprites</t>
   </si>
@@ -395,6 +395,9 @@
   </si>
   <si>
     <t>Zoom in and out using the mouse wheel</t>
+  </si>
+  <si>
+    <t>Loading screen while the board is being generated</t>
   </si>
 </sst>
 </file>
@@ -510,7 +513,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
@@ -544,13 +547,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -873,10 +877,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4D254F2-4E19-40CF-BD85-766CDBA8C5EF}">
-  <dimension ref="A2:G87"/>
+  <dimension ref="A2:G88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G85" sqref="G85"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="J74" sqref="J74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -895,14 +899,14 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="18" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -1091,14 +1095,14 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A16" s="34" t="s">
+      <c r="A16" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="34"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
@@ -1218,14 +1222,14 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="35" t="s">
+      <c r="A29" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="35"/>
-      <c r="C29" s="35"/>
-      <c r="D29" s="35"/>
-      <c r="E29" s="35"/>
-      <c r="F29" s="35"/>
+      <c r="B29" s="34"/>
+      <c r="C29" s="34"/>
+      <c r="D29" s="34"/>
+      <c r="E29" s="34"/>
+      <c r="F29" s="34"/>
     </row>
     <row r="30" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
@@ -1233,64 +1237,64 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="33" t="s">
+      <c r="A31" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="B31" s="33"/>
-      <c r="C31" s="33"/>
-      <c r="D31" s="33"/>
-      <c r="E31" s="33"/>
-      <c r="F31" s="33"/>
+      <c r="B31" s="35"/>
+      <c r="C31" s="35"/>
+      <c r="D31" s="35"/>
+      <c r="E31" s="35"/>
+      <c r="F31" s="35"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="33" t="s">
+      <c r="A32" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="B32" s="33"/>
-      <c r="C32" s="33"/>
-      <c r="D32" s="33"/>
-      <c r="E32" s="33"/>
-      <c r="F32" s="33"/>
+      <c r="B32" s="35"/>
+      <c r="C32" s="35"/>
+      <c r="D32" s="35"/>
+      <c r="E32" s="35"/>
+      <c r="F32" s="35"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="33" t="s">
+      <c r="A33" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="B33" s="33"/>
-      <c r="C33" s="33"/>
-      <c r="D33" s="33"/>
-      <c r="E33" s="33"/>
-      <c r="F33" s="33"/>
+      <c r="B33" s="35"/>
+      <c r="C33" s="35"/>
+      <c r="D33" s="35"/>
+      <c r="E33" s="35"/>
+      <c r="F33" s="35"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="33" t="s">
+      <c r="A34" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="B34" s="33"/>
-      <c r="C34" s="33"/>
-      <c r="D34" s="33"/>
-      <c r="E34" s="33"/>
-      <c r="F34" s="33"/>
+      <c r="B34" s="35"/>
+      <c r="C34" s="35"/>
+      <c r="D34" s="35"/>
+      <c r="E34" s="35"/>
+      <c r="F34" s="35"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="33" t="s">
+      <c r="A35" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="B35" s="33"/>
-      <c r="C35" s="33"/>
-      <c r="D35" s="33"/>
-      <c r="E35" s="33"/>
-      <c r="F35" s="33"/>
+      <c r="B35" s="35"/>
+      <c r="C35" s="35"/>
+      <c r="D35" s="35"/>
+      <c r="E35" s="35"/>
+      <c r="F35" s="35"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="33" t="s">
+      <c r="A36" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="B36" s="33"/>
-      <c r="C36" s="33"/>
-      <c r="D36" s="33"/>
-      <c r="E36" s="33"/>
-      <c r="F36" s="33"/>
+      <c r="B36" s="35"/>
+      <c r="C36" s="35"/>
+      <c r="D36" s="35"/>
+      <c r="E36" s="35"/>
+      <c r="F36" s="35"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="26" t="s">
@@ -1308,34 +1312,34 @@
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="32" t="s">
+      <c r="A40" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="B40" s="32"/>
-      <c r="C40" s="32"/>
-      <c r="D40" s="32"/>
-      <c r="E40" s="32"/>
-      <c r="F40" s="32"/>
+      <c r="B40" s="36"/>
+      <c r="C40" s="36"/>
+      <c r="D40" s="36"/>
+      <c r="E40" s="36"/>
+      <c r="F40" s="36"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="32" t="s">
+      <c r="A41" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="B41" s="32"/>
-      <c r="C41" s="32"/>
-      <c r="D41" s="32"/>
-      <c r="E41" s="32"/>
-      <c r="F41" s="32"/>
+      <c r="B41" s="36"/>
+      <c r="C41" s="36"/>
+      <c r="D41" s="36"/>
+      <c r="E41" s="36"/>
+      <c r="F41" s="36"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="32" t="s">
+      <c r="A42" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="B42" s="32"/>
-      <c r="C42" s="32"/>
-      <c r="D42" s="32"/>
-      <c r="E42" s="32"/>
-      <c r="F42" s="32"/>
+      <c r="B42" s="36"/>
+      <c r="C42" s="36"/>
+      <c r="D42" s="36"/>
+      <c r="E42" s="36"/>
+      <c r="F42" s="36"/>
     </row>
     <row r="43" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
@@ -1346,44 +1350,44 @@
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="33" t="s">
+      <c r="A45" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="B45" s="33"/>
-      <c r="C45" s="33"/>
-      <c r="D45" s="33"/>
-      <c r="E45" s="33"/>
-      <c r="F45" s="33"/>
+      <c r="B45" s="35"/>
+      <c r="C45" s="35"/>
+      <c r="D45" s="35"/>
+      <c r="E45" s="35"/>
+      <c r="F45" s="35"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="33" t="s">
+      <c r="A46" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="B46" s="33"/>
-      <c r="C46" s="33"/>
-      <c r="D46" s="33"/>
-      <c r="E46" s="33"/>
-      <c r="F46" s="33"/>
+      <c r="B46" s="35"/>
+      <c r="C46" s="35"/>
+      <c r="D46" s="35"/>
+      <c r="E46" s="35"/>
+      <c r="F46" s="35"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="33" t="s">
+      <c r="A47" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="B47" s="33"/>
-      <c r="C47" s="33"/>
-      <c r="D47" s="33"/>
-      <c r="E47" s="33"/>
-      <c r="F47" s="33"/>
+      <c r="B47" s="35"/>
+      <c r="C47" s="35"/>
+      <c r="D47" s="35"/>
+      <c r="E47" s="35"/>
+      <c r="F47" s="35"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="33" t="s">
+      <c r="A48" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="B48" s="33"/>
-      <c r="C48" s="33"/>
-      <c r="D48" s="33"/>
-      <c r="E48" s="33"/>
-      <c r="F48" s="33"/>
+      <c r="B48" s="35"/>
+      <c r="C48" s="35"/>
+      <c r="D48" s="35"/>
+      <c r="E48" s="35"/>
+      <c r="F48" s="35"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
@@ -1401,44 +1405,44 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="33" t="s">
+      <c r="A52" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="B52" s="33"/>
-      <c r="C52" s="33"/>
-      <c r="D52" s="33"/>
-      <c r="E52" s="33"/>
-      <c r="F52" s="33"/>
+      <c r="B52" s="35"/>
+      <c r="C52" s="35"/>
+      <c r="D52" s="35"/>
+      <c r="E52" s="35"/>
+      <c r="F52" s="35"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="33" t="s">
+      <c r="A53" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="B53" s="33"/>
-      <c r="C53" s="33"/>
-      <c r="D53" s="33"/>
-      <c r="E53" s="33"/>
-      <c r="F53" s="33"/>
+      <c r="B53" s="35"/>
+      <c r="C53" s="35"/>
+      <c r="D53" s="35"/>
+      <c r="E53" s="35"/>
+      <c r="F53" s="35"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="33" t="s">
+      <c r="A54" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="B54" s="33"/>
-      <c r="C54" s="33"/>
-      <c r="D54" s="33"/>
-      <c r="E54" s="33"/>
-      <c r="F54" s="33"/>
+      <c r="B54" s="35"/>
+      <c r="C54" s="35"/>
+      <c r="D54" s="35"/>
+      <c r="E54" s="35"/>
+      <c r="F54" s="35"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="32" t="s">
+      <c r="A55" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="B55" s="32"/>
-      <c r="C55" s="32"/>
-      <c r="D55" s="32"/>
-      <c r="E55" s="32"/>
-      <c r="F55" s="32"/>
+      <c r="B55" s="36"/>
+      <c r="C55" s="36"/>
+      <c r="D55" s="36"/>
+      <c r="E55" s="36"/>
+      <c r="F55" s="36"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="12" t="s">
@@ -1456,34 +1460,34 @@
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="33" t="s">
+      <c r="A59" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="B59" s="33"/>
-      <c r="C59" s="33"/>
-      <c r="D59" s="33"/>
-      <c r="E59" s="33"/>
-      <c r="F59" s="33"/>
+      <c r="B59" s="35"/>
+      <c r="C59" s="35"/>
+      <c r="D59" s="35"/>
+      <c r="E59" s="35"/>
+      <c r="F59" s="35"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="33" t="s">
+      <c r="A60" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="B60" s="33"/>
-      <c r="C60" s="33"/>
-      <c r="D60" s="33"/>
-      <c r="E60" s="33"/>
-      <c r="F60" s="33"/>
+      <c r="B60" s="35"/>
+      <c r="C60" s="35"/>
+      <c r="D60" s="35"/>
+      <c r="E60" s="35"/>
+      <c r="F60" s="35"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="33" t="s">
+      <c r="A61" s="35" t="s">
         <v>85</v>
       </c>
-      <c r="B61" s="33"/>
-      <c r="C61" s="33"/>
-      <c r="D61" s="33"/>
-      <c r="E61" s="33"/>
-      <c r="F61" s="33"/>
+      <c r="B61" s="35"/>
+      <c r="C61" s="35"/>
+      <c r="D61" s="35"/>
+      <c r="E61" s="35"/>
+      <c r="F61" s="35"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="12" t="s">
@@ -1496,14 +1500,14 @@
       <c r="F62" s="12"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="32" t="s">
+      <c r="A63" s="36" t="s">
         <v>118</v>
       </c>
-      <c r="B63" s="32"/>
-      <c r="C63" s="32"/>
-      <c r="D63" s="32"/>
-      <c r="E63" s="32"/>
-      <c r="F63" s="32"/>
+      <c r="B63" s="36"/>
+      <c r="C63" s="36"/>
+      <c r="D63" s="36"/>
+      <c r="E63" s="36"/>
+      <c r="F63" s="36"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="17" t="s">
@@ -1536,14 +1540,14 @@
       <c r="F66" s="25"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="32" t="s">
+      <c r="A67" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="B67" s="32"/>
-      <c r="C67" s="32"/>
-      <c r="D67" s="32"/>
-      <c r="E67" s="32"/>
-      <c r="F67" s="32"/>
+      <c r="B67" s="36"/>
+      <c r="C67" s="36"/>
+      <c r="D67" s="36"/>
+      <c r="E67" s="36"/>
+      <c r="F67" s="36"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="24" t="s">
@@ -1571,44 +1575,44 @@
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="32" t="s">
+      <c r="A72" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="B72" s="32"/>
-      <c r="C72" s="32"/>
-      <c r="D72" s="32"/>
-      <c r="E72" s="32"/>
-      <c r="F72" s="32"/>
+      <c r="B72" s="36"/>
+      <c r="C72" s="36"/>
+      <c r="D72" s="36"/>
+      <c r="E72" s="36"/>
+      <c r="F72" s="36"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="32" t="s">
+      <c r="A73" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="B73" s="32"/>
-      <c r="C73" s="32"/>
-      <c r="D73" s="32"/>
-      <c r="E73" s="32"/>
-      <c r="F73" s="32"/>
+      <c r="B73" s="36"/>
+      <c r="C73" s="36"/>
+      <c r="D73" s="36"/>
+      <c r="E73" s="36"/>
+      <c r="F73" s="36"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="32" t="s">
+      <c r="A74" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="B74" s="32"/>
-      <c r="C74" s="32"/>
-      <c r="D74" s="32"/>
-      <c r="E74" s="32"/>
-      <c r="F74" s="32"/>
+      <c r="B74" s="36"/>
+      <c r="C74" s="36"/>
+      <c r="D74" s="36"/>
+      <c r="E74" s="36"/>
+      <c r="F74" s="36"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="32" t="s">
+      <c r="A75" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="B75" s="32"/>
-      <c r="C75" s="32"/>
-      <c r="D75" s="32"/>
-      <c r="E75" s="32"/>
-      <c r="F75" s="32"/>
+      <c r="B75" s="36"/>
+      <c r="C75" s="36"/>
+      <c r="D75" s="36"/>
+      <c r="E75" s="36"/>
+      <c r="F75" s="36"/>
     </row>
     <row r="77" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
@@ -1706,28 +1710,18 @@
       <c r="E87" s="31"/>
       <c r="F87" s="31"/>
     </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="B88" s="32"/>
+      <c r="C88" s="32"/>
+      <c r="D88" s="32"/>
+      <c r="E88" s="32"/>
+      <c r="F88" s="32"/>
+    </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A16:F16"/>
-    <mergeCell ref="A29:F29"/>
-    <mergeCell ref="A31:F31"/>
-    <mergeCell ref="A32:F32"/>
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="A34:F34"/>
-    <mergeCell ref="A35:F35"/>
-    <mergeCell ref="A36:F36"/>
-    <mergeCell ref="A40:F40"/>
-    <mergeCell ref="A41:F41"/>
-    <mergeCell ref="A42:F42"/>
-    <mergeCell ref="A45:F45"/>
-    <mergeCell ref="A46:F46"/>
-    <mergeCell ref="A47:F47"/>
-    <mergeCell ref="A48:F48"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="A53:F53"/>
-    <mergeCell ref="A54:F54"/>
-    <mergeCell ref="A55:F55"/>
     <mergeCell ref="A72:F72"/>
     <mergeCell ref="A73:F73"/>
     <mergeCell ref="A74:F74"/>
@@ -1737,6 +1731,26 @@
     <mergeCell ref="A61:F61"/>
     <mergeCell ref="A63:F63"/>
     <mergeCell ref="A67:F67"/>
+    <mergeCell ref="A48:F48"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="A53:F53"/>
+    <mergeCell ref="A54:F54"/>
+    <mergeCell ref="A55:F55"/>
+    <mergeCell ref="A41:F41"/>
+    <mergeCell ref="A42:F42"/>
+    <mergeCell ref="A45:F45"/>
+    <mergeCell ref="A46:F46"/>
+    <mergeCell ref="A47:F47"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A34:F34"/>
+    <mergeCell ref="A35:F35"/>
+    <mergeCell ref="A36:F36"/>
+    <mergeCell ref="A40:F40"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A29:F29"/>
+    <mergeCell ref="A31:F31"/>
+    <mergeCell ref="A32:F32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated todo list to be ready for next submittal
</commit_message>
<xml_diff>
--- a/Production Documents/To-Do.xlsx
+++ b/Production Documents/To-Do.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmgam\Desktop\Shiva\Production Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Shiva\Production Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7940FB70-7D0C-46EF-ACD5-D1FFBE09FF42}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88C96DE8-35A7-4C31-9A3E-B72F8DD39A4F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{669DCC34-C837-4342-A908-0F87EB315612}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{669DCC34-C837-4342-A908-0F87EB315612}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="123">
   <si>
     <t>Sprites</t>
   </si>
@@ -398,6 +398,9 @@
   </si>
   <si>
     <t>Loading screen while the board is being generated</t>
+  </si>
+  <si>
+    <t>Title Screen</t>
   </si>
 </sst>
 </file>
@@ -513,7 +516,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
@@ -547,14 +550,15 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -877,38 +881,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4D254F2-4E19-40CF-BD85-766CDBA8C5EF}">
-  <dimension ref="A2:G88"/>
+  <dimension ref="A2:G89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H48" sqref="H48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="18" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="33" t="s">
+    <row r="3" spans="1:7" ht="18" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-    </row>
-    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+    </row>
+    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -931,7 +935,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>73</v>
       </c>
@@ -954,7 +958,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -977,7 +981,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
@@ -1000,7 +1004,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
@@ -1019,7 +1023,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
@@ -1038,7 +1042,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
@@ -1055,7 +1059,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="28" t="s">
         <v>13</v>
       </c>
@@ -1070,7 +1074,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
@@ -1081,7 +1085,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="29" t="s">
         <v>119</v>
       </c>
@@ -1089,22 +1093,22 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C14" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A16" s="33" t="s">
+    <row r="16" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A16" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="33"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
-    </row>
-    <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="36"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+    </row>
+    <row r="17" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
         <v>3</v>
@@ -1122,7 +1126,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B18" s="8" t="s">
         <v>15</v>
       </c>
@@ -1139,7 +1143,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
@@ -1154,7 +1158,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
@@ -1169,7 +1173,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B21" s="19" t="s">
         <v>18</v>
       </c>
@@ -1179,7 +1183,7 @@
       <c r="D21" s="4"/>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B22" s="19" t="s">
         <v>19</v>
       </c>
@@ -1190,7 +1194,7 @@
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B23" s="19" t="s">
         <v>20</v>
       </c>
@@ -1201,42 +1205,42 @@
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C24" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C25" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C26" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C27" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="34" t="s">
+    <row r="29" spans="1:6" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A29" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="34"/>
-      <c r="C29" s="34"/>
-      <c r="D29" s="34"/>
-      <c r="E29" s="34"/>
-      <c r="F29" s="34"/>
-    </row>
-    <row r="30" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="37"/>
+      <c r="C29" s="37"/>
+      <c r="D29" s="37"/>
+      <c r="E29" s="37"/>
+      <c r="F29" s="37"/>
+    </row>
+    <row r="30" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="35" t="s">
         <v>44</v>
       </c>
@@ -1246,7 +1250,7 @@
       <c r="E31" s="35"/>
       <c r="F31" s="35"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="35" t="s">
         <v>45</v>
       </c>
@@ -1256,7 +1260,7 @@
       <c r="E32" s="35"/>
       <c r="F32" s="35"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="35" t="s">
         <v>72</v>
       </c>
@@ -1266,7 +1270,7 @@
       <c r="E33" s="35"/>
       <c r="F33" s="35"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="35" t="s">
         <v>46</v>
       </c>
@@ -1276,7 +1280,7 @@
       <c r="E34" s="35"/>
       <c r="F34" s="35"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="35" t="s">
         <v>47</v>
       </c>
@@ -1286,7 +1290,7 @@
       <c r="E35" s="35"/>
       <c r="F35" s="35"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="35" t="s">
         <v>48</v>
       </c>
@@ -1296,7 +1300,7 @@
       <c r="E36" s="35"/>
       <c r="F36" s="35"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="26" t="s">
         <v>114</v>
       </c>
@@ -1306,50 +1310,53 @@
       <c r="E37" s="26"/>
       <c r="F37" s="26"/>
     </row>
-    <row r="39" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="36" t="s">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="B40" s="36"/>
-      <c r="C40" s="36"/>
-      <c r="D40" s="36"/>
-      <c r="E40" s="36"/>
-      <c r="F40" s="36"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="36" t="s">
+      <c r="B40" s="34"/>
+      <c r="C40" s="34"/>
+      <c r="D40" s="34"/>
+      <c r="E40" s="34"/>
+      <c r="F40" s="34"/>
+      <c r="G40" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="B41" s="36"/>
-      <c r="C41" s="36"/>
-      <c r="D41" s="36"/>
-      <c r="E41" s="36"/>
-      <c r="F41" s="36"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="36" t="s">
+      <c r="B41" s="34"/>
+      <c r="C41" s="34"/>
+      <c r="D41" s="34"/>
+      <c r="E41" s="34"/>
+      <c r="F41" s="34"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="B42" s="36"/>
-      <c r="C42" s="36"/>
-      <c r="D42" s="36"/>
-      <c r="E42" s="36"/>
-      <c r="F42" s="36"/>
-    </row>
-    <row r="43" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="34"/>
+      <c r="C42" s="34"/>
+      <c r="D42" s="34"/>
+      <c r="E42" s="34"/>
+      <c r="F42" s="34"/>
+    </row>
+    <row r="43" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="1"/>
     </row>
-    <row r="44" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="35" t="s">
         <v>49</v>
       </c>
@@ -1359,7 +1366,7 @@
       <c r="E45" s="35"/>
       <c r="F45" s="35"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="35" t="s">
         <v>50</v>
       </c>
@@ -1369,7 +1376,7 @@
       <c r="E46" s="35"/>
       <c r="F46" s="35"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="35" t="s">
         <v>52</v>
       </c>
@@ -1379,7 +1386,7 @@
       <c r="E47" s="35"/>
       <c r="F47" s="35"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="35" t="s">
         <v>53</v>
       </c>
@@ -1389,7 +1396,7 @@
       <c r="E48" s="35"/>
       <c r="F48" s="35"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="10" t="s">
         <v>75</v>
       </c>
@@ -1398,13 +1405,16 @@
       <c r="D49" s="10"/>
       <c r="E49" s="10"/>
       <c r="F49" s="10"/>
-    </row>
-    <row r="51" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G49" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="35" t="s">
         <v>55</v>
       </c>
@@ -1414,7 +1424,7 @@
       <c r="E52" s="35"/>
       <c r="F52" s="35"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="35" t="s">
         <v>56</v>
       </c>
@@ -1424,7 +1434,7 @@
       <c r="E53" s="35"/>
       <c r="F53" s="35"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="35" t="s">
         <v>57</v>
       </c>
@@ -1434,17 +1444,17 @@
       <c r="E54" s="35"/>
       <c r="F54" s="35"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="36" t="s">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A55" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="B55" s="36"/>
-      <c r="C55" s="36"/>
-      <c r="D55" s="36"/>
-      <c r="E55" s="36"/>
-      <c r="F55" s="36"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B55" s="34"/>
+      <c r="C55" s="34"/>
+      <c r="D55" s="34"/>
+      <c r="E55" s="34"/>
+      <c r="F55" s="34"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="12" t="s">
         <v>76</v>
       </c>
@@ -1454,12 +1464,12 @@
       <c r="E56" s="12"/>
       <c r="F56" s="12"/>
     </row>
-    <row r="58" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="35" t="s">
         <v>64</v>
       </c>
@@ -1469,7 +1479,7 @@
       <c r="E59" s="35"/>
       <c r="F59" s="35"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="35" t="s">
         <v>65</v>
       </c>
@@ -1479,7 +1489,7 @@
       <c r="E60" s="35"/>
       <c r="F60" s="35"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="35" t="s">
         <v>85</v>
       </c>
@@ -1489,7 +1499,7 @@
       <c r="E61" s="35"/>
       <c r="F61" s="35"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="12" t="s">
         <v>84</v>
       </c>
@@ -1499,17 +1509,20 @@
       <c r="E62" s="12"/>
       <c r="F62" s="12"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="36" t="s">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A63" s="34" t="s">
         <v>118</v>
       </c>
-      <c r="B63" s="36"/>
-      <c r="C63" s="36"/>
-      <c r="D63" s="36"/>
-      <c r="E63" s="36"/>
-      <c r="F63" s="36"/>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B63" s="34"/>
+      <c r="C63" s="34"/>
+      <c r="D63" s="34"/>
+      <c r="E63" s="34"/>
+      <c r="F63" s="34"/>
+      <c r="G63" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="17" t="s">
         <v>98</v>
       </c>
@@ -1519,7 +1532,7 @@
       <c r="E64" s="17"/>
       <c r="F64" s="17"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" s="23" t="s">
         <v>82</v>
       </c>
@@ -1529,7 +1542,7 @@
       <c r="E65" s="23"/>
       <c r="F65" s="23"/>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" s="25" t="s">
         <v>83</v>
       </c>
@@ -1539,17 +1552,20 @@
       <c r="E66" s="25"/>
       <c r="F66" s="25"/>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="36" t="s">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A67" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="B67" s="36"/>
-      <c r="C67" s="36"/>
-      <c r="D67" s="36"/>
-      <c r="E67" s="36"/>
-      <c r="F67" s="36"/>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B67" s="34"/>
+      <c r="C67" s="34"/>
+      <c r="D67" s="34"/>
+      <c r="E67" s="34"/>
+      <c r="F67" s="34"/>
+      <c r="G67" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="24" t="s">
         <v>99</v>
       </c>
@@ -1559,7 +1575,7 @@
       <c r="E68" s="24"/>
       <c r="F68" s="24"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="26" t="s">
         <v>117</v>
       </c>
@@ -1569,57 +1585,57 @@
       <c r="E69" s="26"/>
       <c r="F69" s="26"/>
     </row>
-    <row r="71" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="36" t="s">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A72" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="B72" s="36"/>
-      <c r="C72" s="36"/>
-      <c r="D72" s="36"/>
-      <c r="E72" s="36"/>
-      <c r="F72" s="36"/>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="36" t="s">
+      <c r="B72" s="34"/>
+      <c r="C72" s="34"/>
+      <c r="D72" s="34"/>
+      <c r="E72" s="34"/>
+      <c r="F72" s="34"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A73" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="B73" s="36"/>
-      <c r="C73" s="36"/>
-      <c r="D73" s="36"/>
-      <c r="E73" s="36"/>
-      <c r="F73" s="36"/>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="36" t="s">
+      <c r="B73" s="34"/>
+      <c r="C73" s="34"/>
+      <c r="D73" s="34"/>
+      <c r="E73" s="34"/>
+      <c r="F73" s="34"/>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A74" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="B74" s="36"/>
-      <c r="C74" s="36"/>
-      <c r="D74" s="36"/>
-      <c r="E74" s="36"/>
-      <c r="F74" s="36"/>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="36" t="s">
+      <c r="B74" s="34"/>
+      <c r="C74" s="34"/>
+      <c r="D74" s="34"/>
+      <c r="E74" s="34"/>
+      <c r="F74" s="34"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A75" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="B75" s="36"/>
-      <c r="C75" s="36"/>
-      <c r="D75" s="36"/>
-      <c r="E75" s="36"/>
-      <c r="F75" s="36"/>
-    </row>
-    <row r="77" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B75" s="34"/>
+      <c r="C75" s="34"/>
+      <c r="D75" s="34"/>
+      <c r="E75" s="34"/>
+      <c r="F75" s="34"/>
+    </row>
+    <row r="77" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" s="15" t="s">
         <v>78</v>
       </c>
@@ -1629,7 +1645,7 @@
       <c r="E78" s="15"/>
       <c r="F78" s="15"/>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" s="11" t="s">
         <v>97</v>
       </c>
@@ -1639,7 +1655,7 @@
       <c r="E79" s="11"/>
       <c r="F79" s="11"/>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" s="27" t="s">
         <v>116</v>
       </c>
@@ -1649,7 +1665,7 @@
       <c r="E80" s="27"/>
       <c r="F80" s="27"/>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" s="29" t="s">
         <v>115</v>
       </c>
@@ -1659,12 +1675,12 @@
       <c r="E81" s="29"/>
       <c r="F81" s="29"/>
     </row>
-    <row r="83" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A83" s="22" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" s="21" t="s">
         <v>111</v>
       </c>
@@ -1677,7 +1693,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" s="30" t="s">
         <v>112</v>
       </c>
@@ -1686,11 +1702,8 @@
       <c r="D85" s="30"/>
       <c r="E85" s="30"/>
       <c r="F85" s="30"/>
-      <c r="G85" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" s="16" t="s">
         <v>100</v>
       </c>
@@ -1699,8 +1712,11 @@
       <c r="D86" s="16"/>
       <c r="E86" s="16"/>
       <c r="F86" s="16"/>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G86" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" s="31" t="s">
         <v>120</v>
       </c>
@@ -1710,7 +1726,7 @@
       <c r="E87" s="31"/>
       <c r="F87" s="31"/>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" s="32" t="s">
         <v>121</v>
       </c>
@@ -1720,8 +1736,41 @@
       <c r="E88" s="32"/>
       <c r="F88" s="32"/>
     </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A89" s="33" t="s">
+        <v>122</v>
+      </c>
+      <c r="B89" s="33"/>
+      <c r="C89" s="33"/>
+      <c r="D89" s="33"/>
+      <c r="E89" s="33"/>
+      <c r="F89" s="33"/>
+      <c r="G89" t="s">
+        <v>113</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A29:F29"/>
+    <mergeCell ref="A31:F31"/>
+    <mergeCell ref="A32:F32"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A34:F34"/>
+    <mergeCell ref="A35:F35"/>
+    <mergeCell ref="A36:F36"/>
+    <mergeCell ref="A40:F40"/>
+    <mergeCell ref="A41:F41"/>
+    <mergeCell ref="A42:F42"/>
+    <mergeCell ref="A45:F45"/>
+    <mergeCell ref="A46:F46"/>
+    <mergeCell ref="A47:F47"/>
+    <mergeCell ref="A48:F48"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="A53:F53"/>
+    <mergeCell ref="A54:F54"/>
+    <mergeCell ref="A55:F55"/>
     <mergeCell ref="A72:F72"/>
     <mergeCell ref="A73:F73"/>
     <mergeCell ref="A74:F74"/>
@@ -1731,26 +1780,6 @@
     <mergeCell ref="A61:F61"/>
     <mergeCell ref="A63:F63"/>
     <mergeCell ref="A67:F67"/>
-    <mergeCell ref="A48:F48"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="A53:F53"/>
-    <mergeCell ref="A54:F54"/>
-    <mergeCell ref="A55:F55"/>
-    <mergeCell ref="A41:F41"/>
-    <mergeCell ref="A42:F42"/>
-    <mergeCell ref="A45:F45"/>
-    <mergeCell ref="A46:F46"/>
-    <mergeCell ref="A47:F47"/>
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="A34:F34"/>
-    <mergeCell ref="A35:F35"/>
-    <mergeCell ref="A36:F36"/>
-    <mergeCell ref="A40:F40"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A16:F16"/>
-    <mergeCell ref="A29:F29"/>
-    <mergeCell ref="A31:F31"/>
-    <mergeCell ref="A32:F32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1764,29 +1793,29 @@
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>81</v>
       </c>
@@ -1794,7 +1823,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>87</v>
       </c>
@@ -1802,7 +1831,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>88</v>
       </c>
@@ -1810,7 +1839,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>89</v>
       </c>
@@ -1818,7 +1847,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>80</v>
       </c>
@@ -1826,7 +1855,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>90</v>
       </c>
@@ -1834,7 +1863,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B9" s="14">
         <f>SUM(B3:B8)</f>
         <v>1</v>
@@ -1846,7 +1875,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="J10" t="s">
         <v>88</v>
       </c>
@@ -1863,7 +1892,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
         <v>13</v>
       </c>
@@ -1883,7 +1912,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>81</v>
       </c>
@@ -1894,7 +1923,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>87</v>
       </c>
@@ -1905,7 +1934,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>88</v>
       </c>
@@ -1913,7 +1942,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>89</v>
       </c>
@@ -1921,7 +1950,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>80</v>
       </c>
@@ -1929,7 +1958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>90</v>
       </c>
@@ -1937,18 +1966,18 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B18" s="14">
         <f>SUM(B12:B17)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="13" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>81</v>
       </c>
@@ -1956,7 +1985,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>87</v>
       </c>
@@ -1964,7 +1993,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>88</v>
       </c>
@@ -1972,7 +2001,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>89</v>
       </c>
@@ -1980,7 +2009,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>80</v>
       </c>
@@ -1988,7 +2017,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>90</v>
       </c>
@@ -1996,18 +2025,18 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B27" s="14">
         <f>SUM(B21:B26)</f>
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>81</v>
       </c>
@@ -2015,7 +2044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>87</v>
       </c>
@@ -2023,7 +2052,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>88</v>
       </c>
@@ -2031,7 +2060,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>89</v>
       </c>
@@ -2039,7 +2068,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>80</v>
       </c>
@@ -2047,7 +2076,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>90</v>
       </c>
@@ -2055,18 +2084,18 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B36" s="14">
         <f>SUM(B30:B35)</f>
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>81</v>
       </c>
@@ -2074,7 +2103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>87</v>
       </c>
@@ -2082,7 +2111,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>88</v>
       </c>
@@ -2090,7 +2119,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>89</v>
       </c>
@@ -2098,7 +2127,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>80</v>
       </c>
@@ -2106,7 +2135,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>90</v>
       </c>
@@ -2114,7 +2143,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B45" s="14">
         <f>SUM(B39:B44)</f>
         <v>1</v>

</xml_diff>

<commit_message>
Added Indra alien and a regen health feature for soldiers so they gain 20 health each round
</commit_message>
<xml_diff>
--- a/Production Documents/To-Do.xlsx
+++ b/Production Documents/To-Do.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmgam\Desktop\Shiva\Production Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{910E7BE6-F6CD-4AC1-963E-078F158CF2E5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ABF5E35-0969-4078-897F-92E4BE0F0D5B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{669DCC34-C837-4342-A908-0F87EB315612}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="127">
   <si>
     <t>Sprites</t>
   </si>
@@ -407,6 +407,12 @@
   </si>
   <si>
     <t>Civilians can be stored in the home base to generate food and research points</t>
+  </si>
+  <si>
+    <t>More aliens</t>
+  </si>
+  <si>
+    <t>Sound</t>
   </si>
 </sst>
 </file>
@@ -516,7 +522,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
@@ -546,6 +552,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
@@ -878,10 +886,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4D254F2-4E19-40CF-BD85-766CDBA8C5EF}">
-  <dimension ref="A2:G91"/>
+  <dimension ref="A2:G93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="G78" sqref="G78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -900,14 +908,14 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="18" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -1096,14 +1104,14 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A16" s="31" t="s">
+      <c r="A16" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="31"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="31"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
@@ -1223,14 +1231,14 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="32" t="s">
+      <c r="A29" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="32"/>
-      <c r="C29" s="32"/>
-      <c r="D29" s="32"/>
-      <c r="E29" s="32"/>
-      <c r="F29" s="32"/>
+      <c r="B29" s="34"/>
+      <c r="C29" s="34"/>
+      <c r="D29" s="34"/>
+      <c r="E29" s="34"/>
+      <c r="F29" s="34"/>
     </row>
     <row r="30" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
@@ -1238,64 +1246,64 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="33" t="s">
+      <c r="A31" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="B31" s="33"/>
-      <c r="C31" s="33"/>
-      <c r="D31" s="33"/>
-      <c r="E31" s="33"/>
-      <c r="F31" s="33"/>
+      <c r="B31" s="35"/>
+      <c r="C31" s="35"/>
+      <c r="D31" s="35"/>
+      <c r="E31" s="35"/>
+      <c r="F31" s="35"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="33" t="s">
+      <c r="A32" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="B32" s="33"/>
-      <c r="C32" s="33"/>
-      <c r="D32" s="33"/>
-      <c r="E32" s="33"/>
-      <c r="F32" s="33"/>
+      <c r="B32" s="35"/>
+      <c r="C32" s="35"/>
+      <c r="D32" s="35"/>
+      <c r="E32" s="35"/>
+      <c r="F32" s="35"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="33" t="s">
+      <c r="A33" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="B33" s="33"/>
-      <c r="C33" s="33"/>
-      <c r="D33" s="33"/>
-      <c r="E33" s="33"/>
-      <c r="F33" s="33"/>
+      <c r="B33" s="35"/>
+      <c r="C33" s="35"/>
+      <c r="D33" s="35"/>
+      <c r="E33" s="35"/>
+      <c r="F33" s="35"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="33" t="s">
+      <c r="A34" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="B34" s="33"/>
-      <c r="C34" s="33"/>
-      <c r="D34" s="33"/>
-      <c r="E34" s="33"/>
-      <c r="F34" s="33"/>
+      <c r="B34" s="35"/>
+      <c r="C34" s="35"/>
+      <c r="D34" s="35"/>
+      <c r="E34" s="35"/>
+      <c r="F34" s="35"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="33" t="s">
+      <c r="A35" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="B35" s="33"/>
-      <c r="C35" s="33"/>
-      <c r="D35" s="33"/>
-      <c r="E35" s="33"/>
-      <c r="F35" s="33"/>
+      <c r="B35" s="35"/>
+      <c r="C35" s="35"/>
+      <c r="D35" s="35"/>
+      <c r="E35" s="35"/>
+      <c r="F35" s="35"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="33" t="s">
+      <c r="A36" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="B36" s="33"/>
-      <c r="C36" s="33"/>
-      <c r="D36" s="33"/>
-      <c r="E36" s="33"/>
-      <c r="F36" s="33"/>
+      <c r="B36" s="35"/>
+      <c r="C36" s="35"/>
+      <c r="D36" s="35"/>
+      <c r="E36" s="35"/>
+      <c r="F36" s="35"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="21" t="s">
@@ -1313,34 +1321,34 @@
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="33" t="s">
+      <c r="A40" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="B40" s="33"/>
-      <c r="C40" s="33"/>
-      <c r="D40" s="33"/>
-      <c r="E40" s="33"/>
-      <c r="F40" s="33"/>
+      <c r="B40" s="35"/>
+      <c r="C40" s="35"/>
+      <c r="D40" s="35"/>
+      <c r="E40" s="35"/>
+      <c r="F40" s="35"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="33" t="s">
+      <c r="A41" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="B41" s="33"/>
-      <c r="C41" s="33"/>
-      <c r="D41" s="33"/>
-      <c r="E41" s="33"/>
-      <c r="F41" s="33"/>
+      <c r="B41" s="35"/>
+      <c r="C41" s="35"/>
+      <c r="D41" s="35"/>
+      <c r="E41" s="35"/>
+      <c r="F41" s="35"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="33" t="s">
+      <c r="A42" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="B42" s="33"/>
-      <c r="C42" s="33"/>
-      <c r="D42" s="33"/>
-      <c r="E42" s="33"/>
-      <c r="F42" s="33"/>
+      <c r="B42" s="35"/>
+      <c r="C42" s="35"/>
+      <c r="D42" s="35"/>
+      <c r="E42" s="35"/>
+      <c r="F42" s="35"/>
     </row>
     <row r="43" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
@@ -1351,44 +1359,44 @@
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="33" t="s">
+      <c r="A45" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="B45" s="33"/>
-      <c r="C45" s="33"/>
-      <c r="D45" s="33"/>
-      <c r="E45" s="33"/>
-      <c r="F45" s="33"/>
+      <c r="B45" s="35"/>
+      <c r="C45" s="35"/>
+      <c r="D45" s="35"/>
+      <c r="E45" s="35"/>
+      <c r="F45" s="35"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="33" t="s">
+      <c r="A46" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="B46" s="33"/>
-      <c r="C46" s="33"/>
-      <c r="D46" s="33"/>
-      <c r="E46" s="33"/>
-      <c r="F46" s="33"/>
+      <c r="B46" s="35"/>
+      <c r="C46" s="35"/>
+      <c r="D46" s="35"/>
+      <c r="E46" s="35"/>
+      <c r="F46" s="35"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="33" t="s">
+      <c r="A47" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="B47" s="33"/>
-      <c r="C47" s="33"/>
-      <c r="D47" s="33"/>
-      <c r="E47" s="33"/>
-      <c r="F47" s="33"/>
+      <c r="B47" s="35"/>
+      <c r="C47" s="35"/>
+      <c r="D47" s="35"/>
+      <c r="E47" s="35"/>
+      <c r="F47" s="35"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="33" t="s">
+      <c r="A48" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="B48" s="33"/>
-      <c r="C48" s="33"/>
-      <c r="D48" s="33"/>
-      <c r="E48" s="33"/>
-      <c r="F48" s="33"/>
+      <c r="B48" s="35"/>
+      <c r="C48" s="35"/>
+      <c r="D48" s="35"/>
+      <c r="E48" s="35"/>
+      <c r="F48" s="35"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="30" t="s">
@@ -1406,44 +1414,44 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="33" t="s">
+      <c r="A52" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="B52" s="33"/>
-      <c r="C52" s="33"/>
-      <c r="D52" s="33"/>
-      <c r="E52" s="33"/>
-      <c r="F52" s="33"/>
+      <c r="B52" s="35"/>
+      <c r="C52" s="35"/>
+      <c r="D52" s="35"/>
+      <c r="E52" s="35"/>
+      <c r="F52" s="35"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="33" t="s">
+      <c r="A53" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="B53" s="33"/>
-      <c r="C53" s="33"/>
-      <c r="D53" s="33"/>
-      <c r="E53" s="33"/>
-      <c r="F53" s="33"/>
+      <c r="B53" s="35"/>
+      <c r="C53" s="35"/>
+      <c r="D53" s="35"/>
+      <c r="E53" s="35"/>
+      <c r="F53" s="35"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="33" t="s">
+      <c r="A54" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="B54" s="33"/>
-      <c r="C54" s="33"/>
-      <c r="D54" s="33"/>
-      <c r="E54" s="33"/>
-      <c r="F54" s="33"/>
+      <c r="B54" s="35"/>
+      <c r="C54" s="35"/>
+      <c r="D54" s="35"/>
+      <c r="E54" s="35"/>
+      <c r="F54" s="35"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="34" t="s">
+      <c r="A55" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="B55" s="34"/>
-      <c r="C55" s="34"/>
-      <c r="D55" s="34"/>
-      <c r="E55" s="34"/>
-      <c r="F55" s="34"/>
+      <c r="B55" s="36"/>
+      <c r="C55" s="36"/>
+      <c r="D55" s="36"/>
+      <c r="E55" s="36"/>
+      <c r="F55" s="36"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="11" t="s">
@@ -1461,34 +1469,34 @@
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="33" t="s">
+      <c r="A59" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="B59" s="33"/>
-      <c r="C59" s="33"/>
-      <c r="D59" s="33"/>
-      <c r="E59" s="33"/>
-      <c r="F59" s="33"/>
+      <c r="B59" s="35"/>
+      <c r="C59" s="35"/>
+      <c r="D59" s="35"/>
+      <c r="E59" s="35"/>
+      <c r="F59" s="35"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="33" t="s">
+      <c r="A60" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="B60" s="33"/>
-      <c r="C60" s="33"/>
-      <c r="D60" s="33"/>
-      <c r="E60" s="33"/>
-      <c r="F60" s="33"/>
+      <c r="B60" s="35"/>
+      <c r="C60" s="35"/>
+      <c r="D60" s="35"/>
+      <c r="E60" s="35"/>
+      <c r="F60" s="35"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="33" t="s">
+      <c r="A61" s="35" t="s">
         <v>85</v>
       </c>
-      <c r="B61" s="33"/>
-      <c r="C61" s="33"/>
-      <c r="D61" s="33"/>
-      <c r="E61" s="33"/>
-      <c r="F61" s="33"/>
+      <c r="B61" s="35"/>
+      <c r="C61" s="35"/>
+      <c r="D61" s="35"/>
+      <c r="E61" s="35"/>
+      <c r="F61" s="35"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="11" t="s">
@@ -1501,14 +1509,14 @@
       <c r="F62" s="11"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="33" t="s">
+      <c r="A63" s="35" t="s">
         <v>118</v>
       </c>
-      <c r="B63" s="33"/>
-      <c r="C63" s="33"/>
-      <c r="D63" s="33"/>
-      <c r="E63" s="33"/>
-      <c r="F63" s="33"/>
+      <c r="B63" s="35"/>
+      <c r="C63" s="35"/>
+      <c r="D63" s="35"/>
+      <c r="E63" s="35"/>
+      <c r="F63" s="35"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="30" t="s">
@@ -1541,14 +1549,14 @@
       <c r="F66" s="30"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="33" t="s">
+      <c r="A67" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="B67" s="33"/>
-      <c r="C67" s="33"/>
-      <c r="D67" s="33"/>
-      <c r="E67" s="33"/>
-      <c r="F67" s="33"/>
+      <c r="B67" s="35"/>
+      <c r="C67" s="35"/>
+      <c r="D67" s="35"/>
+      <c r="E67" s="35"/>
+      <c r="F67" s="35"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="20" t="s">
@@ -1576,44 +1584,44 @@
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="34" t="s">
+      <c r="A72" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="B72" s="34"/>
-      <c r="C72" s="34"/>
-      <c r="D72" s="34"/>
-      <c r="E72" s="34"/>
-      <c r="F72" s="34"/>
+      <c r="B72" s="36"/>
+      <c r="C72" s="36"/>
+      <c r="D72" s="36"/>
+      <c r="E72" s="36"/>
+      <c r="F72" s="36"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="34" t="s">
+      <c r="A73" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="B73" s="34"/>
-      <c r="C73" s="34"/>
-      <c r="D73" s="34"/>
-      <c r="E73" s="34"/>
-      <c r="F73" s="34"/>
+      <c r="B73" s="36"/>
+      <c r="C73" s="36"/>
+      <c r="D73" s="36"/>
+      <c r="E73" s="36"/>
+      <c r="F73" s="36"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="34" t="s">
+      <c r="A74" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="B74" s="34"/>
-      <c r="C74" s="34"/>
-      <c r="D74" s="34"/>
-      <c r="E74" s="34"/>
-      <c r="F74" s="34"/>
+      <c r="B74" s="36"/>
+      <c r="C74" s="36"/>
+      <c r="D74" s="36"/>
+      <c r="E74" s="36"/>
+      <c r="F74" s="36"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="34" t="s">
+      <c r="A75" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="B75" s="34"/>
-      <c r="C75" s="34"/>
-      <c r="D75" s="34"/>
-      <c r="E75" s="34"/>
-      <c r="F75" s="34"/>
+      <c r="B75" s="36"/>
+      <c r="C75" s="36"/>
+      <c r="D75" s="36"/>
+      <c r="E75" s="36"/>
+      <c r="F75" s="36"/>
     </row>
     <row r="77" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
@@ -1669,6 +1677,9 @@
       <c r="D82" s="29"/>
       <c r="E82" s="29"/>
       <c r="F82" s="29"/>
+      <c r="G82" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="29" t="s">
@@ -1680,77 +1691,100 @@
       <c r="E83" s="29"/>
       <c r="F83" s="29"/>
     </row>
-    <row r="85" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="1" t="s">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="B84" s="32"/>
+      <c r="C84" s="32"/>
+      <c r="D84" s="32"/>
+      <c r="E84" s="32"/>
+      <c r="F84" s="32"/>
+      <c r="G84" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85" s="31" t="s">
+        <v>126</v>
+      </c>
+      <c r="B85" s="31"/>
+      <c r="C85" s="31"/>
+      <c r="D85" s="31"/>
+      <c r="E85" s="31"/>
+      <c r="F85" s="31"/>
+    </row>
+    <row r="87" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A86" s="19" t="s">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="B86" s="19"/>
-      <c r="C86" s="19"/>
-      <c r="D86" s="19"/>
-      <c r="E86" s="19"/>
-      <c r="F86" s="19"/>
-      <c r="G86" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A87" s="25" t="s">
-        <v>112</v>
-      </c>
-      <c r="B87" s="25"/>
-      <c r="C87" s="25"/>
-      <c r="D87" s="25"/>
-      <c r="E87" s="25"/>
-      <c r="F87" s="25"/>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A88" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="B88" s="15"/>
-      <c r="C88" s="15"/>
-      <c r="D88" s="15"/>
-      <c r="E88" s="15"/>
-      <c r="F88" s="15"/>
+      <c r="B88" s="19"/>
+      <c r="C88" s="19"/>
+      <c r="D88" s="19"/>
+      <c r="E88" s="19"/>
+      <c r="F88" s="19"/>
       <c r="G88" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A89" s="26" t="s">
+      <c r="A89" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="B89" s="25"/>
+      <c r="C89" s="25"/>
+      <c r="D89" s="25"/>
+      <c r="E89" s="25"/>
+      <c r="F89" s="25"/>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="B90" s="15"/>
+      <c r="C90" s="15"/>
+      <c r="D90" s="15"/>
+      <c r="E90" s="15"/>
+      <c r="F90" s="15"/>
+      <c r="G90" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="B89" s="26"/>
-      <c r="C89" s="26"/>
-      <c r="D89" s="26"/>
-      <c r="E89" s="26"/>
-      <c r="F89" s="26"/>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A90" s="27" t="s">
+      <c r="B91" s="26"/>
+      <c r="C91" s="26"/>
+      <c r="D91" s="26"/>
+      <c r="E91" s="26"/>
+      <c r="F91" s="26"/>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A92" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="B90" s="27"/>
-      <c r="C90" s="27"/>
-      <c r="D90" s="27"/>
-      <c r="E90" s="27"/>
-      <c r="F90" s="27"/>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A91" s="28" t="s">
+      <c r="B92" s="27"/>
+      <c r="C92" s="27"/>
+      <c r="D92" s="27"/>
+      <c r="E92" s="27"/>
+      <c r="F92" s="27"/>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93" s="28" t="s">
         <v>122</v>
       </c>
-      <c r="B91" s="28"/>
-      <c r="C91" s="28"/>
-      <c r="D91" s="28"/>
-      <c r="E91" s="28"/>
-      <c r="F91" s="28"/>
-      <c r="G91" t="s">
+      <c r="B93" s="28"/>
+      <c r="C93" s="28"/>
+      <c r="D93" s="28"/>
+      <c r="E93" s="28"/>
+      <c r="F93" s="28"/>
+      <c r="G93" t="s">
         <v>113</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed a couple bugs and added level ups to walls
</commit_message>
<xml_diff>
--- a/Production Documents/To-Do.xlsx
+++ b/Production Documents/To-Do.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmgam\Desktop\Shiva\Production Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Shiva\Production Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ABF5E35-0969-4078-897F-92E4BE0F0D5B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3109506-D652-40AE-9E94-35603BEFE67D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{669DCC34-C837-4342-A908-0F87EB315612}"/>
+    <workbookView xWindow="5760" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{669DCC34-C837-4342-A908-0F87EB315612}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -522,7 +522,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
@@ -556,14 +556,15 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -888,36 +889,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4D254F2-4E19-40CF-BD85-766CDBA8C5EF}">
   <dimension ref="A2:G93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="G78" sqref="G78"/>
+    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A82" sqref="A82:F82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="18" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="33" t="s">
+    <row r="3" spans="1:7" ht="18" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-    </row>
-    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+    </row>
+    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -940,7 +941,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>73</v>
       </c>
@@ -963,7 +964,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -986,7 +987,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
@@ -1009,7 +1010,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
@@ -1028,7 +1029,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
@@ -1047,7 +1048,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
@@ -1064,7 +1065,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="23" t="s">
         <v>13</v>
       </c>
@@ -1079,7 +1080,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
@@ -1090,7 +1091,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
         <v>119</v>
       </c>
@@ -1098,22 +1099,22 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C14" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A16" s="33" t="s">
+    <row r="16" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A16" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="33"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
-    </row>
-    <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="36"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+    </row>
+    <row r="17" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
         <v>3</v>
@@ -1131,7 +1132,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B18" s="8" t="s">
         <v>15</v>
       </c>
@@ -1148,7 +1149,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
@@ -1163,7 +1164,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
@@ -1178,7 +1179,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B21" s="17" t="s">
         <v>18</v>
       </c>
@@ -1188,7 +1189,7 @@
       <c r="D21" s="4"/>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B22" s="17" t="s">
         <v>19</v>
       </c>
@@ -1199,7 +1200,7 @@
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B23" s="17" t="s">
         <v>20</v>
       </c>
@@ -1210,42 +1211,42 @@
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C24" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C25" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C26" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C27" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="34" t="s">
+    <row r="29" spans="1:6" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A29" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="34"/>
-      <c r="C29" s="34"/>
-      <c r="D29" s="34"/>
-      <c r="E29" s="34"/>
-      <c r="F29" s="34"/>
-    </row>
-    <row r="30" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="37"/>
+      <c r="C29" s="37"/>
+      <c r="D29" s="37"/>
+      <c r="E29" s="37"/>
+      <c r="F29" s="37"/>
+    </row>
+    <row r="30" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="35" t="s">
         <v>44</v>
       </c>
@@ -1255,7 +1256,7 @@
       <c r="E31" s="35"/>
       <c r="F31" s="35"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="35" t="s">
         <v>45</v>
       </c>
@@ -1265,7 +1266,7 @@
       <c r="E32" s="35"/>
       <c r="F32" s="35"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="35" t="s">
         <v>72</v>
       </c>
@@ -1275,7 +1276,7 @@
       <c r="E33" s="35"/>
       <c r="F33" s="35"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="35" t="s">
         <v>46</v>
       </c>
@@ -1285,7 +1286,7 @@
       <c r="E34" s="35"/>
       <c r="F34" s="35"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="35" t="s">
         <v>47</v>
       </c>
@@ -1295,7 +1296,7 @@
       <c r="E35" s="35"/>
       <c r="F35" s="35"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="35" t="s">
         <v>48</v>
       </c>
@@ -1305,7 +1306,7 @@
       <c r="E36" s="35"/>
       <c r="F36" s="35"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="21" t="s">
         <v>114</v>
       </c>
@@ -1315,12 +1316,12 @@
       <c r="E37" s="21"/>
       <c r="F37" s="21"/>
     </row>
-    <row r="39" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="35" t="s">
         <v>60</v>
       </c>
@@ -1330,7 +1331,7 @@
       <c r="E40" s="35"/>
       <c r="F40" s="35"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="35" t="s">
         <v>61</v>
       </c>
@@ -1340,7 +1341,7 @@
       <c r="E41" s="35"/>
       <c r="F41" s="35"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="35" t="s">
         <v>62</v>
       </c>
@@ -1350,15 +1351,15 @@
       <c r="E42" s="35"/>
       <c r="F42" s="35"/>
     </row>
-    <row r="43" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="1"/>
     </row>
-    <row r="44" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="35" t="s">
         <v>49</v>
       </c>
@@ -1368,7 +1369,7 @@
       <c r="E45" s="35"/>
       <c r="F45" s="35"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="35" t="s">
         <v>50</v>
       </c>
@@ -1378,7 +1379,7 @@
       <c r="E46" s="35"/>
       <c r="F46" s="35"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="35" t="s">
         <v>52</v>
       </c>
@@ -1388,7 +1389,7 @@
       <c r="E47" s="35"/>
       <c r="F47" s="35"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="35" t="s">
         <v>53</v>
       </c>
@@ -1398,7 +1399,7 @@
       <c r="E48" s="35"/>
       <c r="F48" s="35"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="30" t="s">
         <v>75</v>
       </c>
@@ -1408,12 +1409,12 @@
       <c r="E49" s="30"/>
       <c r="F49" s="30"/>
     </row>
-    <row r="51" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="35" t="s">
         <v>55</v>
       </c>
@@ -1423,7 +1424,7 @@
       <c r="E52" s="35"/>
       <c r="F52" s="35"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="35" t="s">
         <v>56</v>
       </c>
@@ -1433,7 +1434,7 @@
       <c r="E53" s="35"/>
       <c r="F53" s="35"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="35" t="s">
         <v>57</v>
       </c>
@@ -1443,17 +1444,17 @@
       <c r="E54" s="35"/>
       <c r="F54" s="35"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="36" t="s">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="B55" s="36"/>
-      <c r="C55" s="36"/>
-      <c r="D55" s="36"/>
-      <c r="E55" s="36"/>
-      <c r="F55" s="36"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B55" s="34"/>
+      <c r="C55" s="34"/>
+      <c r="D55" s="34"/>
+      <c r="E55" s="34"/>
+      <c r="F55" s="34"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="11" t="s">
         <v>76</v>
       </c>
@@ -1463,12 +1464,12 @@
       <c r="E56" s="11"/>
       <c r="F56" s="11"/>
     </row>
-    <row r="58" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="35" t="s">
         <v>64</v>
       </c>
@@ -1478,7 +1479,7 @@
       <c r="E59" s="35"/>
       <c r="F59" s="35"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="35" t="s">
         <v>65</v>
       </c>
@@ -1488,7 +1489,7 @@
       <c r="E60" s="35"/>
       <c r="F60" s="35"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="35" t="s">
         <v>85</v>
       </c>
@@ -1498,7 +1499,7 @@
       <c r="E61" s="35"/>
       <c r="F61" s="35"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="11" t="s">
         <v>84</v>
       </c>
@@ -1508,7 +1509,7 @@
       <c r="E62" s="11"/>
       <c r="F62" s="11"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="35" t="s">
         <v>118</v>
       </c>
@@ -1518,7 +1519,7 @@
       <c r="E63" s="35"/>
       <c r="F63" s="35"/>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="30" t="s">
         <v>98</v>
       </c>
@@ -1528,7 +1529,7 @@
       <c r="E64" s="30"/>
       <c r="F64" s="30"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="30" t="s">
         <v>82</v>
       </c>
@@ -1538,7 +1539,7 @@
       <c r="E65" s="30"/>
       <c r="F65" s="30"/>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="30" t="s">
         <v>83</v>
       </c>
@@ -1548,7 +1549,7 @@
       <c r="E66" s="30"/>
       <c r="F66" s="30"/>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="35" t="s">
         <v>67</v>
       </c>
@@ -1558,7 +1559,7 @@
       <c r="E67" s="35"/>
       <c r="F67" s="35"/>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="20" t="s">
         <v>99</v>
       </c>
@@ -1568,7 +1569,7 @@
       <c r="E68" s="20"/>
       <c r="F68" s="20"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="21" t="s">
         <v>117</v>
       </c>
@@ -1578,57 +1579,57 @@
       <c r="E69" s="21"/>
       <c r="F69" s="21"/>
     </row>
-    <row r="71" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="36" t="s">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A72" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="B72" s="36"/>
-      <c r="C72" s="36"/>
-      <c r="D72" s="36"/>
-      <c r="E72" s="36"/>
-      <c r="F72" s="36"/>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="36" t="s">
+      <c r="B72" s="34"/>
+      <c r="C72" s="34"/>
+      <c r="D72" s="34"/>
+      <c r="E72" s="34"/>
+      <c r="F72" s="34"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A73" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="B73" s="36"/>
-      <c r="C73" s="36"/>
-      <c r="D73" s="36"/>
-      <c r="E73" s="36"/>
-      <c r="F73" s="36"/>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="36" t="s">
+      <c r="B73" s="34"/>
+      <c r="C73" s="34"/>
+      <c r="D73" s="34"/>
+      <c r="E73" s="34"/>
+      <c r="F73" s="34"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A74" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="B74" s="36"/>
-      <c r="C74" s="36"/>
-      <c r="D74" s="36"/>
-      <c r="E74" s="36"/>
-      <c r="F74" s="36"/>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="36" t="s">
+      <c r="B74" s="34"/>
+      <c r="C74" s="34"/>
+      <c r="D74" s="34"/>
+      <c r="E74" s="34"/>
+      <c r="F74" s="34"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A75" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="B75" s="36"/>
-      <c r="C75" s="36"/>
-      <c r="D75" s="36"/>
-      <c r="E75" s="36"/>
-      <c r="F75" s="36"/>
-    </row>
-    <row r="77" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B75" s="34"/>
+      <c r="C75" s="34"/>
+      <c r="D75" s="34"/>
+      <c r="E75" s="34"/>
+      <c r="F75" s="34"/>
+    </row>
+    <row r="77" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" s="14" t="s">
         <v>78</v>
       </c>
@@ -1638,7 +1639,7 @@
       <c r="E78" s="14"/>
       <c r="F78" s="14"/>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" s="10" t="s">
         <v>97</v>
       </c>
@@ -1648,7 +1649,7 @@
       <c r="E79" s="10"/>
       <c r="F79" s="10"/>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" s="22" t="s">
         <v>116</v>
       </c>
@@ -1658,7 +1659,7 @@
       <c r="E80" s="22"/>
       <c r="F80" s="22"/>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" s="24" t="s">
         <v>115</v>
       </c>
@@ -1668,20 +1669,20 @@
       <c r="E81" s="24"/>
       <c r="F81" s="24"/>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82" s="29" t="s">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A82" s="33" t="s">
         <v>123</v>
       </c>
-      <c r="B82" s="29"/>
-      <c r="C82" s="29"/>
-      <c r="D82" s="29"/>
-      <c r="E82" s="29"/>
-      <c r="F82" s="29"/>
+      <c r="B82" s="33"/>
+      <c r="C82" s="33"/>
+      <c r="D82" s="33"/>
+      <c r="E82" s="33"/>
+      <c r="F82" s="33"/>
       <c r="G82" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" s="29" t="s">
         <v>124</v>
       </c>
@@ -1691,7 +1692,7 @@
       <c r="E83" s="29"/>
       <c r="F83" s="29"/>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" s="32" t="s">
         <v>125</v>
       </c>
@@ -1704,7 +1705,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" s="31" t="s">
         <v>126</v>
       </c>
@@ -1714,12 +1715,12 @@
       <c r="E85" s="31"/>
       <c r="F85" s="31"/>
     </row>
-    <row r="87" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" s="19" t="s">
         <v>111</v>
       </c>
@@ -1732,7 +1733,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" s="25" t="s">
         <v>112</v>
       </c>
@@ -1742,7 +1743,7 @@
       <c r="E89" s="25"/>
       <c r="F89" s="25"/>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" s="15" t="s">
         <v>100</v>
       </c>
@@ -1755,7 +1756,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" s="26" t="s">
         <v>120</v>
       </c>
@@ -1765,7 +1766,7 @@
       <c r="E91" s="26"/>
       <c r="F91" s="26"/>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" s="27" t="s">
         <v>121</v>
       </c>
@@ -1775,7 +1776,7 @@
       <c r="E92" s="27"/>
       <c r="F92" s="27"/>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" s="28" t="s">
         <v>122</v>
       </c>
@@ -1790,6 +1791,26 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A29:F29"/>
+    <mergeCell ref="A31:F31"/>
+    <mergeCell ref="A32:F32"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A34:F34"/>
+    <mergeCell ref="A35:F35"/>
+    <mergeCell ref="A36:F36"/>
+    <mergeCell ref="A40:F40"/>
+    <mergeCell ref="A41:F41"/>
+    <mergeCell ref="A42:F42"/>
+    <mergeCell ref="A45:F45"/>
+    <mergeCell ref="A46:F46"/>
+    <mergeCell ref="A47:F47"/>
+    <mergeCell ref="A48:F48"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="A53:F53"/>
+    <mergeCell ref="A54:F54"/>
+    <mergeCell ref="A55:F55"/>
     <mergeCell ref="A72:F72"/>
     <mergeCell ref="A73:F73"/>
     <mergeCell ref="A74:F74"/>
@@ -1799,26 +1820,6 @@
     <mergeCell ref="A61:F61"/>
     <mergeCell ref="A63:F63"/>
     <mergeCell ref="A67:F67"/>
-    <mergeCell ref="A48:F48"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="A53:F53"/>
-    <mergeCell ref="A54:F54"/>
-    <mergeCell ref="A55:F55"/>
-    <mergeCell ref="A41:F41"/>
-    <mergeCell ref="A42:F42"/>
-    <mergeCell ref="A45:F45"/>
-    <mergeCell ref="A46:F46"/>
-    <mergeCell ref="A47:F47"/>
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="A34:F34"/>
-    <mergeCell ref="A35:F35"/>
-    <mergeCell ref="A36:F36"/>
-    <mergeCell ref="A40:F40"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A16:F16"/>
-    <mergeCell ref="A29:F29"/>
-    <mergeCell ref="A31:F31"/>
-    <mergeCell ref="A32:F32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1832,29 +1833,29 @@
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>81</v>
       </c>
@@ -1862,7 +1863,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>87</v>
       </c>
@@ -1870,7 +1871,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>88</v>
       </c>
@@ -1878,7 +1879,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>89</v>
       </c>
@@ -1886,7 +1887,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>80</v>
       </c>
@@ -1894,7 +1895,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>90</v>
       </c>
@@ -1902,7 +1903,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B9" s="13">
         <f>SUM(B3:B8)</f>
         <v>1</v>
@@ -1914,7 +1915,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="J10" t="s">
         <v>88</v>
       </c>
@@ -1931,7 +1932,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
         <v>13</v>
       </c>
@@ -1951,7 +1952,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>81</v>
       </c>
@@ -1962,7 +1963,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>87</v>
       </c>
@@ -1973,7 +1974,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>88</v>
       </c>
@@ -1981,7 +1982,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>89</v>
       </c>
@@ -1989,7 +1990,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>80</v>
       </c>
@@ -1997,7 +1998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>90</v>
       </c>
@@ -2005,18 +2006,18 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B18" s="13">
         <f>SUM(B12:B17)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>81</v>
       </c>
@@ -2024,7 +2025,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>87</v>
       </c>
@@ -2032,7 +2033,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>88</v>
       </c>
@@ -2040,7 +2041,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>89</v>
       </c>
@@ -2048,7 +2049,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>80</v>
       </c>
@@ -2056,7 +2057,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>90</v>
       </c>
@@ -2064,18 +2065,18 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B27" s="13">
         <f>SUM(B21:B26)</f>
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>81</v>
       </c>
@@ -2083,7 +2084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>87</v>
       </c>
@@ -2091,7 +2092,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>88</v>
       </c>
@@ -2099,7 +2100,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>89</v>
       </c>
@@ -2107,7 +2108,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>80</v>
       </c>
@@ -2115,7 +2116,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>90</v>
       </c>
@@ -2123,18 +2124,18 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B36" s="13">
         <f>SUM(B30:B35)</f>
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>81</v>
       </c>
@@ -2142,7 +2143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>87</v>
       </c>
@@ -2150,7 +2151,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>88</v>
       </c>
@@ -2158,7 +2159,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>89</v>
       </c>
@@ -2166,7 +2167,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>80</v>
       </c>
@@ -2174,7 +2175,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>90</v>
       </c>
@@ -2182,7 +2183,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B45" s="13">
         <f>SUM(B39:B44)</f>
         <v>1</v>

</xml_diff>

<commit_message>
Added Fog system to the game. Fog is dispelled by Humans, Static Plains Tiles, and Spawn Pods. Fogged tiles cannot be clicked on to reveal what they are, and hide anything beneath them. Started changing textures for map tiles.
</commit_message>
<xml_diff>
--- a/Production Documents/To-Do.xlsx
+++ b/Production Documents/To-Do.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Shiva\Production Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jareds\Documents\GitHub\Shiva\Production Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3109506-D652-40AE-9E94-35603BEFE67D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B193CB-A0CD-407B-B0EE-05A19C6314A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{669DCC34-C837-4342-A908-0F87EB315612}"/>
+    <workbookView xWindow="2370" yWindow="6165" windowWidth="28800" windowHeight="15435" xr2:uid="{669DCC34-C837-4342-A908-0F87EB315612}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -334,9 +334,6 @@
     <t>Humans have a 'Feed' button to be given food</t>
   </si>
   <si>
-    <t>Only certain tiles are visable</t>
-  </si>
-  <si>
     <t>Inventory</t>
   </si>
   <si>
@@ -413,6 +410,9 @@
   </si>
   <si>
     <t>Sound</t>
+  </si>
+  <si>
+    <t>Only certain tiles are visable (Fog implemented)</t>
   </si>
 </sst>
 </file>
@@ -460,7 +460,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -476,6 +476,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -538,7 +544,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3" applyFill="1"/>
@@ -557,14 +562,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -889,36 +895,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4D254F2-4E19-40CF-BD85-766CDBA8C5EF}">
   <dimension ref="A2:G93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A82" sqref="A82:F82"/>
+    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55:F55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="18" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="36" t="s">
+    <row r="3" spans="1:7" ht="18" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-    </row>
-    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -937,11 +943,11 @@
       <c r="F4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="18" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G4" s="17" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>73</v>
       </c>
@@ -960,11 +966,11 @@
       <c r="F5" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="16" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G5" s="15" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -983,11 +989,11 @@
       <c r="F6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="16" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G6" s="15" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
@@ -1006,11 +1012,11 @@
       <c r="F7" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="16" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G7" s="15" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
@@ -1025,11 +1031,11 @@
         <v>27</v>
       </c>
       <c r="F8" s="4"/>
-      <c r="G8" s="16" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G8" s="15" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
@@ -1044,11 +1050,11 @@
         <v>28</v>
       </c>
       <c r="F9" s="4"/>
-      <c r="G9" s="16" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G9" s="15" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
@@ -1061,12 +1067,12 @@
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
-      <c r="G10" s="16" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="23" t="s">
+      <c r="G10" s="15" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="22" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="4"/>
@@ -1076,45 +1082,45 @@
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
-      <c r="G11" s="16" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G11" s="15" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="G12" s="16" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="24" t="s">
-        <v>119</v>
+      <c r="G12" s="15" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="23" t="s">
+        <v>118</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C14" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A16" s="36" t="s">
+    <row r="16" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A16" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="36"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-    </row>
-    <row r="17" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="33"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
         <v>3</v>
@@ -1132,7 +1138,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B18" s="8" t="s">
         <v>15</v>
       </c>
@@ -1149,7 +1155,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
@@ -1164,7 +1170,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
@@ -1179,8 +1185,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B21" s="17" t="s">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="16" t="s">
         <v>18</v>
       </c>
       <c r="C21" s="3" t="s">
@@ -1189,8 +1195,8 @@
       <c r="D21" s="4"/>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B22" s="17" t="s">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="16" t="s">
         <v>19</v>
       </c>
       <c r="C22" s="9" t="s">
@@ -1200,8 +1206,8 @@
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B23" s="17" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="16" t="s">
         <v>20</v>
       </c>
       <c r="C23" s="3" t="s">
@@ -1211,42 +1217,42 @@
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C24" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C25" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C26" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C27" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="37" t="s">
+    <row r="29" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="37"/>
-      <c r="C29" s="37"/>
-      <c r="D29" s="37"/>
-      <c r="E29" s="37"/>
-      <c r="F29" s="37"/>
-    </row>
-    <row r="30" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="34"/>
+      <c r="C29" s="34"/>
+      <c r="D29" s="34"/>
+      <c r="E29" s="34"/>
+      <c r="F29" s="34"/>
+    </row>
+    <row r="30" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="35" t="s">
         <v>44</v>
       </c>
@@ -1256,7 +1262,7 @@
       <c r="E31" s="35"/>
       <c r="F31" s="35"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="35" t="s">
         <v>45</v>
       </c>
@@ -1266,7 +1272,7 @@
       <c r="E32" s="35"/>
       <c r="F32" s="35"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="35" t="s">
         <v>72</v>
       </c>
@@ -1276,7 +1282,7 @@
       <c r="E33" s="35"/>
       <c r="F33" s="35"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="35" t="s">
         <v>46</v>
       </c>
@@ -1286,7 +1292,7 @@
       <c r="E34" s="35"/>
       <c r="F34" s="35"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="35" t="s">
         <v>47</v>
       </c>
@@ -1296,7 +1302,7 @@
       <c r="E35" s="35"/>
       <c r="F35" s="35"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="35" t="s">
         <v>48</v>
       </c>
@@ -1306,22 +1312,22 @@
       <c r="E36" s="35"/>
       <c r="F36" s="35"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="21" t="s">
-        <v>114</v>
-      </c>
-      <c r="B37" s="21"/>
-      <c r="C37" s="21"/>
-      <c r="D37" s="21"/>
-      <c r="E37" s="21"/>
-      <c r="F37" s="21"/>
-    </row>
-    <row r="39" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="B37" s="20"/>
+      <c r="C37" s="20"/>
+      <c r="D37" s="20"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="20"/>
+    </row>
+    <row r="39" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="35" t="s">
         <v>60</v>
       </c>
@@ -1331,7 +1337,7 @@
       <c r="E40" s="35"/>
       <c r="F40" s="35"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="35" t="s">
         <v>61</v>
       </c>
@@ -1341,7 +1347,7 @@
       <c r="E41" s="35"/>
       <c r="F41" s="35"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="35" t="s">
         <v>62</v>
       </c>
@@ -1351,15 +1357,15 @@
       <c r="E42" s="35"/>
       <c r="F42" s="35"/>
     </row>
-    <row r="43" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
     </row>
-    <row r="44" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="35" t="s">
         <v>49</v>
       </c>
@@ -1369,7 +1375,7 @@
       <c r="E45" s="35"/>
       <c r="F45" s="35"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="35" t="s">
         <v>50</v>
       </c>
@@ -1379,7 +1385,7 @@
       <c r="E46" s="35"/>
       <c r="F46" s="35"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="35" t="s">
         <v>52</v>
       </c>
@@ -1389,7 +1395,7 @@
       <c r="E47" s="35"/>
       <c r="F47" s="35"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="35" t="s">
         <v>53</v>
       </c>
@@ -1399,22 +1405,22 @@
       <c r="E48" s="35"/>
       <c r="F48" s="35"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49" s="30" t="s">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="B49" s="30"/>
-      <c r="C49" s="30"/>
-      <c r="D49" s="30"/>
-      <c r="E49" s="30"/>
-      <c r="F49" s="30"/>
-    </row>
-    <row r="51" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B49" s="29"/>
+      <c r="C49" s="29"/>
+      <c r="D49" s="29"/>
+      <c r="E49" s="29"/>
+      <c r="F49" s="29"/>
+    </row>
+    <row r="51" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="35" t="s">
         <v>55</v>
       </c>
@@ -1424,7 +1430,7 @@
       <c r="E52" s="35"/>
       <c r="F52" s="35"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="35" t="s">
         <v>56</v>
       </c>
@@ -1434,7 +1440,7 @@
       <c r="E53" s="35"/>
       <c r="F53" s="35"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="35" t="s">
         <v>57</v>
       </c>
@@ -1444,17 +1450,17 @@
       <c r="E54" s="35"/>
       <c r="F54" s="35"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A55" s="34" t="s">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="B55" s="34"/>
-      <c r="C55" s="34"/>
-      <c r="D55" s="34"/>
-      <c r="E55" s="34"/>
-      <c r="F55" s="34"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B55" s="36"/>
+      <c r="C55" s="36"/>
+      <c r="D55" s="36"/>
+      <c r="E55" s="36"/>
+      <c r="F55" s="36"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="11" t="s">
         <v>76</v>
       </c>
@@ -1464,12 +1470,12 @@
       <c r="E56" s="11"/>
       <c r="F56" s="11"/>
     </row>
-    <row r="58" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="35" t="s">
         <v>64</v>
       </c>
@@ -1479,7 +1485,7 @@
       <c r="E59" s="35"/>
       <c r="F59" s="35"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="35" t="s">
         <v>65</v>
       </c>
@@ -1489,7 +1495,7 @@
       <c r="E60" s="35"/>
       <c r="F60" s="35"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="35" t="s">
         <v>85</v>
       </c>
@@ -1499,7 +1505,7 @@
       <c r="E61" s="35"/>
       <c r="F61" s="35"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="11" t="s">
         <v>84</v>
       </c>
@@ -1509,9 +1515,9 @@
       <c r="E62" s="11"/>
       <c r="F62" s="11"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="35" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B63" s="35"/>
       <c r="C63" s="35"/>
@@ -1519,37 +1525,37 @@
       <c r="E63" s="35"/>
       <c r="F63" s="35"/>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A64" s="30" t="s">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="B64" s="30"/>
-      <c r="C64" s="30"/>
-      <c r="D64" s="30"/>
-      <c r="E64" s="30"/>
-      <c r="F64" s="30"/>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A65" s="30" t="s">
+      <c r="B64" s="29"/>
+      <c r="C64" s="29"/>
+      <c r="D64" s="29"/>
+      <c r="E64" s="29"/>
+      <c r="F64" s="29"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="B65" s="30"/>
-      <c r="C65" s="30"/>
-      <c r="D65" s="30"/>
-      <c r="E65" s="30"/>
-      <c r="F65" s="30"/>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A66" s="30" t="s">
+      <c r="B65" s="29"/>
+      <c r="C65" s="29"/>
+      <c r="D65" s="29"/>
+      <c r="E65" s="29"/>
+      <c r="F65" s="29"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="B66" s="30"/>
-      <c r="C66" s="30"/>
-      <c r="D66" s="30"/>
-      <c r="E66" s="30"/>
-      <c r="F66" s="30"/>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B66" s="29"/>
+      <c r="C66" s="29"/>
+      <c r="D66" s="29"/>
+      <c r="E66" s="29"/>
+      <c r="F66" s="29"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="35" t="s">
         <v>67</v>
       </c>
@@ -1559,77 +1565,77 @@
       <c r="E67" s="35"/>
       <c r="F67" s="35"/>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A68" s="20" t="s">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="B68" s="20"/>
-      <c r="C68" s="20"/>
-      <c r="D68" s="20"/>
-      <c r="E68" s="20"/>
-      <c r="F68" s="20"/>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A69" s="21" t="s">
-        <v>117</v>
-      </c>
-      <c r="B69" s="21"/>
-      <c r="C69" s="21"/>
-      <c r="D69" s="21"/>
-      <c r="E69" s="21"/>
-      <c r="F69" s="21"/>
-    </row>
-    <row r="71" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B68" s="19"/>
+      <c r="C68" s="19"/>
+      <c r="D68" s="19"/>
+      <c r="E68" s="19"/>
+      <c r="F68" s="19"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="B69" s="20"/>
+      <c r="C69" s="20"/>
+      <c r="D69" s="20"/>
+      <c r="E69" s="20"/>
+      <c r="F69" s="20"/>
+    </row>
+    <row r="71" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A72" s="34" t="s">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="B72" s="34"/>
-      <c r="C72" s="34"/>
-      <c r="D72" s="34"/>
-      <c r="E72" s="34"/>
-      <c r="F72" s="34"/>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A73" s="34" t="s">
+      <c r="B72" s="36"/>
+      <c r="C72" s="36"/>
+      <c r="D72" s="36"/>
+      <c r="E72" s="36"/>
+      <c r="F72" s="36"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="B73" s="34"/>
-      <c r="C73" s="34"/>
-      <c r="D73" s="34"/>
-      <c r="E73" s="34"/>
-      <c r="F73" s="34"/>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A74" s="34" t="s">
+      <c r="B73" s="36"/>
+      <c r="C73" s="36"/>
+      <c r="D73" s="36"/>
+      <c r="E73" s="36"/>
+      <c r="F73" s="36"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="B74" s="34"/>
-      <c r="C74" s="34"/>
-      <c r="D74" s="34"/>
-      <c r="E74" s="34"/>
-      <c r="F74" s="34"/>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A75" s="34" t="s">
+      <c r="B74" s="36"/>
+      <c r="C74" s="36"/>
+      <c r="D74" s="36"/>
+      <c r="E74" s="36"/>
+      <c r="F74" s="36"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="B75" s="34"/>
-      <c r="C75" s="34"/>
-      <c r="D75" s="34"/>
-      <c r="E75" s="34"/>
-      <c r="F75" s="34"/>
-    </row>
-    <row r="77" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B75" s="36"/>
+      <c r="C75" s="36"/>
+      <c r="D75" s="36"/>
+      <c r="E75" s="36"/>
+      <c r="F75" s="36"/>
+    </row>
+    <row r="77" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="14" t="s">
         <v>78</v>
       </c>
@@ -1639,7 +1645,7 @@
       <c r="E78" s="14"/>
       <c r="F78" s="14"/>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="10" t="s">
         <v>97</v>
       </c>
@@ -1649,168 +1655,148 @@
       <c r="E79" s="10"/>
       <c r="F79" s="10"/>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A80" s="22" t="s">
-        <v>116</v>
-      </c>
-      <c r="B80" s="22"/>
-      <c r="C80" s="22"/>
-      <c r="D80" s="22"/>
-      <c r="E80" s="22"/>
-      <c r="F80" s="22"/>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A81" s="24" t="s">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="B81" s="24"/>
-      <c r="C81" s="24"/>
-      <c r="D81" s="24"/>
-      <c r="E81" s="24"/>
-      <c r="F81" s="24"/>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A82" s="33" t="s">
+      <c r="B80" s="21"/>
+      <c r="C80" s="21"/>
+      <c r="D80" s="21"/>
+      <c r="E80" s="21"/>
+      <c r="F80" s="21"/>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="B81" s="23"/>
+      <c r="C81" s="23"/>
+      <c r="D81" s="23"/>
+      <c r="E81" s="23"/>
+      <c r="F81" s="23"/>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82" s="32" t="s">
+        <v>122</v>
+      </c>
+      <c r="B82" s="32"/>
+      <c r="C82" s="32"/>
+      <c r="D82" s="32"/>
+      <c r="E82" s="32"/>
+      <c r="F82" s="32"/>
+      <c r="G82" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83" s="28" t="s">
         <v>123</v>
       </c>
-      <c r="B82" s="33"/>
-      <c r="C82" s="33"/>
-      <c r="D82" s="33"/>
-      <c r="E82" s="33"/>
-      <c r="F82" s="33"/>
-      <c r="G82" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A83" s="29" t="s">
+      <c r="B83" s="28"/>
+      <c r="C83" s="28"/>
+      <c r="D83" s="28"/>
+      <c r="E83" s="28"/>
+      <c r="F83" s="28"/>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" s="31" t="s">
         <v>124</v>
       </c>
-      <c r="B83" s="29"/>
-      <c r="C83" s="29"/>
-      <c r="D83" s="29"/>
-      <c r="E83" s="29"/>
-      <c r="F83" s="29"/>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A84" s="32" t="s">
+      <c r="B84" s="31"/>
+      <c r="C84" s="31"/>
+      <c r="D84" s="31"/>
+      <c r="E84" s="31"/>
+      <c r="F84" s="31"/>
+      <c r="G84" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85" s="30" t="s">
         <v>125</v>
       </c>
-      <c r="B84" s="32"/>
-      <c r="C84" s="32"/>
-      <c r="D84" s="32"/>
-      <c r="E84" s="32"/>
-      <c r="F84" s="32"/>
-      <c r="G84" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A85" s="31" t="s">
+      <c r="B85" s="30"/>
+      <c r="C85" s="30"/>
+      <c r="D85" s="30"/>
+      <c r="E85" s="30"/>
+      <c r="F85" s="30"/>
+    </row>
+    <row r="87" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="B88" s="18"/>
+      <c r="C88" s="18"/>
+      <c r="D88" s="18"/>
+      <c r="E88" s="18"/>
+      <c r="F88" s="18"/>
+      <c r="G88" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="B89" s="24"/>
+      <c r="C89" s="24"/>
+      <c r="D89" s="24"/>
+      <c r="E89" s="24"/>
+      <c r="F89" s="24"/>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="B85" s="31"/>
-      <c r="C85" s="31"/>
-      <c r="D85" s="31"/>
-      <c r="E85" s="31"/>
-      <c r="F85" s="31"/>
-    </row>
-    <row r="87" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A87" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A88" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="B88" s="19"/>
-      <c r="C88" s="19"/>
-      <c r="D88" s="19"/>
-      <c r="E88" s="19"/>
-      <c r="F88" s="19"/>
-      <c r="G88" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A89" s="25" t="s">
+      <c r="B90" s="37"/>
+      <c r="C90" s="37"/>
+      <c r="D90" s="37"/>
+      <c r="E90" s="37"/>
+      <c r="F90" s="37"/>
+      <c r="G90" t="s">
         <v>112</v>
       </c>
-      <c r="B89" s="25"/>
-      <c r="C89" s="25"/>
-      <c r="D89" s="25"/>
-      <c r="E89" s="25"/>
-      <c r="F89" s="25"/>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A90" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="B90" s="15"/>
-      <c r="C90" s="15"/>
-      <c r="D90" s="15"/>
-      <c r="E90" s="15"/>
-      <c r="F90" s="15"/>
-      <c r="G90" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A91" s="26" t="s">
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="B91" s="25"/>
+      <c r="C91" s="25"/>
+      <c r="D91" s="25"/>
+      <c r="E91" s="25"/>
+      <c r="F91" s="25"/>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A92" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="B91" s="26"/>
-      <c r="C91" s="26"/>
-      <c r="D91" s="26"/>
-      <c r="E91" s="26"/>
-      <c r="F91" s="26"/>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A92" s="27" t="s">
+      <c r="B92" s="26"/>
+      <c r="C92" s="26"/>
+      <c r="D92" s="26"/>
+      <c r="E92" s="26"/>
+      <c r="F92" s="26"/>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="B92" s="27"/>
-      <c r="C92" s="27"/>
-      <c r="D92" s="27"/>
-      <c r="E92" s="27"/>
-      <c r="F92" s="27"/>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A93" s="28" t="s">
-        <v>122</v>
-      </c>
-      <c r="B93" s="28"/>
-      <c r="C93" s="28"/>
-      <c r="D93" s="28"/>
-      <c r="E93" s="28"/>
-      <c r="F93" s="28"/>
+      <c r="B93" s="27"/>
+      <c r="C93" s="27"/>
+      <c r="D93" s="27"/>
+      <c r="E93" s="27"/>
+      <c r="F93" s="27"/>
       <c r="G93" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A16:F16"/>
-    <mergeCell ref="A29:F29"/>
-    <mergeCell ref="A31:F31"/>
-    <mergeCell ref="A32:F32"/>
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="A34:F34"/>
-    <mergeCell ref="A35:F35"/>
-    <mergeCell ref="A36:F36"/>
-    <mergeCell ref="A40:F40"/>
-    <mergeCell ref="A41:F41"/>
-    <mergeCell ref="A42:F42"/>
-    <mergeCell ref="A45:F45"/>
-    <mergeCell ref="A46:F46"/>
-    <mergeCell ref="A47:F47"/>
-    <mergeCell ref="A48:F48"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="A53:F53"/>
-    <mergeCell ref="A54:F54"/>
-    <mergeCell ref="A55:F55"/>
     <mergeCell ref="A72:F72"/>
     <mergeCell ref="A73:F73"/>
     <mergeCell ref="A74:F74"/>
@@ -1820,6 +1806,26 @@
     <mergeCell ref="A61:F61"/>
     <mergeCell ref="A63:F63"/>
     <mergeCell ref="A67:F67"/>
+    <mergeCell ref="A48:F48"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="A53:F53"/>
+    <mergeCell ref="A54:F54"/>
+    <mergeCell ref="A55:F55"/>
+    <mergeCell ref="A41:F41"/>
+    <mergeCell ref="A42:F42"/>
+    <mergeCell ref="A45:F45"/>
+    <mergeCell ref="A46:F46"/>
+    <mergeCell ref="A47:F47"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A34:F34"/>
+    <mergeCell ref="A35:F35"/>
+    <mergeCell ref="A36:F36"/>
+    <mergeCell ref="A40:F40"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A29:F29"/>
+    <mergeCell ref="A31:F31"/>
+    <mergeCell ref="A32:F32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1833,29 +1839,29 @@
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.109375" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>81</v>
       </c>
@@ -1863,7 +1869,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>87</v>
       </c>
@@ -1871,7 +1877,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>88</v>
       </c>
@@ -1879,7 +1885,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>89</v>
       </c>
@@ -1887,7 +1893,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>80</v>
       </c>
@@ -1895,7 +1901,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>90</v>
       </c>
@@ -1903,7 +1909,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B9" s="13">
         <f>SUM(B3:B8)</f>
         <v>1</v>
@@ -1915,7 +1921,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="J10" t="s">
         <v>88</v>
       </c>
@@ -1932,7 +1938,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>13</v>
       </c>
@@ -1952,7 +1958,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>81</v>
       </c>
@@ -1963,7 +1969,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>87</v>
       </c>
@@ -1974,7 +1980,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>88</v>
       </c>
@@ -1982,7 +1988,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>89</v>
       </c>
@@ -1990,7 +1996,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>80</v>
       </c>
@@ -1998,7 +2004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>90</v>
       </c>
@@ -2006,18 +2012,18 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B18" s="13">
         <f>SUM(B12:B17)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>81</v>
       </c>
@@ -2025,7 +2031,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>87</v>
       </c>
@@ -2033,7 +2039,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>88</v>
       </c>
@@ -2041,7 +2047,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>89</v>
       </c>
@@ -2049,7 +2055,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>80</v>
       </c>
@@ -2057,7 +2063,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>90</v>
       </c>
@@ -2065,18 +2071,18 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B27" s="13">
         <f>SUM(B21:B26)</f>
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>81</v>
       </c>
@@ -2084,7 +2090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>87</v>
       </c>
@@ -2092,7 +2098,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>88</v>
       </c>
@@ -2100,7 +2106,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>89</v>
       </c>
@@ -2108,7 +2114,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>80</v>
       </c>
@@ -2116,7 +2122,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>90</v>
       </c>
@@ -2124,18 +2130,18 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B36" s="13">
         <f>SUM(B30:B35)</f>
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>81</v>
       </c>
@@ -2143,7 +2149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>87</v>
       </c>
@@ -2151,7 +2157,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>88</v>
       </c>
@@ -2159,7 +2165,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>89</v>
       </c>
@@ -2167,7 +2173,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>80</v>
       </c>
@@ -2175,7 +2181,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>90</v>
       </c>
@@ -2183,7 +2189,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B45" s="13">
         <f>SUM(B39:B44)</f>
         <v>1</v>

</xml_diff>

<commit_message>
working on sound effects
</commit_message>
<xml_diff>
--- a/Production Documents/To-Do.xlsx
+++ b/Production Documents/To-Do.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmgam\Desktop\Shiva\Production Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ABF5E35-0969-4078-897F-92E4BE0F0D5B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92EF8252-5B65-41B8-8224-9DC07BE33C11}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{669DCC34-C837-4342-A908-0F87EB315612}"/>
   </bookViews>
@@ -412,7 +412,7 @@
     <t>More aliens</t>
   </si>
   <si>
-    <t>Sound</t>
+    <t>Sound is played when something is attacked</t>
   </si>
 </sst>
 </file>
@@ -522,7 +522,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
@@ -556,14 +556,15 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -888,8 +889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4D254F2-4E19-40CF-BD85-766CDBA8C5EF}">
   <dimension ref="A2:G93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="G78" sqref="G78"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="J74" sqref="J74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -908,14 +909,14 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="18" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -1104,14 +1105,14 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="33"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
+      <c r="B16" s="36"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
@@ -1231,14 +1232,14 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="34" t="s">
+      <c r="A29" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="34"/>
-      <c r="C29" s="34"/>
-      <c r="D29" s="34"/>
-      <c r="E29" s="34"/>
-      <c r="F29" s="34"/>
+      <c r="B29" s="37"/>
+      <c r="C29" s="37"/>
+      <c r="D29" s="37"/>
+      <c r="E29" s="37"/>
+      <c r="F29" s="37"/>
     </row>
     <row r="30" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
@@ -1444,14 +1445,14 @@
       <c r="F54" s="35"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="36" t="s">
+      <c r="A55" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="B55" s="36"/>
-      <c r="C55" s="36"/>
-      <c r="D55" s="36"/>
-      <c r="E55" s="36"/>
-      <c r="F55" s="36"/>
+      <c r="B55" s="34"/>
+      <c r="C55" s="34"/>
+      <c r="D55" s="34"/>
+      <c r="E55" s="34"/>
+      <c r="F55" s="34"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="11" t="s">
@@ -1584,44 +1585,44 @@
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="36" t="s">
+      <c r="A72" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="B72" s="36"/>
-      <c r="C72" s="36"/>
-      <c r="D72" s="36"/>
-      <c r="E72" s="36"/>
-      <c r="F72" s="36"/>
+      <c r="B72" s="34"/>
+      <c r="C72" s="34"/>
+      <c r="D72" s="34"/>
+      <c r="E72" s="34"/>
+      <c r="F72" s="34"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="36" t="s">
+      <c r="A73" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="B73" s="36"/>
-      <c r="C73" s="36"/>
-      <c r="D73" s="36"/>
-      <c r="E73" s="36"/>
-      <c r="F73" s="36"/>
+      <c r="B73" s="34"/>
+      <c r="C73" s="34"/>
+      <c r="D73" s="34"/>
+      <c r="E73" s="34"/>
+      <c r="F73" s="34"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="36" t="s">
+      <c r="A74" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="B74" s="36"/>
-      <c r="C74" s="36"/>
-      <c r="D74" s="36"/>
-      <c r="E74" s="36"/>
-      <c r="F74" s="36"/>
+      <c r="B74" s="34"/>
+      <c r="C74" s="34"/>
+      <c r="D74" s="34"/>
+      <c r="E74" s="34"/>
+      <c r="F74" s="34"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="36" t="s">
+      <c r="A75" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="B75" s="36"/>
-      <c r="C75" s="36"/>
-      <c r="D75" s="36"/>
-      <c r="E75" s="36"/>
-      <c r="F75" s="36"/>
+      <c r="B75" s="34"/>
+      <c r="C75" s="34"/>
+      <c r="D75" s="34"/>
+      <c r="E75" s="34"/>
+      <c r="F75" s="34"/>
     </row>
     <row r="77" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
@@ -1669,14 +1670,14 @@
       <c r="F81" s="24"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82" s="29" t="s">
+      <c r="A82" s="33" t="s">
         <v>123</v>
       </c>
-      <c r="B82" s="29"/>
-      <c r="C82" s="29"/>
-      <c r="D82" s="29"/>
-      <c r="E82" s="29"/>
-      <c r="F82" s="29"/>
+      <c r="B82" s="33"/>
+      <c r="C82" s="33"/>
+      <c r="D82" s="33"/>
+      <c r="E82" s="33"/>
+      <c r="F82" s="33"/>
       <c r="G82" t="s">
         <v>113</v>
       </c>
@@ -1790,6 +1791,26 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A29:F29"/>
+    <mergeCell ref="A31:F31"/>
+    <mergeCell ref="A32:F32"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A34:F34"/>
+    <mergeCell ref="A35:F35"/>
+    <mergeCell ref="A36:F36"/>
+    <mergeCell ref="A40:F40"/>
+    <mergeCell ref="A41:F41"/>
+    <mergeCell ref="A42:F42"/>
+    <mergeCell ref="A45:F45"/>
+    <mergeCell ref="A46:F46"/>
+    <mergeCell ref="A47:F47"/>
+    <mergeCell ref="A48:F48"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="A53:F53"/>
+    <mergeCell ref="A54:F54"/>
+    <mergeCell ref="A55:F55"/>
     <mergeCell ref="A72:F72"/>
     <mergeCell ref="A73:F73"/>
     <mergeCell ref="A74:F74"/>
@@ -1799,26 +1820,6 @@
     <mergeCell ref="A61:F61"/>
     <mergeCell ref="A63:F63"/>
     <mergeCell ref="A67:F67"/>
-    <mergeCell ref="A48:F48"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="A53:F53"/>
-    <mergeCell ref="A54:F54"/>
-    <mergeCell ref="A55:F55"/>
-    <mergeCell ref="A41:F41"/>
-    <mergeCell ref="A42:F42"/>
-    <mergeCell ref="A45:F45"/>
-    <mergeCell ref="A46:F46"/>
-    <mergeCell ref="A47:F47"/>
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="A34:F34"/>
-    <mergeCell ref="A35:F35"/>
-    <mergeCell ref="A36:F36"/>
-    <mergeCell ref="A40:F40"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A16:F16"/>
-    <mergeCell ref="A29:F29"/>
-    <mergeCell ref="A31:F31"/>
-    <mergeCell ref="A32:F32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>